<commit_message>
Start GDD & Pitch & Sub-Rol & Presentatie & Uren Registratie 04-02-2016 &  Logo
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="49">
   <si>
     <t>Fahrettin</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Mack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kevin </t>
   </si>
   <si>
     <t>Week 5:</t>
@@ -815,22 +812,22 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1120,7 +1117,7 @@
   <dimension ref="A1:L175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,10 +1152,10 @@
         <v>15</v>
       </c>
       <c r="H1" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="72" t="s">
         <v>40</v>
-      </c>
-      <c r="I1" s="72" t="s">
-        <v>41</v>
       </c>
       <c r="J1" s="81" t="s">
         <v>9</v>
@@ -1169,7 +1166,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1190,8 +1187,9 @@
         <f>J2/I2</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="L2" s="82" t="s">
-        <v>0</v>
+      <c r="L2" s="82" t="str">
+        <f>C1</f>
+        <v>Fahrettin</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1224,8 +1222,9 @@
         <f>J3/I2</f>
         <v>1</v>
       </c>
-      <c r="L3" s="56" t="s">
-        <v>12</v>
+      <c r="L3" s="56" t="str">
+        <f>D1</f>
+        <v>Lara</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1258,8 +1257,9 @@
         <f>J4/I2</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="L4" s="77" t="s">
-        <v>13</v>
+      <c r="L4" s="77" t="str">
+        <f>E1</f>
+        <v>Ruben</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1292,8 +1292,9 @@
         <f>J5/I2</f>
         <v>1</v>
       </c>
-      <c r="L5" s="85" t="s">
-        <v>16</v>
+      <c r="L5" s="85" t="str">
+        <f>F1</f>
+        <v>Kevin</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1301,7 +1302,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="123">
+      <c r="C6" s="120">
         <v>0</v>
       </c>
       <c r="D6" s="102">
@@ -1317,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="78">
@@ -1328,8 +1329,9 @@
         <f>J6/I2</f>
         <v>0.94444444444444442</v>
       </c>
-      <c r="L6" s="78" t="s">
-        <v>15</v>
+      <c r="L6" s="78" t="str">
+        <f>G1</f>
+        <v>Mack</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1337,23 +1339,23 @@
         <v>5</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="124">
+      <c r="C7" s="121">
         <v>8</v>
       </c>
-      <c r="D7" s="119">
+      <c r="D7" s="124">
         <v>8</v>
       </c>
-      <c r="E7" s="122">
-        <v>0</v>
-      </c>
-      <c r="F7" s="120">
+      <c r="E7" s="119">
+        <v>0</v>
+      </c>
+      <c r="F7" s="123">
         <v>8</v>
       </c>
-      <c r="G7" s="121">
+      <c r="G7" s="122">
         <v>7</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I7" s="10"/>
       <c r="L7" s="35"/>
@@ -1405,7 +1407,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="26"/>
@@ -1416,7 +1418,7 @@
       <c r="H10" s="17"/>
       <c r="I10" s="10"/>
       <c r="J10" s="96" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1432,7 +1434,7 @@
       <c r="H11" s="18"/>
       <c r="I11" s="10"/>
       <c r="J11" s="97" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1448,7 +1450,7 @@
       <c r="H12" s="18"/>
       <c r="I12" s="10"/>
       <c r="J12" s="98" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1464,7 +1466,7 @@
       <c r="H13" s="18"/>
       <c r="I13" s="10"/>
       <c r="J13" s="99" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1480,7 +1482,7 @@
       <c r="H14" s="18"/>
       <c r="I14" s="10"/>
       <c r="J14" s="100" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1536,7 +1538,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="26"/>
@@ -1651,7 +1653,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="26"/>
@@ -1766,7 +1768,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="25"/>
@@ -1811,7 +1813,7 @@
       <c r="C37" s="52"/>
       <c r="D37" s="54"/>
       <c r="E37" s="64" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F37" s="53"/>
       <c r="G37" s="94"/>
@@ -1853,7 +1855,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="26"/>
@@ -1968,7 +1970,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="26"/>
@@ -2083,7 +2085,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="26"/>
@@ -2200,7 +2202,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B65" s="66"/>
       <c r="C65" s="26"/>
@@ -2315,7 +2317,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B73" s="8"/>
       <c r="C73" s="26"/>
@@ -2430,7 +2432,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="26"/>
@@ -2545,7 +2547,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B89" s="8"/>
       <c r="C89" s="26"/>
@@ -2660,7 +2662,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B97" s="8"/>
       <c r="C97" s="26"/>
@@ -2775,7 +2777,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="61" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B105" s="51"/>
       <c r="C105" s="25"/>
@@ -2820,7 +2822,7 @@
       <c r="C108" s="52"/>
       <c r="D108" s="54"/>
       <c r="E108" s="118" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F108" s="54"/>
       <c r="G108" s="114"/>
@@ -2862,7 +2864,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B112" s="8"/>
       <c r="C112" s="26"/>
@@ -2977,7 +2979,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B120" s="8"/>
       <c r="C120" s="26"/>
@@ -3092,7 +3094,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B128" s="8"/>
       <c r="C128" s="26"/>
@@ -3207,7 +3209,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B136" s="26"/>
       <c r="C136" s="26"/>
@@ -3324,7 +3326,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B144" s="26"/>
       <c r="C144" s="26"/>
@@ -3439,7 +3441,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B152" s="8"/>
       <c r="C152" s="26"/>
@@ -3554,7 +3556,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B160" s="8"/>
       <c r="C160" s="26"/>
@@ -3669,7 +3671,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B168" s="8"/>
       <c r="C168" s="26"/>

</xml_diff>

<commit_message>
Uren Registratie 08-02-2016 & Voorbeeld AI Core Plaatje & GDD uitgewerkt (moet nog opmaak en spellingscontrole overheen)
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="49">
   <si>
     <t>Fahrettin</t>
   </si>
@@ -504,7 +504,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -524,15 +524,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -683,15 +674,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -722,15 +704,9 @@
     <xf numFmtId="10" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -771,9 +747,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -828,6 +801,105 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1117,7 +1189,7 @@
   <dimension ref="A1:L175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,39 +1200,39 @@
     <col min="8" max="8" width="59.140625" customWidth="1"/>
     <col min="9" max="9" width="27.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.140625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="142" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="74" t="s">
+      <c r="C1" s="117" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="E1" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="F1" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="76" t="s">
+      <c r="G1" s="121" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="65" t="s">
+      <c r="H1" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="81" t="s">
+      <c r="J1" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="73" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1168,26 +1240,26 @@
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="104"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="124"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="91">
+      <c r="I2" s="83">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>18</v>
-      </c>
-      <c r="J2" s="82">
+        <v>22</v>
+      </c>
+      <c r="J2" s="76">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>16</v>
-      </c>
-      <c r="K2" s="88">
+        <v>20</v>
+      </c>
+      <c r="K2" s="81">
         <f>J2/I2</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="L2" s="82" t="str">
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="L2" s="76" t="str">
         <f>C1</f>
         <v>Fahrettin</v>
       </c>
@@ -1196,33 +1268,35 @@
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="101">
+      <c r="B3" s="143">
         <v>4</v>
       </c>
-      <c r="D3" s="102">
+      <c r="C3" s="93">
         <v>4</v>
       </c>
-      <c r="E3" s="102">
+      <c r="D3" s="94">
         <v>4</v>
       </c>
-      <c r="F3" s="102">
+      <c r="E3" s="94">
         <v>4</v>
       </c>
-      <c r="G3" s="105">
+      <c r="F3" s="94">
+        <v>4</v>
+      </c>
+      <c r="G3" s="96">
         <v>4</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="56">
+      <c r="J3" s="53">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>18</v>
-      </c>
-      <c r="K3" s="83">
+        <v>22</v>
+      </c>
+      <c r="K3" s="77">
         <f>J3/I2</f>
         <v>1</v>
       </c>
-      <c r="L3" s="56" t="str">
+      <c r="L3" s="53" t="str">
         <f>D1</f>
         <v>Lara</v>
       </c>
@@ -1231,33 +1305,35 @@
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="101">
+      <c r="B4" s="143">
         <v>2</v>
       </c>
-      <c r="D4" s="102">
+      <c r="C4" s="93">
         <v>2</v>
       </c>
-      <c r="E4" s="102">
+      <c r="D4" s="94">
         <v>2</v>
       </c>
-      <c r="F4" s="102">
+      <c r="E4" s="94">
         <v>2</v>
       </c>
-      <c r="G4" s="105">
+      <c r="F4" s="94">
+        <v>2</v>
+      </c>
+      <c r="G4" s="96">
         <v>2</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="77">
+      <c r="J4" s="71">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
         <v>10</v>
       </c>
-      <c r="K4" s="84">
+      <c r="K4" s="78">
         <f>J4/I2</f>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="L4" s="77" t="str">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="L4" s="71" t="str">
         <f>E1</f>
         <v>Ruben</v>
       </c>
@@ -1266,33 +1342,35 @@
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="101">
+      <c r="B5" s="143">
         <v>2</v>
       </c>
-      <c r="D5" s="102">
+      <c r="C5" s="93">
         <v>2</v>
       </c>
-      <c r="E5" s="102">
+      <c r="D5" s="94">
         <v>2</v>
       </c>
-      <c r="F5" s="102">
+      <c r="E5" s="94">
         <v>2</v>
       </c>
-      <c r="G5" s="105">
+      <c r="F5" s="94">
+        <v>2</v>
+      </c>
+      <c r="G5" s="96">
         <v>2</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="85">
+      <c r="J5" s="79">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>18</v>
-      </c>
-      <c r="K5" s="86">
+        <v>22</v>
+      </c>
+      <c r="K5" s="80">
         <f>J5/I2</f>
         <v>1</v>
       </c>
-      <c r="L5" s="85" t="str">
+      <c r="L5" s="79" t="str">
         <f>F1</f>
         <v>Kevin</v>
       </c>
@@ -1301,35 +1379,37 @@
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="120">
-        <v>0</v>
-      </c>
-      <c r="D6" s="102">
+      <c r="B6" s="143">
         <v>2</v>
       </c>
-      <c r="E6" s="102">
+      <c r="C6" s="111">
+        <v>0</v>
+      </c>
+      <c r="D6" s="94">
         <v>2</v>
       </c>
-      <c r="F6" s="102">
+      <c r="E6" s="94">
         <v>2</v>
       </c>
-      <c r="G6" s="105">
+      <c r="F6" s="94">
+        <v>2</v>
+      </c>
+      <c r="G6" s="96">
         <v>2</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>47</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="78">
+      <c r="J6" s="72">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>17</v>
-      </c>
-      <c r="K6" s="90">
+        <v>21</v>
+      </c>
+      <c r="K6" s="82">
         <f>J6/I2</f>
-        <v>0.94444444444444442</v>
-      </c>
-      <c r="L6" s="78" t="str">
+        <v>0.95454545454545459</v>
+      </c>
+      <c r="L6" s="72" t="str">
         <f>G1</f>
         <v>Mack</v>
       </c>
@@ -1338,102 +1418,120 @@
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="121">
+      <c r="B7" s="144">
         <v>8</v>
       </c>
-      <c r="D7" s="124">
+      <c r="C7" s="112">
         <v>8</v>
       </c>
-      <c r="E7" s="119">
-        <v>0</v>
-      </c>
-      <c r="F7" s="123">
+      <c r="D7" s="115">
         <v>8</v>
       </c>
-      <c r="G7" s="122">
+      <c r="E7" s="110">
+        <v>0</v>
+      </c>
+      <c r="F7" s="114">
+        <v>8</v>
+      </c>
+      <c r="G7" s="113">
         <v>7</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="12" t="s">
         <v>48</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="L7" s="35"/>
+      <c r="L7" s="32"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="91">
+      <c r="B8" s="145">
+        <f>B3+B4+B5+B6+B7</f>
         <v>18</v>
       </c>
-      <c r="C8" s="69">
+      <c r="C8" s="125">
         <f t="shared" ref="C8:G8" si="0">SUM(C3:C7)</f>
         <v>16</v>
       </c>
-      <c r="D8" s="70">
+      <c r="D8" s="126">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E8" s="70">
+      <c r="E8" s="126">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F8" s="70">
+      <c r="F8" s="126">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="G8" s="71">
+      <c r="G8" s="127">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H8" s="103"/>
+      <c r="H8" s="95"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="72" t="s">
+      <c r="J8" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="80">
+      <c r="K8" s="74">
         <f>SUM(K2:K7)</f>
-        <v>4.3888888888888893</v>
+        <v>4.3181818181818183</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="16"/>
+      <c r="B9" s="141"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="17"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="130"/>
+      <c r="G10" s="131"/>
+      <c r="H10" s="14"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="96" t="s">
+      <c r="J10" s="88" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="18"/>
+      <c r="B11" s="146">
+        <v>4</v>
+      </c>
+      <c r="C11" s="148">
+        <v>4</v>
+      </c>
+      <c r="D11" s="94">
+        <v>4</v>
+      </c>
+      <c r="E11" s="116">
+        <v>0</v>
+      </c>
+      <c r="F11" s="94">
+        <v>4</v>
+      </c>
+      <c r="G11" s="96">
+        <v>4</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="I11" s="10"/>
-      <c r="J11" s="97" t="s">
+      <c r="J11" s="89" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1441,15 +1539,15 @@
       <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="18"/>
+      <c r="B12" s="146"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="132"/>
+      <c r="F12" s="135"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="15"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="98" t="s">
+      <c r="J12" s="90" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1457,15 +1555,15 @@
       <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="106"/>
-      <c r="H13" s="18"/>
+      <c r="B13" s="146"/>
+      <c r="C13" s="134"/>
+      <c r="D13" s="136"/>
+      <c r="E13" s="136"/>
+      <c r="F13" s="132"/>
+      <c r="G13" s="133"/>
+      <c r="H13" s="15"/>
       <c r="I13" s="10"/>
-      <c r="J13" s="99" t="s">
+      <c r="J13" s="91" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1473,15 +1571,15 @@
       <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="18"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="15"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="100" t="s">
+      <c r="J14" s="92" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1489,64 +1587,65 @@
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="15"/>
+      <c r="B15" s="147"/>
+      <c r="C15" s="137"/>
+      <c r="D15" s="138"/>
+      <c r="E15" s="138"/>
+      <c r="F15" s="139"/>
+      <c r="G15" s="140"/>
+      <c r="H15" s="12"/>
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="91">
-        <v>0</v>
-      </c>
-      <c r="C16" s="69">
+      <c r="B16" s="145">
+        <f>B11+B12+B13+B14+B15</f>
+        <v>4</v>
+      </c>
+      <c r="C16" s="125">
         <f t="shared" ref="C16:G16" si="1">SUM(C11:C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="70">
+        <v>4</v>
+      </c>
+      <c r="D16" s="126">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="70">
+        <v>4</v>
+      </c>
+      <c r="E16" s="126">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F16" s="70">
+      <c r="F16" s="126">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="71">
+        <v>4</v>
+      </c>
+      <c r="G16" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="103"/>
+        <v>4</v>
+      </c>
+      <c r="H16" s="95"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="16"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="8"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="17"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="14"/>
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1554,12 +1653,12 @@
         <v>1</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="18"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="15"/>
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1567,12 +1666,12 @@
         <v>2</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="106"/>
-      <c r="H20" s="18"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="15"/>
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1580,12 +1679,12 @@
         <v>3</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="106"/>
-      <c r="H21" s="18"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="15"/>
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1593,12 +1692,12 @@
         <v>4</v>
       </c>
       <c r="B22" s="10"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="106"/>
-      <c r="H22" s="18"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="97"/>
+      <c r="H22" s="15"/>
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1606,61 +1705,61 @@
         <v>5</v>
       </c>
       <c r="B23" s="9"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="107"/>
-      <c r="H23" s="15"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="98"/>
+      <c r="H23" s="12"/>
       <c r="I23" s="10"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="91">
-        <v>0</v>
-      </c>
-      <c r="C24" s="69">
+      <c r="B24" s="83">
+        <v>0</v>
+      </c>
+      <c r="C24" s="66">
         <f t="shared" ref="C24:G24" si="2">SUM(C19:C23)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="70">
+      <c r="D24" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E24" s="70">
+      <c r="E24" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F24" s="70">
+      <c r="F24" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G24" s="71">
+      <c r="G24" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H24" s="108"/>
+      <c r="H24" s="99"/>
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="47"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="44"/>
       <c r="H26" s="1"/>
       <c r="I26" s="10"/>
     </row>
@@ -1669,11 +1768,11 @@
         <v>1</v>
       </c>
       <c r="B27" s="10"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="106"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="97"/>
       <c r="H27" s="2"/>
       <c r="I27" s="10"/>
     </row>
@@ -1682,11 +1781,11 @@
         <v>2</v>
       </c>
       <c r="B28" s="10"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="110"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="101"/>
       <c r="H28" s="2"/>
       <c r="I28" s="10"/>
     </row>
@@ -1695,11 +1794,11 @@
         <v>3</v>
       </c>
       <c r="B29" s="10"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="106"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="97"/>
       <c r="H29" s="2"/>
       <c r="I29" s="10"/>
     </row>
@@ -1708,11 +1807,11 @@
         <v>4</v>
       </c>
       <c r="B30" s="10"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="106"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="97"/>
       <c r="H30" s="2"/>
       <c r="I30" s="10"/>
     </row>
@@ -1721,11 +1820,11 @@
         <v>5</v>
       </c>
       <c r="B31" s="9"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="109"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="100"/>
       <c r="H31" s="3"/>
       <c r="I31" s="10"/>
     </row>
@@ -1733,136 +1832,136 @@
       <c r="A32" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="91">
-        <v>0</v>
-      </c>
-      <c r="C32" s="69">
+      <c r="B32" s="83">
+        <v>0</v>
+      </c>
+      <c r="C32" s="66">
         <f t="shared" ref="C32:G32" si="3">SUM(C27:C31)</f>
         <v>0</v>
       </c>
-      <c r="D32" s="70">
+      <c r="D32" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E32" s="70">
+      <c r="E32" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F32" s="70">
+      <c r="F32" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G32" s="71">
+      <c r="G32" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H32" s="108"/>
+      <c r="H32" s="99"/>
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="61" t="s">
+      <c r="A34" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="92"/>
-      <c r="H34" s="20"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="17"/>
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="62" t="s">
+      <c r="A35" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="22"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="19"/>
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="62" t="s">
+      <c r="A36" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="93"/>
-      <c r="H36" s="22"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="85"/>
+      <c r="H36" s="19"/>
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="62" t="s">
+      <c r="A37" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="64" t="s">
+      <c r="B37" s="18"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="53"/>
-      <c r="G37" s="94"/>
-      <c r="H37" s="22"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="86"/>
+      <c r="H37" s="19"/>
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="62" t="s">
+      <c r="A38" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="93"/>
-      <c r="H38" s="22"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="85"/>
+      <c r="H38" s="19"/>
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="63" t="s">
+      <c r="A39" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="59"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="95"/>
-      <c r="H39" s="24"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="87"/>
+      <c r="H39" s="21"/>
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="8"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="47"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="44"/>
       <c r="H41" s="1"/>
       <c r="I41" s="10"/>
     </row>
@@ -1871,11 +1970,11 @@
         <v>1</v>
       </c>
       <c r="B42" s="10"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="106"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="97"/>
       <c r="H42" s="2"/>
       <c r="I42" s="10"/>
     </row>
@@ -1884,11 +1983,11 @@
         <v>2</v>
       </c>
       <c r="B43" s="10"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="106"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="97"/>
       <c r="H43" s="2"/>
       <c r="I43" s="10"/>
     </row>
@@ -1897,11 +1996,11 @@
         <v>3</v>
       </c>
       <c r="B44" s="10"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="106"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="97"/>
       <c r="H44" s="2"/>
       <c r="I44" s="10"/>
     </row>
@@ -1910,11 +2009,11 @@
         <v>4</v>
       </c>
       <c r="B45" s="10"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="106"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="97"/>
       <c r="H45" s="2"/>
       <c r="I45" s="10"/>
     </row>
@@ -1923,11 +2022,11 @@
         <v>5</v>
       </c>
       <c r="B46" s="9"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="109"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="100"/>
       <c r="H46" s="3"/>
       <c r="I46" s="10"/>
     </row>
@@ -1935,49 +2034,49 @@
       <c r="A47" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="91">
-        <v>0</v>
-      </c>
-      <c r="C47" s="69">
+      <c r="B47" s="83">
+        <v>0</v>
+      </c>
+      <c r="C47" s="66">
         <f t="shared" ref="C47:G47" si="4">SUM(C42:C46)</f>
         <v>0</v>
       </c>
-      <c r="D47" s="70">
+      <c r="D47" s="67">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E47" s="70">
+      <c r="E47" s="67">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F47" s="70">
+      <c r="F47" s="67">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G47" s="71">
+      <c r="G47" s="68">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H47" s="108"/>
+      <c r="H47" s="99"/>
       <c r="I47" s="10"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B49" s="8"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="47"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="44"/>
       <c r="H49" s="1"/>
       <c r="I49" s="10"/>
     </row>
@@ -1986,11 +2085,11 @@
         <v>1</v>
       </c>
       <c r="B50" s="10"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="106"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="97"/>
       <c r="H50" s="2"/>
       <c r="I50" s="10"/>
     </row>
@@ -1999,11 +2098,11 @@
         <v>2</v>
       </c>
       <c r="B51" s="10"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="106"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="97"/>
       <c r="H51" s="2"/>
       <c r="I51" s="10"/>
     </row>
@@ -2012,11 +2111,11 @@
         <v>3</v>
       </c>
       <c r="B52" s="10"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="106"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="97"/>
       <c r="H52" s="2"/>
       <c r="I52" s="10"/>
     </row>
@@ -2025,11 +2124,11 @@
         <v>4</v>
       </c>
       <c r="B53" s="10"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="106"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="97"/>
       <c r="H53" s="2"/>
       <c r="I53" s="10"/>
     </row>
@@ -2038,11 +2137,11 @@
         <v>5</v>
       </c>
       <c r="B54" s="9"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="109"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="100"/>
       <c r="H54" s="3"/>
       <c r="I54" s="10"/>
     </row>
@@ -2050,49 +2149,49 @@
       <c r="A55" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B55" s="91">
-        <v>0</v>
-      </c>
-      <c r="C55" s="69">
+      <c r="B55" s="83">
+        <v>0</v>
+      </c>
+      <c r="C55" s="66">
         <f t="shared" ref="C55:G55" si="5">SUM(C50:C54)</f>
         <v>0</v>
       </c>
-      <c r="D55" s="70">
+      <c r="D55" s="67">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E55" s="70">
+      <c r="E55" s="67">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F55" s="70">
+      <c r="F55" s="67">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G55" s="71">
+      <c r="G55" s="68">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H55" s="108"/>
+      <c r="H55" s="99"/>
       <c r="I55" s="10"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="35"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="35"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B57" s="8"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="47"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="44"/>
       <c r="H57" s="1"/>
       <c r="I57" s="10"/>
     </row>
@@ -2101,11 +2200,11 @@
         <v>1</v>
       </c>
       <c r="B58" s="10"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="44"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="106"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="97"/>
       <c r="H58" s="2"/>
       <c r="I58" s="10"/>
     </row>
@@ -2114,11 +2213,11 @@
         <v>2</v>
       </c>
       <c r="B59" s="10"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="106"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="97"/>
       <c r="H59" s="2"/>
       <c r="I59" s="10"/>
     </row>
@@ -2127,11 +2226,11 @@
         <v>3</v>
       </c>
       <c r="B60" s="10"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="37"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="106"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="97"/>
       <c r="H60" s="2"/>
       <c r="I60" s="10"/>
     </row>
@@ -2140,11 +2239,11 @@
         <v>4</v>
       </c>
       <c r="B61" s="10"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="38"/>
-      <c r="G61" s="106"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="97"/>
       <c r="H61" s="2"/>
       <c r="I61" s="10"/>
     </row>
@@ -2153,11 +2252,11 @@
         <v>5</v>
       </c>
       <c r="B62" s="9"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="40"/>
-      <c r="F62" s="41"/>
-      <c r="G62" s="109"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="100"/>
       <c r="H62" s="3"/>
       <c r="I62" s="10"/>
     </row>
@@ -2165,166 +2264,166 @@
       <c r="A63" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="91">
-        <v>0</v>
-      </c>
-      <c r="C63" s="69">
+      <c r="B63" s="83">
+        <v>0</v>
+      </c>
+      <c r="C63" s="66">
         <f t="shared" ref="C63:G63" si="6">SUM(C58:C62)</f>
         <v>0</v>
       </c>
-      <c r="D63" s="70">
+      <c r="D63" s="67">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E63" s="70">
+      <c r="E63" s="67">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F63" s="70">
+      <c r="F63" s="67">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G63" s="71">
+      <c r="G63" s="68">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H63" s="108"/>
+      <c r="H63" s="99"/>
       <c r="I63" s="10"/>
     </row>
     <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="10"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="27"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="24"/>
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="66"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="47"/>
-      <c r="H65" s="28"/>
+      <c r="B65" s="63"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="44"/>
+      <c r="H65" s="25"/>
       <c r="I65" s="10"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="67"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="30"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="31"/>
+      <c r="B66" s="64"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="45"/>
+      <c r="H66" s="28"/>
       <c r="I66" s="10"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="67"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30"/>
-      <c r="G67" s="48"/>
-      <c r="H67" s="31"/>
+      <c r="B67" s="64"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="27"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="45"/>
+      <c r="H67" s="28"/>
       <c r="I67" s="10"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="67"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="30"/>
-      <c r="G68" s="48"/>
-      <c r="H68" s="31"/>
+      <c r="B68" s="64"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="27"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="45"/>
+      <c r="H68" s="28"/>
       <c r="I68" s="10"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="67"/>
-      <c r="C69" s="29"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
-      <c r="G69" s="48"/>
-      <c r="H69" s="31"/>
+      <c r="B69" s="64"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="45"/>
+      <c r="H69" s="28"/>
       <c r="I69" s="10"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B70" s="68"/>
-      <c r="C70" s="32"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="33"/>
-      <c r="G70" s="49"/>
-      <c r="H70" s="34"/>
+      <c r="B70" s="65"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="30"/>
+      <c r="G70" s="46"/>
+      <c r="H70" s="31"/>
       <c r="I70" s="10"/>
     </row>
     <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="73" t="s">
+      <c r="A71" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="91">
-        <v>0</v>
-      </c>
-      <c r="C71" s="69">
+      <c r="B71" s="83">
+        <v>0</v>
+      </c>
+      <c r="C71" s="66">
         <f t="shared" ref="C71:G71" si="7">SUM(C66:C70)</f>
         <v>0</v>
       </c>
-      <c r="D71" s="70">
+      <c r="D71" s="67">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="E71" s="70">
+      <c r="E71" s="67">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F71" s="70">
+      <c r="F71" s="67">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G71" s="71">
+      <c r="G71" s="68">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H71" s="108"/>
+      <c r="H71" s="99"/>
       <c r="I71" s="10"/>
     </row>
     <row r="72" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C72" s="35"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="35"/>
-      <c r="G72" s="35"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="32"/>
+      <c r="G72" s="32"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B73" s="8"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="47"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="44"/>
       <c r="H73" s="1"/>
       <c r="I73" s="10"/>
     </row>
@@ -2333,11 +2432,11 @@
         <v>1</v>
       </c>
       <c r="B74" s="10"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="106"/>
+      <c r="C74" s="33"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="34"/>
+      <c r="G74" s="97"/>
       <c r="H74" s="2"/>
       <c r="I74" s="10"/>
     </row>
@@ -2346,11 +2445,11 @@
         <v>2</v>
       </c>
       <c r="B75" s="10"/>
-      <c r="C75" s="43"/>
-      <c r="D75" s="44"/>
-      <c r="E75" s="37"/>
-      <c r="F75" s="37"/>
-      <c r="G75" s="106"/>
+      <c r="C75" s="40"/>
+      <c r="D75" s="41"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="34"/>
+      <c r="G75" s="97"/>
       <c r="H75" s="2"/>
       <c r="I75" s="10"/>
     </row>
@@ -2359,11 +2458,11 @@
         <v>3</v>
       </c>
       <c r="B76" s="10"/>
-      <c r="C76" s="36"/>
-      <c r="D76" s="44"/>
-      <c r="E76" s="44"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="106"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="41"/>
+      <c r="E76" s="41"/>
+      <c r="F76" s="34"/>
+      <c r="G76" s="97"/>
       <c r="H76" s="2"/>
       <c r="I76" s="10"/>
     </row>
@@ -2372,11 +2471,11 @@
         <v>4</v>
       </c>
       <c r="B77" s="10"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="38"/>
-      <c r="G77" s="106"/>
+      <c r="C77" s="33"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="97"/>
       <c r="H77" s="2"/>
       <c r="I77" s="10"/>
     </row>
@@ -2385,11 +2484,11 @@
         <v>5</v>
       </c>
       <c r="B78" s="9"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="40"/>
-      <c r="F78" s="40"/>
-      <c r="G78" s="109"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="100"/>
       <c r="H78" s="3"/>
       <c r="I78" s="10"/>
     </row>
@@ -2397,49 +2496,49 @@
       <c r="A79" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="91">
-        <v>0</v>
-      </c>
-      <c r="C79" s="69">
+      <c r="B79" s="83">
+        <v>0</v>
+      </c>
+      <c r="C79" s="66">
         <f t="shared" ref="C79:G79" si="8">SUM(C74:C78)</f>
         <v>0</v>
       </c>
-      <c r="D79" s="70">
+      <c r="D79" s="67">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="E79" s="70">
+      <c r="E79" s="67">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F79" s="70">
+      <c r="F79" s="67">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G79" s="71">
+      <c r="G79" s="68">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H79" s="108"/>
+      <c r="H79" s="99"/>
       <c r="I79" s="10"/>
     </row>
     <row r="80" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C80" s="35"/>
-      <c r="D80" s="35"/>
-      <c r="E80" s="35"/>
-      <c r="F80" s="35"/>
-      <c r="G80" s="35"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="32"/>
+      <c r="E80" s="32"/>
+      <c r="F80" s="32"/>
+      <c r="G80" s="32"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B81" s="8"/>
-      <c r="C81" s="26"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="47"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="44"/>
       <c r="H81" s="1"/>
       <c r="I81" s="10"/>
     </row>
@@ -2448,11 +2547,11 @@
         <v>1</v>
       </c>
       <c r="B82" s="10"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="37"/>
-      <c r="G82" s="110"/>
+      <c r="C82" s="40"/>
+      <c r="D82" s="35"/>
+      <c r="E82" s="34"/>
+      <c r="F82" s="34"/>
+      <c r="G82" s="101"/>
       <c r="H82" s="2"/>
       <c r="I82" s="10"/>
     </row>
@@ -2461,11 +2560,11 @@
         <v>2</v>
       </c>
       <c r="B83" s="10"/>
-      <c r="C83" s="36"/>
-      <c r="D83" s="38"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="38"/>
-      <c r="G83" s="106"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="35"/>
+      <c r="E83" s="34"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="97"/>
       <c r="H83" s="2"/>
       <c r="I83" s="10"/>
     </row>
@@ -2474,11 +2573,11 @@
         <v>3</v>
       </c>
       <c r="B84" s="10"/>
-      <c r="C84" s="45"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="44"/>
-      <c r="F84" s="37"/>
-      <c r="G84" s="106"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="35"/>
+      <c r="E84" s="41"/>
+      <c r="F84" s="34"/>
+      <c r="G84" s="97"/>
       <c r="H84" s="2"/>
       <c r="I84" s="10"/>
     </row>
@@ -2487,11 +2586,11 @@
         <v>4</v>
       </c>
       <c r="B85" s="10"/>
-      <c r="C85" s="43"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="37"/>
-      <c r="G85" s="106"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="35"/>
+      <c r="E85" s="34"/>
+      <c r="F85" s="34"/>
+      <c r="G85" s="97"/>
       <c r="H85" s="2"/>
       <c r="I85" s="10"/>
     </row>
@@ -2500,11 +2599,11 @@
         <v>5</v>
       </c>
       <c r="B86" s="9"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="42"/>
-      <c r="E86" s="40"/>
-      <c r="F86" s="40"/>
-      <c r="G86" s="107"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="37"/>
+      <c r="G86" s="98"/>
       <c r="H86" s="3"/>
       <c r="I86" s="10"/>
     </row>
@@ -2512,49 +2611,49 @@
       <c r="A87" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B87" s="91">
-        <v>0</v>
-      </c>
-      <c r="C87" s="69">
+      <c r="B87" s="83">
+        <v>0</v>
+      </c>
+      <c r="C87" s="66">
         <f t="shared" ref="C87:G87" si="9">SUM(C82:C86)</f>
         <v>0</v>
       </c>
-      <c r="D87" s="70">
+      <c r="D87" s="67">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="E87" s="70">
+      <c r="E87" s="67">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="F87" s="70">
+      <c r="F87" s="67">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G87" s="71">
+      <c r="G87" s="68">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H87" s="108"/>
+      <c r="H87" s="99"/>
       <c r="I87" s="10"/>
     </row>
     <row r="88" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C88" s="35"/>
-      <c r="D88" s="35"/>
-      <c r="E88" s="35"/>
-      <c r="F88" s="35"/>
-      <c r="G88" s="35"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="32"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="32"/>
+      <c r="G88" s="32"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B89" s="8"/>
-      <c r="C89" s="26"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="47"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="44"/>
       <c r="H89" s="1"/>
       <c r="I89" s="10"/>
     </row>
@@ -2563,11 +2662,11 @@
         <v>1</v>
       </c>
       <c r="B90" s="10"/>
-      <c r="C90" s="43"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="37"/>
-      <c r="F90" s="37"/>
-      <c r="G90" s="106"/>
+      <c r="C90" s="40"/>
+      <c r="D90" s="35"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="34"/>
+      <c r="G90" s="97"/>
       <c r="H90" s="2"/>
       <c r="I90" s="10"/>
     </row>
@@ -2576,11 +2675,11 @@
         <v>2</v>
       </c>
       <c r="B91" s="10"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="38"/>
-      <c r="E91" s="37"/>
-      <c r="F91" s="37"/>
-      <c r="G91" s="106"/>
+      <c r="C91" s="33"/>
+      <c r="D91" s="35"/>
+      <c r="E91" s="34"/>
+      <c r="F91" s="34"/>
+      <c r="G91" s="97"/>
       <c r="H91" s="2"/>
       <c r="I91" s="10"/>
     </row>
@@ -2589,11 +2688,11 @@
         <v>3</v>
       </c>
       <c r="B92" s="10"/>
-      <c r="C92" s="36"/>
-      <c r="D92" s="44"/>
-      <c r="E92" s="37"/>
-      <c r="F92" s="38"/>
-      <c r="G92" s="106"/>
+      <c r="C92" s="33"/>
+      <c r="D92" s="41"/>
+      <c r="E92" s="34"/>
+      <c r="F92" s="35"/>
+      <c r="G92" s="97"/>
       <c r="H92" s="2"/>
       <c r="I92" s="10"/>
     </row>
@@ -2602,11 +2701,11 @@
         <v>4</v>
       </c>
       <c r="B93" s="10"/>
-      <c r="C93" s="36"/>
-      <c r="D93" s="37"/>
-      <c r="E93" s="37"/>
-      <c r="F93" s="38"/>
-      <c r="G93" s="112"/>
+      <c r="C93" s="33"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="34"/>
+      <c r="F93" s="35"/>
+      <c r="G93" s="103"/>
       <c r="H93" s="2"/>
       <c r="I93" s="10"/>
     </row>
@@ -2615,11 +2714,11 @@
         <v>5</v>
       </c>
       <c r="B94" s="9"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="42"/>
-      <c r="E94" s="41"/>
-      <c r="F94" s="40"/>
-      <c r="G94" s="109"/>
+      <c r="C94" s="36"/>
+      <c r="D94" s="39"/>
+      <c r="E94" s="38"/>
+      <c r="F94" s="37"/>
+      <c r="G94" s="100"/>
       <c r="H94" s="3"/>
       <c r="I94" s="10"/>
     </row>
@@ -2627,49 +2726,49 @@
       <c r="A95" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B95" s="91">
-        <v>0</v>
-      </c>
-      <c r="C95" s="69">
+      <c r="B95" s="83">
+        <v>0</v>
+      </c>
+      <c r="C95" s="66">
         <f t="shared" ref="C95:G95" si="10">SUM(C90:C94)</f>
         <v>0</v>
       </c>
-      <c r="D95" s="70">
+      <c r="D95" s="67">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="E95" s="70">
+      <c r="E95" s="67">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F95" s="70">
+      <c r="F95" s="67">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G95" s="71">
+      <c r="G95" s="68">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H95" s="108"/>
+      <c r="H95" s="99"/>
       <c r="I95" s="10"/>
     </row>
     <row r="96" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C96" s="35"/>
-      <c r="D96" s="35"/>
-      <c r="E96" s="35"/>
-      <c r="F96" s="35"/>
-      <c r="G96" s="35"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="32"/>
+      <c r="E96" s="32"/>
+      <c r="F96" s="32"/>
+      <c r="G96" s="32"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B97" s="8"/>
-      <c r="C97" s="26"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="47"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="44"/>
       <c r="H97" s="1"/>
       <c r="I97" s="10"/>
     </row>
@@ -2678,11 +2777,11 @@
         <v>1</v>
       </c>
       <c r="B98" s="10"/>
-      <c r="C98" s="43"/>
-      <c r="D98" s="38"/>
-      <c r="E98" s="37"/>
-      <c r="F98" s="38"/>
-      <c r="G98" s="106"/>
+      <c r="C98" s="40"/>
+      <c r="D98" s="35"/>
+      <c r="E98" s="34"/>
+      <c r="F98" s="35"/>
+      <c r="G98" s="97"/>
       <c r="H98" s="2"/>
       <c r="I98" s="10"/>
     </row>
@@ -2691,11 +2790,11 @@
         <v>2</v>
       </c>
       <c r="B99" s="10"/>
-      <c r="C99" s="43"/>
-      <c r="D99" s="44"/>
-      <c r="E99" s="37"/>
-      <c r="F99" s="37"/>
-      <c r="G99" s="106"/>
+      <c r="C99" s="40"/>
+      <c r="D99" s="41"/>
+      <c r="E99" s="34"/>
+      <c r="F99" s="34"/>
+      <c r="G99" s="97"/>
       <c r="H99" s="2"/>
       <c r="I99" s="10"/>
     </row>
@@ -2704,11 +2803,11 @@
         <v>3</v>
       </c>
       <c r="B100" s="10"/>
-      <c r="C100" s="43"/>
-      <c r="D100" s="37"/>
-      <c r="E100" s="37"/>
-      <c r="F100" s="37"/>
-      <c r="G100" s="106"/>
+      <c r="C100" s="40"/>
+      <c r="D100" s="34"/>
+      <c r="E100" s="34"/>
+      <c r="F100" s="34"/>
+      <c r="G100" s="97"/>
       <c r="H100" s="2"/>
       <c r="I100" s="10"/>
     </row>
@@ -2717,11 +2816,11 @@
         <v>4</v>
       </c>
       <c r="B101" s="10"/>
-      <c r="C101" s="43"/>
-      <c r="D101" s="38"/>
-      <c r="E101" s="37"/>
-      <c r="F101" s="37"/>
-      <c r="G101" s="106"/>
+      <c r="C101" s="40"/>
+      <c r="D101" s="35"/>
+      <c r="E101" s="34"/>
+      <c r="F101" s="34"/>
+      <c r="G101" s="97"/>
       <c r="H101" s="2"/>
       <c r="I101" s="10"/>
     </row>
@@ -2730,11 +2829,11 @@
         <v>5</v>
       </c>
       <c r="B102" s="9"/>
-      <c r="C102" s="46"/>
-      <c r="D102" s="42"/>
-      <c r="E102" s="40"/>
-      <c r="F102" s="40"/>
-      <c r="G102" s="107"/>
+      <c r="C102" s="43"/>
+      <c r="D102" s="39"/>
+      <c r="E102" s="37"/>
+      <c r="F102" s="37"/>
+      <c r="G102" s="98"/>
       <c r="H102" s="3"/>
       <c r="I102" s="10"/>
     </row>
@@ -2742,136 +2841,136 @@
       <c r="A103" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B103" s="91">
-        <v>0</v>
-      </c>
-      <c r="C103" s="69">
+      <c r="B103" s="83">
+        <v>0</v>
+      </c>
+      <c r="C103" s="66">
         <f t="shared" ref="C103:G103" si="11">SUM(C98:C102)</f>
         <v>0</v>
       </c>
-      <c r="D103" s="70">
+      <c r="D103" s="67">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="E103" s="70">
+      <c r="E103" s="67">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F103" s="70">
+      <c r="F103" s="67">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="G103" s="71">
+      <c r="G103" s="68">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="H103" s="108"/>
+      <c r="H103" s="99"/>
       <c r="I103" s="10"/>
     </row>
     <row r="104" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C104" s="35"/>
-      <c r="D104" s="35"/>
-      <c r="E104" s="35"/>
-      <c r="F104" s="35"/>
-      <c r="G104" s="35"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="32"/>
+      <c r="E104" s="32"/>
+      <c r="F104" s="32"/>
+      <c r="G104" s="32"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="61" t="s">
+      <c r="A105" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="B105" s="51"/>
-      <c r="C105" s="25"/>
-      <c r="D105" s="19"/>
-      <c r="E105" s="19"/>
-      <c r="F105" s="19"/>
-      <c r="G105" s="92"/>
-      <c r="H105" s="61"/>
+      <c r="B105" s="48"/>
+      <c r="C105" s="22"/>
+      <c r="D105" s="16"/>
+      <c r="E105" s="16"/>
+      <c r="F105" s="16"/>
+      <c r="G105" s="84"/>
+      <c r="H105" s="58"/>
       <c r="I105" s="10"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="62" t="s">
+      <c r="A106" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B106" s="56"/>
-      <c r="C106" s="52"/>
-      <c r="D106" s="53"/>
-      <c r="E106" s="53"/>
-      <c r="F106" s="54"/>
-      <c r="G106" s="93"/>
-      <c r="H106" s="62"/>
+      <c r="B106" s="53"/>
+      <c r="C106" s="49"/>
+      <c r="D106" s="50"/>
+      <c r="E106" s="50"/>
+      <c r="F106" s="51"/>
+      <c r="G106" s="85"/>
+      <c r="H106" s="59"/>
       <c r="I106" s="10"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="62" t="s">
+      <c r="A107" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B107" s="56"/>
-      <c r="C107" s="52"/>
-      <c r="D107" s="53"/>
-      <c r="E107" s="55"/>
-      <c r="F107" s="53"/>
-      <c r="G107" s="93"/>
-      <c r="H107" s="62"/>
+      <c r="B107" s="53"/>
+      <c r="C107" s="49"/>
+      <c r="D107" s="50"/>
+      <c r="E107" s="52"/>
+      <c r="F107" s="50"/>
+      <c r="G107" s="85"/>
+      <c r="H107" s="59"/>
       <c r="I107" s="10"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="62" t="s">
+      <c r="A108" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B108" s="56"/>
-      <c r="C108" s="52"/>
-      <c r="D108" s="54"/>
-      <c r="E108" s="118" t="s">
+      <c r="B108" s="53"/>
+      <c r="C108" s="49"/>
+      <c r="D108" s="51"/>
+      <c r="E108" s="109" t="s">
         <v>46</v>
       </c>
-      <c r="F108" s="54"/>
-      <c r="G108" s="114"/>
-      <c r="H108" s="62"/>
+      <c r="F108" s="51"/>
+      <c r="G108" s="105"/>
+      <c r="H108" s="59"/>
       <c r="I108" s="10"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="62" t="s">
+      <c r="A109" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B109" s="56"/>
-      <c r="C109" s="52"/>
-      <c r="D109" s="53"/>
-      <c r="E109" s="54"/>
-      <c r="F109" s="54"/>
-      <c r="G109" s="93"/>
-      <c r="H109" s="62"/>
+      <c r="B109" s="53"/>
+      <c r="C109" s="49"/>
+      <c r="D109" s="50"/>
+      <c r="E109" s="51"/>
+      <c r="F109" s="51"/>
+      <c r="G109" s="85"/>
+      <c r="H109" s="59"/>
       <c r="I109" s="10"/>
     </row>
     <row r="110" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="63" t="s">
+      <c r="A110" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B110" s="60"/>
-      <c r="C110" s="115"/>
-      <c r="D110" s="116"/>
-      <c r="E110" s="59"/>
-      <c r="F110" s="116"/>
-      <c r="G110" s="117"/>
-      <c r="H110" s="63"/>
+      <c r="B110" s="57"/>
+      <c r="C110" s="106"/>
+      <c r="D110" s="107"/>
+      <c r="E110" s="56"/>
+      <c r="F110" s="107"/>
+      <c r="G110" s="108"/>
+      <c r="H110" s="60"/>
       <c r="I110" s="10"/>
     </row>
     <row r="111" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C111" s="35"/>
-      <c r="D111" s="35"/>
-      <c r="E111" s="35"/>
-      <c r="F111" s="35"/>
-      <c r="G111" s="35"/>
+      <c r="C111" s="32"/>
+      <c r="D111" s="32"/>
+      <c r="E111" s="32"/>
+      <c r="F111" s="32"/>
+      <c r="G111" s="32"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B112" s="8"/>
-      <c r="C112" s="26"/>
-      <c r="D112" s="27"/>
-      <c r="E112" s="27"/>
-      <c r="F112" s="27"/>
-      <c r="G112" s="47"/>
+      <c r="C112" s="23"/>
+      <c r="D112" s="24"/>
+      <c r="E112" s="24"/>
+      <c r="F112" s="24"/>
+      <c r="G112" s="44"/>
       <c r="H112" s="1"/>
       <c r="I112" s="10"/>
     </row>
@@ -2880,11 +2979,11 @@
         <v>1</v>
       </c>
       <c r="B113" s="10"/>
-      <c r="C113" s="43"/>
-      <c r="D113" s="38"/>
-      <c r="E113" s="37"/>
-      <c r="F113" s="38"/>
-      <c r="G113" s="106"/>
+      <c r="C113" s="40"/>
+      <c r="D113" s="35"/>
+      <c r="E113" s="34"/>
+      <c r="F113" s="35"/>
+      <c r="G113" s="97"/>
       <c r="H113" s="2"/>
       <c r="I113" s="10"/>
     </row>
@@ -2893,11 +2992,11 @@
         <v>2</v>
       </c>
       <c r="B114" s="10"/>
-      <c r="C114" s="36"/>
-      <c r="D114" s="44"/>
-      <c r="E114" s="37"/>
-      <c r="F114" s="38"/>
-      <c r="G114" s="110"/>
+      <c r="C114" s="33"/>
+      <c r="D114" s="41"/>
+      <c r="E114" s="34"/>
+      <c r="F114" s="35"/>
+      <c r="G114" s="101"/>
       <c r="H114" s="2"/>
       <c r="I114" s="10"/>
     </row>
@@ -2906,11 +3005,11 @@
         <v>3</v>
       </c>
       <c r="B115" s="10"/>
-      <c r="C115" s="36"/>
-      <c r="D115" s="38"/>
-      <c r="E115" s="37"/>
-      <c r="F115" s="38"/>
-      <c r="G115" s="106"/>
+      <c r="C115" s="33"/>
+      <c r="D115" s="35"/>
+      <c r="E115" s="34"/>
+      <c r="F115" s="35"/>
+      <c r="G115" s="97"/>
       <c r="H115" s="2"/>
       <c r="I115" s="10"/>
     </row>
@@ -2919,11 +3018,11 @@
         <v>4</v>
       </c>
       <c r="B116" s="10"/>
-      <c r="C116" s="36"/>
-      <c r="D116" s="38"/>
-      <c r="E116" s="37"/>
-      <c r="F116" s="38"/>
-      <c r="G116" s="106"/>
+      <c r="C116" s="33"/>
+      <c r="D116" s="35"/>
+      <c r="E116" s="34"/>
+      <c r="F116" s="35"/>
+      <c r="G116" s="97"/>
       <c r="H116" s="2"/>
       <c r="I116" s="10"/>
     </row>
@@ -2932,11 +3031,11 @@
         <v>5</v>
       </c>
       <c r="B117" s="9"/>
-      <c r="C117" s="39"/>
-      <c r="D117" s="42"/>
-      <c r="E117" s="41"/>
-      <c r="F117" s="42"/>
-      <c r="G117" s="107"/>
+      <c r="C117" s="36"/>
+      <c r="D117" s="39"/>
+      <c r="E117" s="38"/>
+      <c r="F117" s="39"/>
+      <c r="G117" s="98"/>
       <c r="H117" s="3"/>
       <c r="I117" s="10"/>
     </row>
@@ -2944,49 +3043,49 @@
       <c r="A118" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B118" s="91">
-        <v>0</v>
-      </c>
-      <c r="C118" s="69">
+      <c r="B118" s="83">
+        <v>0</v>
+      </c>
+      <c r="C118" s="66">
         <f>SUM(C113:C117)</f>
         <v>0</v>
       </c>
-      <c r="D118" s="70">
+      <c r="D118" s="67">
         <f t="shared" ref="D118:G118" si="12">SUM(D113:D117)</f>
         <v>0</v>
       </c>
-      <c r="E118" s="70">
+      <c r="E118" s="67">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="F118" s="70">
+      <c r="F118" s="67">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G118" s="71">
+      <c r="G118" s="68">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="H118" s="108"/>
+      <c r="H118" s="99"/>
       <c r="I118" s="10"/>
     </row>
     <row r="119" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C119" s="35"/>
-      <c r="D119" s="35"/>
-      <c r="E119" s="35"/>
-      <c r="F119" s="35"/>
-      <c r="G119" s="35"/>
+      <c r="C119" s="32"/>
+      <c r="D119" s="32"/>
+      <c r="E119" s="32"/>
+      <c r="F119" s="32"/>
+      <c r="G119" s="32"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B120" s="8"/>
-      <c r="C120" s="26"/>
-      <c r="D120" s="27"/>
-      <c r="E120" s="27"/>
-      <c r="F120" s="27"/>
-      <c r="G120" s="47"/>
+      <c r="C120" s="23"/>
+      <c r="D120" s="24"/>
+      <c r="E120" s="24"/>
+      <c r="F120" s="24"/>
+      <c r="G120" s="44"/>
       <c r="H120" s="1"/>
       <c r="I120" s="10"/>
     </row>
@@ -2995,11 +3094,11 @@
         <v>1</v>
       </c>
       <c r="B121" s="10"/>
-      <c r="C121" s="43"/>
-      <c r="D121" s="38"/>
-      <c r="E121" s="37"/>
-      <c r="F121" s="37"/>
-      <c r="G121" s="106"/>
+      <c r="C121" s="40"/>
+      <c r="D121" s="35"/>
+      <c r="E121" s="34"/>
+      <c r="F121" s="34"/>
+      <c r="G121" s="97"/>
       <c r="H121" s="2"/>
       <c r="I121" s="10"/>
     </row>
@@ -3008,11 +3107,11 @@
         <v>2</v>
       </c>
       <c r="B122" s="10"/>
-      <c r="C122" s="43"/>
-      <c r="D122" s="38"/>
-      <c r="E122" s="37"/>
-      <c r="F122" s="44"/>
-      <c r="G122" s="106"/>
+      <c r="C122" s="40"/>
+      <c r="D122" s="35"/>
+      <c r="E122" s="34"/>
+      <c r="F122" s="41"/>
+      <c r="G122" s="97"/>
       <c r="H122" s="2"/>
       <c r="I122" s="10"/>
     </row>
@@ -3021,11 +3120,11 @@
         <v>3</v>
       </c>
       <c r="B123" s="10"/>
-      <c r="C123" s="43"/>
-      <c r="D123" s="38"/>
-      <c r="E123" s="37"/>
-      <c r="F123" s="37"/>
-      <c r="G123" s="106"/>
+      <c r="C123" s="40"/>
+      <c r="D123" s="35"/>
+      <c r="E123" s="34"/>
+      <c r="F123" s="34"/>
+      <c r="G123" s="97"/>
       <c r="H123" s="2"/>
       <c r="I123" s="10"/>
     </row>
@@ -3034,11 +3133,11 @@
         <v>4</v>
       </c>
       <c r="B124" s="10"/>
-      <c r="C124" s="43"/>
-      <c r="D124" s="37"/>
-      <c r="E124" s="37"/>
-      <c r="F124" s="37"/>
-      <c r="G124" s="112"/>
+      <c r="C124" s="40"/>
+      <c r="D124" s="34"/>
+      <c r="E124" s="34"/>
+      <c r="F124" s="34"/>
+      <c r="G124" s="103"/>
       <c r="H124" s="2"/>
       <c r="I124" s="10"/>
     </row>
@@ -3047,11 +3146,11 @@
         <v>5</v>
       </c>
       <c r="B125" s="9"/>
-      <c r="C125" s="46"/>
-      <c r="D125" s="42"/>
-      <c r="E125" s="40"/>
-      <c r="F125" s="42"/>
-      <c r="G125" s="113"/>
+      <c r="C125" s="43"/>
+      <c r="D125" s="39"/>
+      <c r="E125" s="37"/>
+      <c r="F125" s="39"/>
+      <c r="G125" s="104"/>
       <c r="H125" s="3"/>
       <c r="I125" s="10"/>
     </row>
@@ -3059,49 +3158,49 @@
       <c r="A126" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B126" s="91">
-        <v>0</v>
-      </c>
-      <c r="C126" s="69">
+      <c r="B126" s="83">
+        <v>0</v>
+      </c>
+      <c r="C126" s="66">
         <f t="shared" ref="C126:G126" si="13">SUM(C121:C125)</f>
         <v>0</v>
       </c>
-      <c r="D126" s="70">
+      <c r="D126" s="67">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="E126" s="70">
+      <c r="E126" s="67">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F126" s="70">
+      <c r="F126" s="67">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G126" s="71">
+      <c r="G126" s="68">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="H126" s="108"/>
+      <c r="H126" s="99"/>
       <c r="I126" s="10"/>
     </row>
     <row r="127" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C127" s="35"/>
-      <c r="D127" s="35"/>
-      <c r="E127" s="35"/>
-      <c r="F127" s="35"/>
-      <c r="G127" s="35"/>
+      <c r="C127" s="32"/>
+      <c r="D127" s="32"/>
+      <c r="E127" s="32"/>
+      <c r="F127" s="32"/>
+      <c r="G127" s="32"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B128" s="8"/>
-      <c r="C128" s="26"/>
-      <c r="D128" s="27"/>
-      <c r="E128" s="27"/>
-      <c r="F128" s="27"/>
-      <c r="G128" s="47"/>
+      <c r="C128" s="23"/>
+      <c r="D128" s="24"/>
+      <c r="E128" s="24"/>
+      <c r="F128" s="24"/>
+      <c r="G128" s="44"/>
       <c r="H128" s="1"/>
       <c r="I128" s="10"/>
     </row>
@@ -3110,11 +3209,11 @@
         <v>1</v>
       </c>
       <c r="B129" s="10"/>
-      <c r="C129" s="36"/>
-      <c r="D129" s="38"/>
-      <c r="E129" s="44"/>
-      <c r="F129" s="37"/>
-      <c r="G129" s="110"/>
+      <c r="C129" s="33"/>
+      <c r="D129" s="35"/>
+      <c r="E129" s="41"/>
+      <c r="F129" s="34"/>
+      <c r="G129" s="101"/>
       <c r="H129" s="2"/>
       <c r="I129" s="10"/>
     </row>
@@ -3123,11 +3222,11 @@
         <v>2</v>
       </c>
       <c r="B130" s="10"/>
-      <c r="C130" s="43"/>
-      <c r="D130" s="44"/>
-      <c r="E130" s="37"/>
-      <c r="F130" s="37"/>
-      <c r="G130" s="110"/>
+      <c r="C130" s="40"/>
+      <c r="D130" s="41"/>
+      <c r="E130" s="34"/>
+      <c r="F130" s="34"/>
+      <c r="G130" s="101"/>
       <c r="H130" s="2"/>
       <c r="I130" s="10"/>
     </row>
@@ -3136,11 +3235,11 @@
         <v>3</v>
       </c>
       <c r="B131" s="10"/>
-      <c r="C131" s="43"/>
-      <c r="D131" s="38"/>
-      <c r="E131" s="37"/>
-      <c r="F131" s="37"/>
-      <c r="G131" s="106"/>
+      <c r="C131" s="40"/>
+      <c r="D131" s="35"/>
+      <c r="E131" s="34"/>
+      <c r="F131" s="34"/>
+      <c r="G131" s="97"/>
       <c r="H131" s="2"/>
       <c r="I131" s="10"/>
     </row>
@@ -3149,11 +3248,11 @@
         <v>4</v>
       </c>
       <c r="B132" s="10"/>
-      <c r="C132" s="43"/>
-      <c r="D132" s="37"/>
-      <c r="E132" s="37"/>
-      <c r="F132" s="37"/>
-      <c r="G132" s="106"/>
+      <c r="C132" s="40"/>
+      <c r="D132" s="34"/>
+      <c r="E132" s="34"/>
+      <c r="F132" s="34"/>
+      <c r="G132" s="97"/>
       <c r="H132" s="2"/>
       <c r="I132" s="10"/>
     </row>
@@ -3162,11 +3261,11 @@
         <v>5</v>
       </c>
       <c r="B133" s="9"/>
-      <c r="C133" s="39"/>
-      <c r="D133" s="42"/>
-      <c r="E133" s="41"/>
-      <c r="F133" s="42"/>
-      <c r="G133" s="107"/>
+      <c r="C133" s="36"/>
+      <c r="D133" s="39"/>
+      <c r="E133" s="38"/>
+      <c r="F133" s="39"/>
+      <c r="G133" s="98"/>
       <c r="H133" s="3"/>
       <c r="I133" s="10"/>
     </row>
@@ -3174,281 +3273,281 @@
       <c r="A134" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B134" s="91">
-        <v>0</v>
-      </c>
-      <c r="C134" s="69">
+      <c r="B134" s="83">
+        <v>0</v>
+      </c>
+      <c r="C134" s="66">
         <f t="shared" ref="C134:G134" si="14">SUM(C129:C133)</f>
         <v>0</v>
       </c>
-      <c r="D134" s="70">
+      <c r="D134" s="67">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="E134" s="70">
+      <c r="E134" s="67">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="F134" s="70">
+      <c r="F134" s="67">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="G134" s="71">
+      <c r="G134" s="68">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="H134" s="108"/>
+      <c r="H134" s="99"/>
       <c r="I134" s="10"/>
     </row>
     <row r="135" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C135" s="35"/>
-      <c r="D135" s="35"/>
-      <c r="E135" s="35"/>
-      <c r="F135" s="35"/>
-      <c r="G135" s="35"/>
+      <c r="C135" s="32"/>
+      <c r="D135" s="32"/>
+      <c r="E135" s="32"/>
+      <c r="F135" s="32"/>
+      <c r="G135" s="32"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B136" s="26"/>
-      <c r="C136" s="26"/>
-      <c r="D136" s="27"/>
-      <c r="E136" s="27"/>
-      <c r="F136" s="27"/>
-      <c r="G136" s="47"/>
-      <c r="H136" s="28"/>
+      <c r="B136" s="23"/>
+      <c r="C136" s="23"/>
+      <c r="D136" s="24"/>
+      <c r="E136" s="24"/>
+      <c r="F136" s="24"/>
+      <c r="G136" s="44"/>
+      <c r="H136" s="25"/>
       <c r="I136" s="10"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B137" s="29"/>
-      <c r="C137" s="29"/>
-      <c r="D137" s="30"/>
-      <c r="E137" s="30"/>
-      <c r="F137" s="30"/>
-      <c r="G137" s="48"/>
-      <c r="H137" s="31"/>
+      <c r="B137" s="26"/>
+      <c r="C137" s="26"/>
+      <c r="D137" s="27"/>
+      <c r="E137" s="27"/>
+      <c r="F137" s="27"/>
+      <c r="G137" s="45"/>
+      <c r="H137" s="28"/>
       <c r="I137" s="10"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B138" s="29"/>
-      <c r="C138" s="29"/>
-      <c r="D138" s="30"/>
-      <c r="E138" s="30"/>
-      <c r="F138" s="30"/>
-      <c r="G138" s="48"/>
-      <c r="H138" s="31"/>
+      <c r="B138" s="26"/>
+      <c r="C138" s="26"/>
+      <c r="D138" s="27"/>
+      <c r="E138" s="27"/>
+      <c r="F138" s="27"/>
+      <c r="G138" s="45"/>
+      <c r="H138" s="28"/>
       <c r="I138" s="10"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B139" s="29"/>
-      <c r="C139" s="29"/>
-      <c r="D139" s="30"/>
-      <c r="E139" s="30"/>
-      <c r="F139" s="30"/>
-      <c r="G139" s="48"/>
-      <c r="H139" s="31"/>
+      <c r="B139" s="26"/>
+      <c r="C139" s="26"/>
+      <c r="D139" s="27"/>
+      <c r="E139" s="27"/>
+      <c r="F139" s="27"/>
+      <c r="G139" s="45"/>
+      <c r="H139" s="28"/>
       <c r="I139" s="10"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B140" s="29"/>
-      <c r="C140" s="29"/>
-      <c r="D140" s="30"/>
-      <c r="E140" s="30"/>
-      <c r="F140" s="30"/>
-      <c r="G140" s="48"/>
-      <c r="H140" s="31"/>
+      <c r="B140" s="26"/>
+      <c r="C140" s="26"/>
+      <c r="D140" s="27"/>
+      <c r="E140" s="27"/>
+      <c r="F140" s="27"/>
+      <c r="G140" s="45"/>
+      <c r="H140" s="28"/>
       <c r="I140" s="10"/>
     </row>
     <row r="141" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B141" s="32"/>
-      <c r="C141" s="32"/>
-      <c r="D141" s="33"/>
-      <c r="E141" s="33"/>
-      <c r="F141" s="33"/>
-      <c r="G141" s="49"/>
-      <c r="H141" s="34"/>
+      <c r="B141" s="29"/>
+      <c r="C141" s="29"/>
+      <c r="D141" s="30"/>
+      <c r="E141" s="30"/>
+      <c r="F141" s="30"/>
+      <c r="G141" s="46"/>
+      <c r="H141" s="31"/>
       <c r="I141" s="10"/>
     </row>
     <row r="142" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B142" s="91">
-        <v>0</v>
-      </c>
-      <c r="C142" s="69">
+      <c r="B142" s="83">
+        <v>0</v>
+      </c>
+      <c r="C142" s="66">
         <f t="shared" ref="C142:G142" si="15">SUM(C137:C141)</f>
         <v>0</v>
       </c>
-      <c r="D142" s="70">
+      <c r="D142" s="67">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="E142" s="70">
+      <c r="E142" s="67">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="F142" s="70">
+      <c r="F142" s="67">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G142" s="71">
+      <c r="G142" s="68">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="H142" s="111"/>
+      <c r="H142" s="102"/>
       <c r="I142" s="10"/>
     </row>
     <row r="143" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="35"/>
-      <c r="C143" s="35"/>
-      <c r="D143" s="35"/>
-      <c r="E143" s="35"/>
-      <c r="F143" s="35"/>
-      <c r="G143" s="35"/>
-      <c r="H143" s="50"/>
+      <c r="B143" s="32"/>
+      <c r="C143" s="32"/>
+      <c r="D143" s="32"/>
+      <c r="E143" s="32"/>
+      <c r="F143" s="32"/>
+      <c r="G143" s="32"/>
+      <c r="H143" s="47"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B144" s="26"/>
-      <c r="C144" s="26"/>
-      <c r="D144" s="27"/>
-      <c r="E144" s="27"/>
-      <c r="F144" s="27"/>
-      <c r="G144" s="47"/>
-      <c r="H144" s="28"/>
+      <c r="B144" s="23"/>
+      <c r="C144" s="23"/>
+      <c r="D144" s="24"/>
+      <c r="E144" s="24"/>
+      <c r="F144" s="24"/>
+      <c r="G144" s="44"/>
+      <c r="H144" s="25"/>
       <c r="I144" s="10"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B145" s="29"/>
-      <c r="C145" s="29"/>
-      <c r="D145" s="30"/>
-      <c r="E145" s="30"/>
-      <c r="F145" s="30"/>
-      <c r="G145" s="48"/>
-      <c r="H145" s="31"/>
+      <c r="B145" s="26"/>
+      <c r="C145" s="26"/>
+      <c r="D145" s="27"/>
+      <c r="E145" s="27"/>
+      <c r="F145" s="27"/>
+      <c r="G145" s="45"/>
+      <c r="H145" s="28"/>
       <c r="I145" s="10"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B146" s="29"/>
-      <c r="C146" s="29"/>
-      <c r="D146" s="30"/>
-      <c r="E146" s="30"/>
-      <c r="F146" s="30"/>
-      <c r="G146" s="48"/>
-      <c r="H146" s="31"/>
+      <c r="B146" s="26"/>
+      <c r="C146" s="26"/>
+      <c r="D146" s="27"/>
+      <c r="E146" s="27"/>
+      <c r="F146" s="27"/>
+      <c r="G146" s="45"/>
+      <c r="H146" s="28"/>
       <c r="I146" s="10"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B147" s="29"/>
-      <c r="C147" s="29"/>
-      <c r="D147" s="30"/>
-      <c r="E147" s="30"/>
-      <c r="F147" s="30"/>
-      <c r="G147" s="48"/>
-      <c r="H147" s="31"/>
+      <c r="B147" s="26"/>
+      <c r="C147" s="26"/>
+      <c r="D147" s="27"/>
+      <c r="E147" s="27"/>
+      <c r="F147" s="27"/>
+      <c r="G147" s="45"/>
+      <c r="H147" s="28"/>
       <c r="I147" s="10"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B148" s="29"/>
-      <c r="C148" s="29"/>
-      <c r="D148" s="30"/>
-      <c r="E148" s="30"/>
-      <c r="F148" s="30"/>
-      <c r="G148" s="48"/>
-      <c r="H148" s="31"/>
+      <c r="B148" s="26"/>
+      <c r="C148" s="26"/>
+      <c r="D148" s="27"/>
+      <c r="E148" s="27"/>
+      <c r="F148" s="27"/>
+      <c r="G148" s="45"/>
+      <c r="H148" s="28"/>
       <c r="I148" s="10"/>
     </row>
     <row r="149" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B149" s="32"/>
-      <c r="C149" s="32"/>
-      <c r="D149" s="33"/>
-      <c r="E149" s="33"/>
-      <c r="F149" s="33"/>
-      <c r="G149" s="49"/>
-      <c r="H149" s="34"/>
+      <c r="B149" s="29"/>
+      <c r="C149" s="29"/>
+      <c r="D149" s="30"/>
+      <c r="E149" s="30"/>
+      <c r="F149" s="30"/>
+      <c r="G149" s="46"/>
+      <c r="H149" s="31"/>
       <c r="I149" s="10"/>
     </row>
     <row r="150" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B150" s="91">
-        <v>0</v>
-      </c>
-      <c r="C150" s="69">
+      <c r="B150" s="83">
+        <v>0</v>
+      </c>
+      <c r="C150" s="66">
         <f t="shared" ref="C150:G150" si="16">SUM(C145:C149)</f>
         <v>0</v>
       </c>
-      <c r="D150" s="70">
+      <c r="D150" s="67">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="E150" s="70">
+      <c r="E150" s="67">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="F150" s="70">
+      <c r="F150" s="67">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="G150" s="71">
+      <c r="G150" s="68">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="H150" s="108"/>
+      <c r="H150" s="99"/>
       <c r="I150" s="10"/>
     </row>
     <row r="151" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C151" s="35"/>
-      <c r="D151" s="35"/>
-      <c r="E151" s="35"/>
-      <c r="F151" s="35"/>
-      <c r="G151" s="35"/>
+      <c r="C151" s="32"/>
+      <c r="D151" s="32"/>
+      <c r="E151" s="32"/>
+      <c r="F151" s="32"/>
+      <c r="G151" s="32"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B152" s="8"/>
-      <c r="C152" s="26"/>
-      <c r="D152" s="27"/>
-      <c r="E152" s="27"/>
-      <c r="F152" s="27"/>
-      <c r="G152" s="47"/>
+      <c r="C152" s="23"/>
+      <c r="D152" s="24"/>
+      <c r="E152" s="24"/>
+      <c r="F152" s="24"/>
+      <c r="G152" s="44"/>
       <c r="H152" s="1"/>
       <c r="I152" s="10"/>
     </row>
@@ -3457,11 +3556,11 @@
         <v>1</v>
       </c>
       <c r="B153" s="10"/>
-      <c r="C153" s="43"/>
-      <c r="D153" s="38"/>
-      <c r="E153" s="37"/>
-      <c r="F153" s="37"/>
-      <c r="G153" s="106"/>
+      <c r="C153" s="40"/>
+      <c r="D153" s="35"/>
+      <c r="E153" s="34"/>
+      <c r="F153" s="34"/>
+      <c r="G153" s="97"/>
       <c r="H153" s="2"/>
       <c r="I153" s="10"/>
     </row>
@@ -3470,11 +3569,11 @@
         <v>2</v>
       </c>
       <c r="B154" s="10"/>
-      <c r="C154" s="36"/>
-      <c r="D154" s="38"/>
-      <c r="E154" s="37"/>
-      <c r="F154" s="38"/>
-      <c r="G154" s="106"/>
+      <c r="C154" s="33"/>
+      <c r="D154" s="35"/>
+      <c r="E154" s="34"/>
+      <c r="F154" s="35"/>
+      <c r="G154" s="97"/>
       <c r="H154" s="2"/>
       <c r="I154" s="10"/>
     </row>
@@ -3483,11 +3582,11 @@
         <v>3</v>
       </c>
       <c r="B155" s="10"/>
-      <c r="C155" s="36"/>
-      <c r="D155" s="44"/>
-      <c r="E155" s="37"/>
-      <c r="F155" s="37"/>
-      <c r="G155" s="106"/>
+      <c r="C155" s="33"/>
+      <c r="D155" s="41"/>
+      <c r="E155" s="34"/>
+      <c r="F155" s="34"/>
+      <c r="G155" s="97"/>
       <c r="H155" s="2"/>
       <c r="I155" s="10"/>
     </row>
@@ -3496,11 +3595,11 @@
         <v>4</v>
       </c>
       <c r="B156" s="10"/>
-      <c r="C156" s="36"/>
-      <c r="D156" s="38"/>
-      <c r="E156" s="37"/>
-      <c r="F156" s="37"/>
-      <c r="G156" s="106"/>
+      <c r="C156" s="33"/>
+      <c r="D156" s="35"/>
+      <c r="E156" s="34"/>
+      <c r="F156" s="34"/>
+      <c r="G156" s="97"/>
       <c r="H156" s="2"/>
       <c r="I156" s="10"/>
     </row>
@@ -3509,11 +3608,11 @@
         <v>5</v>
       </c>
       <c r="B157" s="9"/>
-      <c r="C157" s="39"/>
-      <c r="D157" s="42"/>
-      <c r="E157" s="40"/>
-      <c r="F157" s="40"/>
-      <c r="G157" s="109"/>
+      <c r="C157" s="36"/>
+      <c r="D157" s="39"/>
+      <c r="E157" s="37"/>
+      <c r="F157" s="37"/>
+      <c r="G157" s="100"/>
       <c r="H157" s="3"/>
       <c r="I157" s="10"/>
     </row>
@@ -3521,49 +3620,49 @@
       <c r="A158" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B158" s="91">
-        <v>0</v>
-      </c>
-      <c r="C158" s="69">
+      <c r="B158" s="83">
+        <v>0</v>
+      </c>
+      <c r="C158" s="66">
         <f t="shared" ref="C158:G158" si="17">SUM(C153:C157)</f>
         <v>0</v>
       </c>
-      <c r="D158" s="70">
+      <c r="D158" s="67">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="E158" s="70">
+      <c r="E158" s="67">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="F158" s="70">
+      <c r="F158" s="67">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="G158" s="71">
+      <c r="G158" s="68">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="H158" s="108"/>
+      <c r="H158" s="99"/>
       <c r="I158" s="10"/>
     </row>
     <row r="159" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C159" s="35"/>
-      <c r="D159" s="35"/>
-      <c r="E159" s="35"/>
-      <c r="F159" s="35"/>
-      <c r="G159" s="35"/>
+      <c r="C159" s="32"/>
+      <c r="D159" s="32"/>
+      <c r="E159" s="32"/>
+      <c r="F159" s="32"/>
+      <c r="G159" s="32"/>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B160" s="8"/>
-      <c r="C160" s="26"/>
-      <c r="D160" s="27"/>
-      <c r="E160" s="27"/>
-      <c r="F160" s="27"/>
-      <c r="G160" s="47"/>
+      <c r="C160" s="23"/>
+      <c r="D160" s="24"/>
+      <c r="E160" s="24"/>
+      <c r="F160" s="24"/>
+      <c r="G160" s="44"/>
       <c r="H160" s="1"/>
       <c r="I160" s="10"/>
     </row>
@@ -3572,11 +3671,11 @@
         <v>1</v>
       </c>
       <c r="B161" s="10"/>
-      <c r="C161" s="36"/>
-      <c r="D161" s="38"/>
-      <c r="E161" s="44"/>
-      <c r="F161" s="38"/>
-      <c r="G161" s="106"/>
+      <c r="C161" s="33"/>
+      <c r="D161" s="35"/>
+      <c r="E161" s="41"/>
+      <c r="F161" s="35"/>
+      <c r="G161" s="97"/>
       <c r="H161" s="2"/>
       <c r="I161" s="10"/>
     </row>
@@ -3585,11 +3684,11 @@
         <v>2</v>
       </c>
       <c r="B162" s="10"/>
-      <c r="C162" s="36"/>
-      <c r="D162" s="44"/>
-      <c r="E162" s="37"/>
-      <c r="F162" s="38"/>
-      <c r="G162" s="106"/>
+      <c r="C162" s="33"/>
+      <c r="D162" s="41"/>
+      <c r="E162" s="34"/>
+      <c r="F162" s="35"/>
+      <c r="G162" s="97"/>
       <c r="H162" s="2"/>
       <c r="I162" s="10"/>
     </row>
@@ -3598,11 +3697,11 @@
         <v>3</v>
       </c>
       <c r="B163" s="10"/>
-      <c r="C163" s="36"/>
-      <c r="D163" s="44"/>
-      <c r="E163" s="44"/>
-      <c r="F163" s="37"/>
-      <c r="G163" s="106"/>
+      <c r="C163" s="33"/>
+      <c r="D163" s="41"/>
+      <c r="E163" s="41"/>
+      <c r="F163" s="34"/>
+      <c r="G163" s="97"/>
       <c r="H163" s="2"/>
       <c r="I163" s="10"/>
     </row>
@@ -3611,11 +3710,11 @@
         <v>4</v>
       </c>
       <c r="B164" s="10"/>
-      <c r="C164" s="36"/>
-      <c r="D164" s="44"/>
-      <c r="E164" s="37"/>
-      <c r="F164" s="37"/>
-      <c r="G164" s="106"/>
+      <c r="C164" s="33"/>
+      <c r="D164" s="41"/>
+      <c r="E164" s="34"/>
+      <c r="F164" s="34"/>
+      <c r="G164" s="97"/>
       <c r="H164" s="2"/>
       <c r="I164" s="10"/>
     </row>
@@ -3624,11 +3723,11 @@
         <v>5</v>
       </c>
       <c r="B165" s="9"/>
-      <c r="C165" s="39"/>
-      <c r="D165" s="40"/>
-      <c r="E165" s="40"/>
-      <c r="F165" s="40"/>
-      <c r="G165" s="109"/>
+      <c r="C165" s="36"/>
+      <c r="D165" s="37"/>
+      <c r="E165" s="37"/>
+      <c r="F165" s="37"/>
+      <c r="G165" s="100"/>
       <c r="H165" s="3"/>
       <c r="I165" s="10"/>
     </row>
@@ -3636,49 +3735,49 @@
       <c r="A166" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B166" s="91">
-        <v>0</v>
-      </c>
-      <c r="C166" s="69">
+      <c r="B166" s="83">
+        <v>0</v>
+      </c>
+      <c r="C166" s="66">
         <f t="shared" ref="C166:G166" si="18">SUM(C161:C165)</f>
         <v>0</v>
       </c>
-      <c r="D166" s="70">
+      <c r="D166" s="67">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E166" s="70">
+      <c r="E166" s="67">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="F166" s="70">
+      <c r="F166" s="67">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="G166" s="71">
+      <c r="G166" s="68">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="H166" s="108"/>
+      <c r="H166" s="99"/>
       <c r="I166" s="10"/>
     </row>
     <row r="167" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C167" s="35"/>
-      <c r="D167" s="35"/>
-      <c r="E167" s="35"/>
-      <c r="F167" s="35"/>
-      <c r="G167" s="35"/>
+      <c r="C167" s="32"/>
+      <c r="D167" s="32"/>
+      <c r="E167" s="32"/>
+      <c r="F167" s="32"/>
+      <c r="G167" s="32"/>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B168" s="8"/>
-      <c r="C168" s="26"/>
-      <c r="D168" s="27"/>
-      <c r="E168" s="27"/>
-      <c r="F168" s="27"/>
-      <c r="G168" s="47"/>
+      <c r="C168" s="23"/>
+      <c r="D168" s="24"/>
+      <c r="E168" s="24"/>
+      <c r="F168" s="24"/>
+      <c r="G168" s="44"/>
       <c r="H168" s="1"/>
       <c r="I168" s="10"/>
     </row>
@@ -3687,11 +3786,11 @@
         <v>1</v>
       </c>
       <c r="B169" s="10"/>
-      <c r="C169" s="36"/>
-      <c r="D169" s="38"/>
-      <c r="E169" s="44"/>
-      <c r="F169" s="37"/>
-      <c r="G169" s="106"/>
+      <c r="C169" s="33"/>
+      <c r="D169" s="35"/>
+      <c r="E169" s="41"/>
+      <c r="F169" s="34"/>
+      <c r="G169" s="97"/>
       <c r="H169" s="2"/>
       <c r="I169" s="10"/>
     </row>
@@ -3700,11 +3799,11 @@
         <v>2</v>
       </c>
       <c r="B170" s="10"/>
-      <c r="C170" s="36"/>
-      <c r="D170" s="44"/>
-      <c r="E170" s="37"/>
-      <c r="F170" s="38"/>
-      <c r="G170" s="106"/>
+      <c r="C170" s="33"/>
+      <c r="D170" s="41"/>
+      <c r="E170" s="34"/>
+      <c r="F170" s="35"/>
+      <c r="G170" s="97"/>
       <c r="H170" s="2"/>
       <c r="I170" s="10"/>
     </row>
@@ -3713,11 +3812,11 @@
         <v>3</v>
       </c>
       <c r="B171" s="10"/>
-      <c r="C171" s="36"/>
-      <c r="D171" s="38"/>
-      <c r="E171" s="37"/>
-      <c r="F171" s="37"/>
-      <c r="G171" s="106"/>
+      <c r="C171" s="33"/>
+      <c r="D171" s="35"/>
+      <c r="E171" s="34"/>
+      <c r="F171" s="34"/>
+      <c r="G171" s="97"/>
       <c r="H171" s="2"/>
       <c r="I171" s="10"/>
     </row>
@@ -3726,11 +3825,11 @@
         <v>4</v>
       </c>
       <c r="B172" s="10"/>
-      <c r="C172" s="36"/>
-      <c r="D172" s="37"/>
-      <c r="E172" s="37"/>
-      <c r="F172" s="37"/>
-      <c r="G172" s="106"/>
+      <c r="C172" s="33"/>
+      <c r="D172" s="34"/>
+      <c r="E172" s="34"/>
+      <c r="F172" s="34"/>
+      <c r="G172" s="97"/>
       <c r="H172" s="2"/>
       <c r="I172" s="10"/>
     </row>
@@ -3739,11 +3838,11 @@
         <v>5</v>
       </c>
       <c r="B173" s="9"/>
-      <c r="C173" s="39"/>
-      <c r="D173" s="42"/>
-      <c r="E173" s="40"/>
-      <c r="F173" s="42"/>
-      <c r="G173" s="107"/>
+      <c r="C173" s="36"/>
+      <c r="D173" s="39"/>
+      <c r="E173" s="37"/>
+      <c r="F173" s="39"/>
+      <c r="G173" s="98"/>
       <c r="H173" s="3"/>
       <c r="I173" s="10"/>
     </row>
@@ -3751,38 +3850,38 @@
       <c r="A174" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B174" s="91">
-        <v>0</v>
-      </c>
-      <c r="C174" s="69">
+      <c r="B174" s="83">
+        <v>0</v>
+      </c>
+      <c r="C174" s="66">
         <f t="shared" ref="C174:G174" si="19">SUM(C169:C173)</f>
         <v>0</v>
       </c>
-      <c r="D174" s="70">
+      <c r="D174" s="67">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="E174" s="70">
+      <c r="E174" s="67">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F174" s="70">
+      <c r="F174" s="67">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="G174" s="71">
+      <c r="G174" s="68">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="H174" s="108"/>
+      <c r="H174" s="99"/>
       <c r="I174" s="10"/>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C175" s="35"/>
-      <c r="D175" s="35"/>
-      <c r="E175" s="35"/>
-      <c r="F175" s="35"/>
-      <c r="G175" s="35"/>
+      <c r="C175" s="32"/>
+      <c r="D175" s="32"/>
+      <c r="E175" s="32"/>
+      <c r="F175" s="32"/>
+      <c r="G175" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uren Registratie 10-02-2016 & SubRol Update & Mappenstructuur begonnen met Ruben
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="50">
   <si>
     <t>Fahrettin</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Ruben: Ziek</t>
+  </si>
+  <si>
+    <t>Lara: Ziek</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -848,21 +851,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -872,9 +866,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -902,6 +893,15 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
@@ -1189,7 +1189,7 @@
   <dimension ref="A1:L175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1205,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="137" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="117" t="s">
@@ -1249,15 +1249,15 @@
       <c r="H2" s="1"/>
       <c r="I2" s="83">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J2" s="76">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K2" s="81">
         <f>J2/I2</f>
-        <v>0.92307692307692313</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="L2" s="76" t="str">
         <f>C1</f>
@@ -1268,7 +1268,7 @@
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="142">
+      <c r="B3" s="138">
         <v>4</v>
       </c>
       <c r="C3" s="93">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="K3" s="77">
         <f>J3/I2</f>
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="L3" s="53" t="str">
         <f>D1</f>
@@ -1305,7 +1305,7 @@
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="142">
+      <c r="B4" s="138">
         <v>2</v>
       </c>
       <c r="C4" s="93">
@@ -1327,11 +1327,11 @@
       <c r="I4" s="10"/>
       <c r="J4" s="71">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K4" s="78">
         <f>J4/I2</f>
-        <v>0.38461538461538464</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="L4" s="71" t="str">
         <f>E1</f>
@@ -1342,7 +1342,7 @@
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="142">
+      <c r="B5" s="138">
         <v>2</v>
       </c>
       <c r="C5" s="93">
@@ -1364,7 +1364,7 @@
       <c r="I5" s="10"/>
       <c r="J5" s="79">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K5" s="80">
         <f>J5/I2</f>
@@ -1379,7 +1379,7 @@
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="142">
+      <c r="B6" s="138">
         <v>2</v>
       </c>
       <c r="C6" s="111">
@@ -1403,11 +1403,11 @@
       <c r="I6" s="10"/>
       <c r="J6" s="72">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K6" s="82">
         <f>J6/I2</f>
-        <v>0.96153846153846156</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="L6" s="72" t="str">
         <f>G1</f>
@@ -1418,7 +1418,7 @@
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="143">
+      <c r="B7" s="139">
         <v>8</v>
       </c>
       <c r="C7" s="112">
@@ -1446,7 +1446,7 @@
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="144">
+      <c r="B8" s="140">
         <f>B3+B4+B5+B6+B7</f>
         <v>18</v>
       </c>
@@ -1477,11 +1477,11 @@
       </c>
       <c r="K8" s="74">
         <f>SUM(K2:K7)</f>
-        <v>4.2692307692307692</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="140"/>
+      <c r="B9" s="136"/>
       <c r="C9" s="128"/>
       <c r="D9" s="128"/>
       <c r="E9" s="128"/>
@@ -1498,21 +1498,21 @@
       <c r="D10" s="130"/>
       <c r="E10" s="130"/>
       <c r="F10" s="130"/>
-      <c r="G10" s="131"/>
-      <c r="H10" s="14"/>
+      <c r="G10" s="130"/>
+      <c r="H10" s="147"/>
       <c r="I10" s="10"/>
       <c r="J10" s="88" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="145">
+      <c r="B11" s="141">
         <v>4</v>
       </c>
-      <c r="C11" s="147">
+      <c r="C11" s="143">
         <v>4</v>
       </c>
       <c r="D11" s="94">
@@ -1524,10 +1524,10 @@
       <c r="F11" s="94">
         <v>4</v>
       </c>
-      <c r="G11" s="96">
+      <c r="G11" s="94">
         <v>4</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="148" t="s">
         <v>48</v>
       </c>
       <c r="I11" s="10"/>
@@ -1535,11 +1535,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="145">
+      <c r="B12" s="141">
         <v>4</v>
       </c>
       <c r="C12" s="93">
@@ -1551,13 +1551,13 @@
       <c r="E12" s="116">
         <v>0</v>
       </c>
-      <c r="F12" s="148">
+      <c r="F12" s="144">
         <v>4</v>
       </c>
-      <c r="G12" s="96">
+      <c r="G12" s="94">
         <v>4</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="148" t="s">
         <v>48</v>
       </c>
       <c r="I12" s="10"/>
@@ -1569,13 +1569,27 @@
       <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="145"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="135"/>
-      <c r="E13" s="135"/>
-      <c r="F13" s="132"/>
-      <c r="G13" s="133"/>
-      <c r="H13" s="15"/>
+      <c r="B13" s="141">
+        <v>2</v>
+      </c>
+      <c r="C13" s="93">
+        <v>2</v>
+      </c>
+      <c r="D13" s="145">
+        <v>0</v>
+      </c>
+      <c r="E13" s="146">
+        <v>2</v>
+      </c>
+      <c r="F13" s="94">
+        <v>2</v>
+      </c>
+      <c r="G13" s="94">
+        <v>2</v>
+      </c>
+      <c r="H13" s="148" t="s">
+        <v>49</v>
+      </c>
       <c r="I13" s="10"/>
       <c r="J13" s="91" t="s">
         <v>44</v>
@@ -1585,13 +1599,13 @@
       <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="145"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="132"/>
-      <c r="G14" s="133"/>
-      <c r="H14" s="15"/>
+      <c r="B14" s="141"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="131"/>
+      <c r="H14" s="148"/>
       <c r="I14" s="10"/>
       <c r="J14" s="92" t="s">
         <v>45</v>
@@ -1601,26 +1615,26 @@
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="146"/>
-      <c r="C15" s="136"/>
-      <c r="D15" s="137"/>
-      <c r="E15" s="137"/>
-      <c r="F15" s="138"/>
-      <c r="G15" s="139"/>
-      <c r="H15" s="12"/>
+      <c r="B15" s="142"/>
+      <c r="C15" s="133"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="134"/>
+      <c r="F15" s="135"/>
+      <c r="G15" s="134"/>
+      <c r="H15" s="149"/>
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="144">
+      <c r="B16" s="140">
         <f>B11+B12+B13+B14+B15</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C16" s="125">
         <f t="shared" ref="C16:G16" si="1">SUM(C11:C15)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D16" s="126">
         <f t="shared" si="1"/>
@@ -1628,17 +1642,17 @@
       </c>
       <c r="E16" s="126">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" s="126">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G16" s="127">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="H16" s="95"/>
+        <v>10</v>
+      </c>
+      <c r="H16" s="12"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Uren Registratie 23-02-2016 & story plaatjes toegevoegd presentatie
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -524,7 +524,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -893,6 +893,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1182,7 +1188,7 @@
   <dimension ref="A1:L175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,15 +1248,15 @@
       <c r="H2" s="1"/>
       <c r="I2" s="54">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="J2" s="47">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="K2" s="52">
         <f>J2/I2</f>
-        <v>0.77192982456140347</v>
+        <v>0.78688524590163933</v>
       </c>
       <c r="L2" s="47" t="str">
         <f>C1</f>
@@ -1283,11 +1289,11 @@
       <c r="I3" s="10"/>
       <c r="J3" s="31">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K3" s="48">
         <f>J3/I2</f>
-        <v>0.85964912280701755</v>
+        <v>0.86885245901639341</v>
       </c>
       <c r="L3" s="31" t="str">
         <f>D1</f>
@@ -1320,11 +1326,11 @@
       <c r="I4" s="10"/>
       <c r="J4" s="42">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K4" s="49">
         <f>J4/I2</f>
-        <v>0.49122807017543857</v>
+        <v>0.52459016393442626</v>
       </c>
       <c r="L4" s="42" t="str">
         <f>E1</f>
@@ -1357,11 +1363,11 @@
       <c r="I5" s="10"/>
       <c r="J5" s="50">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="K5" s="51">
         <f>J5/I2</f>
-        <v>0.98245614035087714</v>
+        <v>0.98360655737704916</v>
       </c>
       <c r="L5" s="50" t="str">
         <f>F1</f>
@@ -1396,11 +1402,11 @@
       <c r="I6" s="10"/>
       <c r="J6" s="43">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="K6" s="53">
         <f>J6/I2</f>
-        <v>0.98245614035087714</v>
+        <v>0.98360655737704916</v>
       </c>
       <c r="L6" s="43" t="str">
         <f>G1</f>
@@ -1470,7 +1476,7 @@
       </c>
       <c r="K8" s="45">
         <f>SUM(K2:K7)</f>
-        <v>4.0877192982456139</v>
+        <v>4.1475409836065573</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1912,12 +1918,24 @@
       <c r="A28" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="113"/>
-      <c r="D28" s="108"/>
-      <c r="E28" s="104"/>
-      <c r="F28" s="104"/>
-      <c r="G28" s="114"/>
+      <c r="B28" s="10">
+        <v>4</v>
+      </c>
+      <c r="C28" s="142">
+        <v>4</v>
+      </c>
+      <c r="D28" s="97">
+        <v>4</v>
+      </c>
+      <c r="E28" s="61">
+        <v>4</v>
+      </c>
+      <c r="F28" s="61">
+        <v>4</v>
+      </c>
+      <c r="G28" s="143">
+        <v>4</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="10"/>
     </row>
@@ -1966,27 +1984,27 @@
       </c>
       <c r="B32" s="54">
         <f>B27+B28+B29+B30+B31</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C32" s="81">
         <f t="shared" ref="C32:G32" si="3">SUM(C27:C31)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D32" s="82">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E32" s="82">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F32" s="82">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G32" s="83">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H32" s="64"/>
       <c r="I32" s="10"/>

</xml_diff>

<commit_message>
Concept in juiste map gezet & Uren registratie tot vakantie
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -524,7 +524,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -899,6 +899,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1188,7 +1191,7 @@
   <dimension ref="A1:L175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,15 +1251,15 @@
       <c r="H2" s="1"/>
       <c r="I2" s="54">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="J2" s="47">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="K2" s="52">
         <f>J2/I2</f>
-        <v>0.78688524590163933</v>
+        <v>0.80303030303030298</v>
       </c>
       <c r="L2" s="47" t="str">
         <f>C1</f>
@@ -1289,11 +1292,11 @@
       <c r="I3" s="10"/>
       <c r="J3" s="31">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="K3" s="48">
         <f>J3/I2</f>
-        <v>0.86885245901639341</v>
+        <v>0.87878787878787878</v>
       </c>
       <c r="L3" s="31" t="str">
         <f>D1</f>
@@ -1326,11 +1329,11 @@
       <c r="I4" s="10"/>
       <c r="J4" s="42">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="K4" s="49">
         <f>J4/I2</f>
-        <v>0.52459016393442626</v>
+        <v>0.56060606060606055</v>
       </c>
       <c r="L4" s="42" t="str">
         <f>E1</f>
@@ -1363,11 +1366,11 @@
       <c r="I5" s="10"/>
       <c r="J5" s="50">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="K5" s="51">
         <f>J5/I2</f>
-        <v>0.98360655737704916</v>
+        <v>0.98484848484848486</v>
       </c>
       <c r="L5" s="50" t="str">
         <f>F1</f>
@@ -1402,11 +1405,11 @@
       <c r="I6" s="10"/>
       <c r="J6" s="43">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="K6" s="53">
         <f>J6/I2</f>
-        <v>0.98360655737704916</v>
+        <v>0.98484848484848486</v>
       </c>
       <c r="L6" s="43" t="str">
         <f>G1</f>
@@ -1476,7 +1479,7 @@
       </c>
       <c r="K8" s="45">
         <f>SUM(K2:K7)</f>
-        <v>4.1475409836065573</v>
+        <v>4.2121212121212119</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1943,12 +1946,24 @@
       <c r="A29" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="104"/>
-      <c r="F29" s="104"/>
-      <c r="G29" s="106"/>
+      <c r="B29" s="10">
+        <v>0</v>
+      </c>
+      <c r="C29" s="67">
+        <v>0</v>
+      </c>
+      <c r="D29" s="72">
+        <v>0</v>
+      </c>
+      <c r="E29" s="72">
+        <v>0</v>
+      </c>
+      <c r="F29" s="72">
+        <v>0</v>
+      </c>
+      <c r="G29" s="121">
+        <v>0</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="10"/>
     </row>
@@ -1956,12 +1971,24 @@
       <c r="A30" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="115"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="104"/>
-      <c r="F30" s="104"/>
-      <c r="G30" s="106"/>
+      <c r="B30" s="10">
+        <v>1</v>
+      </c>
+      <c r="C30" s="94">
+        <v>1</v>
+      </c>
+      <c r="D30" s="61">
+        <v>1</v>
+      </c>
+      <c r="E30" s="61">
+        <v>1</v>
+      </c>
+      <c r="F30" s="61">
+        <v>1</v>
+      </c>
+      <c r="G30" s="63">
+        <v>1</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="10"/>
     </row>
@@ -1969,12 +1996,24 @@
       <c r="A31" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="109"/>
-      <c r="D31" s="111"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="110"/>
-      <c r="G31" s="116"/>
+      <c r="B31" s="9">
+        <v>4</v>
+      </c>
+      <c r="C31" s="68">
+        <v>4</v>
+      </c>
+      <c r="D31" s="101">
+        <v>4</v>
+      </c>
+      <c r="E31" s="101">
+        <v>4</v>
+      </c>
+      <c r="F31" s="71">
+        <v>4</v>
+      </c>
+      <c r="G31" s="144">
+        <v>4</v>
+      </c>
       <c r="H31" s="3"/>
       <c r="I31" s="10"/>
     </row>
@@ -1984,27 +2023,27 @@
       </c>
       <c r="B32" s="54">
         <f>B27+B28+B29+B30+B31</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C32" s="81">
         <f t="shared" ref="C32:G32" si="3">SUM(C27:C31)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D32" s="82">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E32" s="82">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F32" s="82">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G32" s="83">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H32" s="64"/>
       <c r="I32" s="10"/>

</xml_diff>

<commit_message>
Uren Registratie & Asest List Update & Scripts Netjes Gemaakt
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="60">
   <si>
     <t>Fahrettin</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>Lara: Ziek | Kevin: Bloed afname |</t>
+  </si>
+  <si>
+    <t>Lara: Ziek | Ruben: Ziek |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fahrettin: Ziek | </t>
   </si>
 </sst>
 </file>
@@ -530,7 +536,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -913,13 +919,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1208,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,15 +1272,15 @@
       <c r="H2" s="1"/>
       <c r="I2" s="54">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J2" s="47">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="K2" s="52">
         <f>J2/I2</f>
-        <v>0.77027027027027029</v>
+        <v>0.74390243902439024</v>
       </c>
       <c r="L2" s="47" t="str">
         <f>C1</f>
@@ -1310,11 +1313,11 @@
       <c r="I3" s="10"/>
       <c r="J3" s="31">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="K3" s="48">
         <f>J3/I2</f>
-        <v>0.83783783783783783</v>
+        <v>0.80487804878048785</v>
       </c>
       <c r="L3" s="31" t="str">
         <f>D1</f>
@@ -1347,11 +1350,11 @@
       <c r="I4" s="10"/>
       <c r="J4" s="42">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K4" s="49">
         <f>J4/I2</f>
-        <v>0.60810810810810811</v>
+        <v>0.59756097560975607</v>
       </c>
       <c r="L4" s="42" t="str">
         <f>E1</f>
@@ -1384,11 +1387,11 @@
       <c r="I5" s="10"/>
       <c r="J5" s="50">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="K5" s="51">
         <f>J5/I2</f>
-        <v>0.93243243243243246</v>
+        <v>0.93902439024390238</v>
       </c>
       <c r="L5" s="50" t="str">
         <f>F1</f>
@@ -1423,11 +1426,11 @@
       <c r="I6" s="10"/>
       <c r="J6" s="43">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="K6" s="53">
         <f>J6/I2</f>
-        <v>0.98648648648648651</v>
+        <v>0.98780487804878048</v>
       </c>
       <c r="L6" s="43" t="str">
         <f>G1</f>
@@ -1497,7 +1500,7 @@
       </c>
       <c r="K8" s="45">
         <f>SUM(K2:K7)</f>
-        <v>4.1351351351351351</v>
+        <v>4.0731707317073171</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2183,16 +2186,16 @@
       <c r="C42" s="145">
         <v>0</v>
       </c>
-      <c r="D42" s="146">
-        <v>4</v>
-      </c>
-      <c r="E42" s="146">
-        <v>4</v>
-      </c>
-      <c r="F42" s="146">
-        <v>4</v>
-      </c>
-      <c r="G42" s="147">
+      <c r="D42" s="61">
+        <v>4</v>
+      </c>
+      <c r="E42" s="61">
+        <v>4</v>
+      </c>
+      <c r="F42" s="61">
+        <v>4</v>
+      </c>
+      <c r="G42" s="63">
         <v>4</v>
       </c>
       <c r="H42" s="2" t="s">
@@ -2207,19 +2210,19 @@
       <c r="B43" s="10">
         <v>4</v>
       </c>
-      <c r="C43" s="148">
+      <c r="C43" s="60">
         <v>4</v>
       </c>
       <c r="D43" s="96">
         <v>0</v>
       </c>
-      <c r="E43" s="146">
+      <c r="E43" s="61">
         <v>4</v>
       </c>
       <c r="F43" s="96">
         <v>0</v>
       </c>
-      <c r="G43" s="147">
+      <c r="G43" s="63">
         <v>4</v>
       </c>
       <c r="H43" s="2" t="s">
@@ -2231,39 +2234,81 @@
       <c r="A44" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="107"/>
-      <c r="D44" s="104"/>
-      <c r="E44" s="104"/>
-      <c r="F44" s="105"/>
-      <c r="G44" s="106"/>
-      <c r="H44" s="2"/>
+      <c r="B44" s="10">
+        <v>2</v>
+      </c>
+      <c r="C44" s="67">
+        <v>0</v>
+      </c>
+      <c r="D44" s="61">
+        <v>2</v>
+      </c>
+      <c r="E44" s="61">
+        <v>2</v>
+      </c>
+      <c r="F44" s="95">
+        <v>2</v>
+      </c>
+      <c r="G44" s="63">
+        <v>2</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="113"/>
-      <c r="D45" s="104"/>
-      <c r="E45" s="104"/>
-      <c r="F45" s="104"/>
-      <c r="G45" s="106"/>
-      <c r="H45" s="2"/>
+      <c r="B45" s="10">
+        <v>2</v>
+      </c>
+      <c r="C45" s="146">
+        <v>0</v>
+      </c>
+      <c r="D45" s="61">
+        <v>2</v>
+      </c>
+      <c r="E45" s="61">
+        <v>2</v>
+      </c>
+      <c r="F45" s="61">
+        <v>2</v>
+      </c>
+      <c r="G45" s="63">
+        <v>2</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="125"/>
-      <c r="D46" s="110"/>
-      <c r="E46" s="110"/>
-      <c r="F46" s="110"/>
-      <c r="G46" s="116"/>
-      <c r="H46" s="3"/>
+      <c r="B46" s="9">
+        <v>4</v>
+      </c>
+      <c r="C46" s="147">
+        <v>4</v>
+      </c>
+      <c r="D46" s="102">
+        <v>0</v>
+      </c>
+      <c r="E46" s="102">
+        <v>0</v>
+      </c>
+      <c r="F46" s="71">
+        <v>4</v>
+      </c>
+      <c r="G46" s="144">
+        <v>4</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="I46" s="10"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2272,27 +2317,27 @@
       </c>
       <c r="B47" s="54">
         <f>B42+B43+B44+B45+B46</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C47" s="81">
         <f t="shared" ref="C47:G47" si="4">SUM(C42:C46)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D47" s="82">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E47" s="82">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F47" s="82">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G47" s="83">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="H47" s="64"/>
       <c r="I47" s="10"/>

</xml_diff>

<commit_message>
Uren Registratie 21-03-2016 & Kleine bug fixes
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,15 +1229,15 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="J2" s="18">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="K2" s="19">
         <f>J2/I2</f>
-        <v>0.73786407766990292</v>
+        <v>0.74766355140186913</v>
       </c>
       <c r="L2" s="18" t="str">
         <f>C1</f>
@@ -1270,11 +1270,11 @@
       <c r="I3" s="26"/>
       <c r="J3" s="27">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="K3" s="28">
         <f>J3/I2</f>
-        <v>0.76699029126213591</v>
+        <v>0.77570093457943923</v>
       </c>
       <c r="L3" s="27" t="str">
         <f>D1</f>
@@ -1307,11 +1307,11 @@
       <c r="I4" s="26"/>
       <c r="J4" s="29">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K4" s="30">
         <f>J4/I2</f>
-        <v>0.64077669902912626</v>
+        <v>0.65420560747663548</v>
       </c>
       <c r="L4" s="29" t="str">
         <f>E1</f>
@@ -1344,11 +1344,11 @@
       <c r="I5" s="26"/>
       <c r="J5" s="31">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="K5" s="32">
         <f>J5/I2</f>
-        <v>0.95145631067961167</v>
+        <v>0.95327102803738317</v>
       </c>
       <c r="L5" s="31" t="str">
         <f>F1</f>
@@ -1383,11 +1383,11 @@
       <c r="I6" s="26"/>
       <c r="J6" s="34">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="K6" s="35">
         <f>J6/I2</f>
-        <v>0.99029126213592233</v>
+        <v>0.99065420560747663</v>
       </c>
       <c r="L6" s="34" t="str">
         <f>G1</f>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K8" s="50">
         <f>SUM(K2:K7)</f>
-        <v>4.0873786407766985</v>
+        <v>4.1214953271028039</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2504,12 +2504,24 @@
       <c r="A58" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="26"/>
-      <c r="C58" s="95"/>
-      <c r="D58" s="90"/>
-      <c r="E58" s="91"/>
-      <c r="F58" s="90"/>
-      <c r="G58" s="92"/>
+      <c r="B58" s="26">
+        <v>4</v>
+      </c>
+      <c r="C58" s="22">
+        <v>4</v>
+      </c>
+      <c r="D58" s="57">
+        <v>4</v>
+      </c>
+      <c r="E58" s="60">
+        <v>4</v>
+      </c>
+      <c r="F58" s="57">
+        <v>4</v>
+      </c>
+      <c r="G58" s="24">
+        <v>4</v>
+      </c>
       <c r="H58" s="25"/>
       <c r="I58" s="26"/>
     </row>
@@ -2570,27 +2582,28 @@
         <v>6</v>
       </c>
       <c r="B63" s="17">
-        <v>0</v>
+        <f>B58+B59+B60+B61+B62</f>
+        <v>4</v>
       </c>
       <c r="C63" s="46">
         <f t="shared" ref="C63:G63" si="6">SUM(C58:C62)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D63" s="47">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E63" s="47">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F63" s="47">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G63" s="48">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H63" s="49"/>
       <c r="I63" s="26"/>

</xml_diff>

<commit_message>
Menu & HUD af
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="47">
   <si>
     <t>Fahrettin</t>
   </si>
@@ -165,90 +165,6 @@
   </si>
   <si>
     <t>MEI VAKANTIE</t>
-  </si>
-  <si>
-    <t>Ruben: Ziek</t>
-  </si>
-  <si>
-    <t>Fahrettin: Opa Ziekenhuis |</t>
-  </si>
-  <si>
-    <t>Ruben: Ziek |</t>
-  </si>
-  <si>
-    <t>Lara: Ziek |</t>
-  </si>
-  <si>
-    <t>Fahrettin: Géén Zin | Lara: Ziek | Ruben: Ziek |</t>
-  </si>
-  <si>
-    <t>Fahrettin: Te Laat | Lara: Te Laat |</t>
-  </si>
-  <si>
-    <t>Kevin: Tandarts | Lara: Ziek | Fahrettin: Vader Ziekenhuis |</t>
-  </si>
-  <si>
-    <t>Lara: Ziek | Fahrettin: Vader Ziekenhuis |</t>
-  </si>
-  <si>
-    <t>Fahrettin: Vader Ziekenhuis |</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fahrettin: Telefoon Lader Stuk | </t>
-  </si>
-  <si>
-    <t>Lara: Ziek | Kevin: Bloed afname |</t>
-  </si>
-  <si>
-    <t>Lara: Ziek | Ruben: Ziek |</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fahrettin: Ziek | </t>
-  </si>
-  <si>
-    <t>Fahrettin: Ziek | Lara: Ziek |</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fahrettin: Te Laat Wakker | </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ruben: Ziek | Mack: Te Laat | </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lara: Geen melding | </t>
-  </si>
-  <si>
-    <t>Rubeb: Ziekenhuis |</t>
-  </si>
-  <si>
-    <t>Fahrettin: Te Laat Wakker | Lara: Ziek |</t>
-  </si>
-  <si>
-    <t>Lara: Geen reden opgegeven |</t>
-  </si>
-  <si>
-    <t>Mack: Batman vs Superman |</t>
-  </si>
-  <si>
-    <t>Fahrettin: Gemeente zaken |</t>
-  </si>
-  <si>
-    <t>2de Paasdag</t>
-  </si>
-  <si>
-    <t>Goeie Vrijdag</t>
-  </si>
-  <si>
-    <t>Opendag</t>
-  </si>
-  <si>
-    <t>Lerarendag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fahrettin: Thuis Stuff | </t>
-  </si>
-  <si>
-    <t>Fahrettin: Thuis Stuff |</t>
   </si>
 </sst>
 </file>
@@ -562,7 +478,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -868,9 +784,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1209,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,11 +1188,11 @@
       </c>
       <c r="J2" s="18">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="K2" s="19">
         <f>J2/I2</f>
-        <v>0.62745098039215685</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="L2" s="18" t="str">
         <f>C1</f>
@@ -1312,11 +1225,11 @@
       <c r="I3" s="26"/>
       <c r="J3" s="27">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="K3" s="28">
         <f>J3/I2</f>
-        <v>0.6470588235294118</v>
+        <v>0.68627450980392157</v>
       </c>
       <c r="L3" s="27" t="str">
         <f>D1</f>
@@ -1349,11 +1262,11 @@
       <c r="I4" s="26"/>
       <c r="J4" s="29">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K4" s="30">
         <f>J4/I2</f>
-        <v>0.65359477124183007</v>
+        <v>0.71895424836601307</v>
       </c>
       <c r="L4" s="29" t="str">
         <f>E1</f>
@@ -1386,11 +1299,11 @@
       <c r="I5" s="26"/>
       <c r="J5" s="31">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="K5" s="32">
         <f>J5/I2</f>
-        <v>0.86274509803921573</v>
+        <v>0.92810457516339873</v>
       </c>
       <c r="L5" s="31" t="str">
         <f>F1</f>
@@ -1419,17 +1332,15 @@
       <c r="G6" s="24">
         <v>1</v>
       </c>
-      <c r="H6" s="25" t="s">
-        <v>48</v>
-      </c>
+      <c r="H6" s="25"/>
       <c r="I6" s="26"/>
       <c r="J6" s="34">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="K6" s="35">
         <f>J6/I2</f>
-        <v>0.87581699346405228</v>
+        <v>0.94117647058823528</v>
       </c>
       <c r="L6" s="34" t="str">
         <f>G1</f>
@@ -1458,9 +1369,7 @@
       <c r="G7" s="42">
         <v>7</v>
       </c>
-      <c r="H7" s="43" t="s">
-        <v>62</v>
-      </c>
+      <c r="H7" s="43"/>
       <c r="I7" s="26"/>
       <c r="L7" s="45"/>
     </row>
@@ -1499,7 +1408,7 @@
       </c>
       <c r="K8" s="50">
         <f>SUM(K2:K7)</f>
-        <v>3.6666666666666665</v>
+        <v>3.9803921568627452</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1547,9 +1456,7 @@
       <c r="G11" s="23">
         <v>4</v>
       </c>
-      <c r="H11" s="20" t="s">
-        <v>49</v>
-      </c>
+      <c r="H11" s="20"/>
       <c r="I11" s="26"/>
       <c r="J11" s="56" t="s">
         <v>42</v>
@@ -1577,9 +1484,7 @@
       <c r="G12" s="23">
         <v>4</v>
       </c>
-      <c r="H12" s="20" t="s">
-        <v>49</v>
-      </c>
+      <c r="H12" s="20"/>
       <c r="I12" s="26"/>
       <c r="J12" s="58" t="s">
         <v>43</v>
@@ -1607,9 +1512,7 @@
       <c r="G13" s="23">
         <v>2</v>
       </c>
-      <c r="H13" s="20" t="s">
-        <v>50</v>
-      </c>
+      <c r="H13" s="20"/>
       <c r="I13" s="26"/>
       <c r="J13" s="61" t="s">
         <v>44</v>
@@ -1637,9 +1540,7 @@
       <c r="G14" s="23">
         <v>1</v>
       </c>
-      <c r="H14" s="20" t="s">
-        <v>51</v>
-      </c>
+      <c r="H14" s="20"/>
       <c r="I14" s="26"/>
       <c r="J14" s="62" t="s">
         <v>45</v>
@@ -1667,9 +1568,7 @@
       <c r="G15" s="39">
         <v>8</v>
       </c>
-      <c r="H15" s="36" t="s">
-        <v>47</v>
-      </c>
+      <c r="H15" s="36"/>
       <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1745,9 +1644,7 @@
       <c r="G19" s="24">
         <v>4</v>
       </c>
-      <c r="H19" s="25" t="s">
-        <v>52</v>
-      </c>
+      <c r="H19" s="25"/>
       <c r="I19" s="26"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1772,9 +1669,7 @@
       <c r="G20" s="24">
         <v>4</v>
       </c>
-      <c r="H20" s="25" t="s">
-        <v>49</v>
-      </c>
+      <c r="H20" s="25"/>
       <c r="I20" s="26"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1799,9 +1694,7 @@
       <c r="G21" s="24">
         <v>1</v>
       </c>
-      <c r="H21" s="25" t="s">
-        <v>53</v>
-      </c>
+      <c r="H21" s="25"/>
       <c r="I21" s="26"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1826,9 +1719,7 @@
       <c r="G22" s="24">
         <v>2</v>
       </c>
-      <c r="H22" s="25" t="s">
-        <v>54</v>
-      </c>
+      <c r="H22" s="25"/>
       <c r="I22" s="26"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1838,8 +1729,8 @@
       <c r="B23" s="63">
         <v>4</v>
       </c>
-      <c r="C23" s="67">
-        <v>0</v>
+      <c r="C23" s="38">
+        <v>4</v>
       </c>
       <c r="D23" s="39">
         <v>4</v>
@@ -1853,9 +1744,7 @@
       <c r="G23" s="42">
         <v>4</v>
       </c>
-      <c r="H23" s="43" t="s">
-        <v>55</v>
-      </c>
+      <c r="H23" s="43"/>
       <c r="I23" s="26"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1868,7 +1757,7 @@
       </c>
       <c r="C24" s="46">
         <f t="shared" ref="C24:G24" si="2">SUM(C19:C23)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D24" s="47">
         <f t="shared" si="2"/>
@@ -2179,8 +2068,8 @@
       <c r="B42" s="26">
         <v>4</v>
       </c>
-      <c r="C42" s="87">
-        <v>0</v>
+      <c r="C42" s="54">
+        <v>4</v>
       </c>
       <c r="D42" s="23">
         <v>4</v>
@@ -2194,9 +2083,7 @@
       <c r="G42" s="24">
         <v>4</v>
       </c>
-      <c r="H42" s="25" t="s">
-        <v>56</v>
-      </c>
+      <c r="H42" s="25"/>
       <c r="I42" s="26"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2221,9 +2108,7 @@
       <c r="G43" s="24">
         <v>4</v>
       </c>
-      <c r="H43" s="25" t="s">
-        <v>57</v>
-      </c>
+      <c r="H43" s="25"/>
       <c r="I43" s="26"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2248,9 +2133,7 @@
       <c r="G44" s="24">
         <v>2</v>
       </c>
-      <c r="H44" s="25" t="s">
-        <v>60</v>
-      </c>
+      <c r="H44" s="25"/>
       <c r="I44" s="26"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2275,9 +2158,7 @@
       <c r="G45" s="24">
         <v>2</v>
       </c>
-      <c r="H45" s="25" t="s">
-        <v>59</v>
-      </c>
+      <c r="H45" s="25"/>
       <c r="I45" s="26"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2302,9 +2183,7 @@
       <c r="G46" s="71">
         <v>4</v>
       </c>
-      <c r="H46" s="43" t="s">
-        <v>58</v>
-      </c>
+      <c r="H46" s="43"/>
       <c r="I46" s="26"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2317,7 +2196,7 @@
       </c>
       <c r="C47" s="46">
         <f t="shared" ref="C47:G47" si="4">SUM(C42:C46)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D47" s="47">
         <f t="shared" si="4"/>
@@ -2380,9 +2259,7 @@
       <c r="G50" s="24">
         <v>4</v>
       </c>
-      <c r="H50" s="25" t="s">
-        <v>61</v>
-      </c>
+      <c r="H50" s="25"/>
       <c r="I50" s="26"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2407,9 +2284,7 @@
       <c r="G51" s="24">
         <v>4</v>
       </c>
-      <c r="H51" s="25" t="s">
-        <v>63</v>
-      </c>
+      <c r="H51" s="25"/>
       <c r="I51" s="26"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2444,8 +2319,8 @@
       <c r="B53" s="26">
         <v>2</v>
       </c>
-      <c r="C53" s="33">
-        <v>0</v>
+      <c r="C53" s="22">
+        <v>2</v>
       </c>
       <c r="D53" s="79">
         <v>0</v>
@@ -2459,9 +2334,7 @@
       <c r="G53" s="24">
         <v>2</v>
       </c>
-      <c r="H53" s="25" t="s">
-        <v>65</v>
-      </c>
+      <c r="H53" s="25"/>
       <c r="I53" s="26"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2486,9 +2359,7 @@
       <c r="G54" s="71">
         <v>4</v>
       </c>
-      <c r="H54" s="43" t="s">
-        <v>64</v>
-      </c>
+      <c r="H54" s="43"/>
       <c r="I54" s="26"/>
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2501,7 +2372,7 @@
       </c>
       <c r="C55" s="46">
         <f t="shared" ref="C55:G55" si="5">SUM(C50:C54)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D55" s="47">
         <f t="shared" si="5"/>
@@ -2589,9 +2460,7 @@
       <c r="G59" s="24">
         <v>4</v>
       </c>
-      <c r="H59" s="25" t="s">
-        <v>66</v>
-      </c>
+      <c r="H59" s="25"/>
       <c r="I59" s="26"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2616,9 +2485,7 @@
       <c r="G60" s="24">
         <v>2</v>
       </c>
-      <c r="H60" s="25" t="s">
-        <v>68</v>
-      </c>
+      <c r="H60" s="25"/>
       <c r="I60" s="26"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2643,9 +2510,7 @@
       <c r="G61" s="70">
         <v>0</v>
       </c>
-      <c r="H61" s="25" t="s">
-        <v>67</v>
-      </c>
+      <c r="H61" s="25"/>
       <c r="I61" s="26"/>
     </row>
     <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2658,7 +2523,7 @@
       <c r="C62" s="67">
         <v>0</v>
       </c>
-      <c r="D62" s="122">
+      <c r="D62" s="121">
         <v>0</v>
       </c>
       <c r="E62" s="64">
@@ -2670,9 +2535,7 @@
       <c r="G62" s="85">
         <v>0</v>
       </c>
-      <c r="H62" s="43" t="s">
-        <v>70</v>
-      </c>
+      <c r="H62" s="43"/>
       <c r="I62" s="26"/>
     </row>
     <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2735,7 +2598,7 @@
       <c r="B66" s="103">
         <v>0</v>
       </c>
-      <c r="C66" s="127">
+      <c r="C66" s="126">
         <v>0</v>
       </c>
       <c r="D66" s="78">
@@ -2747,12 +2610,10 @@
       <c r="F66" s="78">
         <v>0</v>
       </c>
-      <c r="G66" s="128">
-        <v>0</v>
-      </c>
-      <c r="H66" s="107" t="s">
-        <v>69</v>
-      </c>
+      <c r="G66" s="127">
+        <v>0</v>
+      </c>
+      <c r="H66" s="107"/>
       <c r="I66" s="26"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2762,7 +2623,7 @@
       <c r="B67" s="103">
         <v>0</v>
       </c>
-      <c r="C67" s="127">
+      <c r="C67" s="126">
         <v>0</v>
       </c>
       <c r="D67" s="78">
@@ -2774,12 +2635,10 @@
       <c r="F67" s="78">
         <v>0</v>
       </c>
-      <c r="G67" s="128">
-        <v>0</v>
-      </c>
-      <c r="H67" s="107" t="s">
-        <v>71</v>
-      </c>
+      <c r="G67" s="127">
+        <v>0</v>
+      </c>
+      <c r="H67" s="107"/>
       <c r="I67" s="26"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2789,7 +2648,7 @@
       <c r="B68" s="103">
         <v>0</v>
       </c>
-      <c r="C68" s="127">
+      <c r="C68" s="126">
         <v>0</v>
       </c>
       <c r="D68" s="78">
@@ -2801,12 +2660,10 @@
       <c r="F68" s="78">
         <v>0</v>
       </c>
-      <c r="G68" s="128">
-        <v>0</v>
-      </c>
-      <c r="H68" s="107" t="s">
-        <v>72</v>
-      </c>
+      <c r="G68" s="127">
+        <v>0</v>
+      </c>
+      <c r="H68" s="107"/>
       <c r="I68" s="26"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2816,24 +2673,22 @@
       <c r="B69" s="103">
         <v>2</v>
       </c>
-      <c r="C69" s="127">
-        <v>0</v>
-      </c>
-      <c r="D69" s="129">
-        <v>2</v>
-      </c>
-      <c r="E69" s="129">
-        <v>2</v>
-      </c>
-      <c r="F69" s="129">
-        <v>2</v>
-      </c>
-      <c r="G69" s="130">
-        <v>2</v>
-      </c>
-      <c r="H69" s="107" t="s">
-        <v>73</v>
-      </c>
+      <c r="C69" s="126">
+        <v>0</v>
+      </c>
+      <c r="D69" s="128">
+        <v>2</v>
+      </c>
+      <c r="E69" s="128">
+        <v>2</v>
+      </c>
+      <c r="F69" s="128">
+        <v>2</v>
+      </c>
+      <c r="G69" s="129">
+        <v>2</v>
+      </c>
+      <c r="H69" s="107"/>
       <c r="I69" s="26"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2843,24 +2698,22 @@
       <c r="B70" s="108">
         <v>4</v>
       </c>
-      <c r="C70" s="133">
-        <v>0</v>
-      </c>
-      <c r="D70" s="131">
-        <v>4</v>
-      </c>
-      <c r="E70" s="131">
-        <v>4</v>
-      </c>
-      <c r="F70" s="131">
-        <v>4</v>
-      </c>
-      <c r="G70" s="132">
-        <v>4</v>
-      </c>
-      <c r="H70" s="112" t="s">
-        <v>73</v>
-      </c>
+      <c r="C70" s="132">
+        <v>0</v>
+      </c>
+      <c r="D70" s="130">
+        <v>4</v>
+      </c>
+      <c r="E70" s="130">
+        <v>4</v>
+      </c>
+      <c r="F70" s="130">
+        <v>4</v>
+      </c>
+      <c r="G70" s="131">
+        <v>4</v>
+      </c>
+      <c r="H70" s="112"/>
       <c r="I70" s="26"/>
     </row>
     <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2936,9 +2789,7 @@
       <c r="G74" s="24">
         <v>4</v>
       </c>
-      <c r="H74" s="25" t="s">
-        <v>74</v>
-      </c>
+      <c r="H74" s="25"/>
       <c r="I74" s="26"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -2963,9 +2814,7 @@
       <c r="G75" s="24">
         <v>4</v>
       </c>
-      <c r="H75" s="25" t="s">
-        <v>50</v>
-      </c>
+      <c r="H75" s="25"/>
       <c r="I75" s="26"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -2990,9 +2839,7 @@
       <c r="G76" s="24">
         <v>2</v>
       </c>
-      <c r="H76" s="25" t="s">
-        <v>74</v>
-      </c>
+      <c r="H76" s="25"/>
       <c r="I76" s="26"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3017,9 +2864,7 @@
       <c r="G77" s="24">
         <v>2</v>
       </c>
-      <c r="H77" s="25" t="s">
-        <v>50</v>
-      </c>
+      <c r="H77" s="25"/>
       <c r="I77" s="26"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3029,11 +2874,21 @@
       <c r="B78" s="63">
         <v>4</v>
       </c>
-      <c r="C78" s="96"/>
-      <c r="D78" s="98"/>
-      <c r="E78" s="98"/>
-      <c r="F78" s="98"/>
-      <c r="G78" s="100"/>
+      <c r="C78" s="67">
+        <v>0</v>
+      </c>
+      <c r="D78" s="39">
+        <v>4</v>
+      </c>
+      <c r="E78" s="39">
+        <v>4</v>
+      </c>
+      <c r="F78" s="39">
+        <v>4</v>
+      </c>
+      <c r="G78" s="71">
+        <v>4</v>
+      </c>
       <c r="H78" s="43"/>
       <c r="I78" s="26"/>
     </row>
@@ -3051,19 +2906,19 @@
       </c>
       <c r="D79" s="47">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E79" s="47">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F79" s="47">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G79" s="48">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H79" s="49"/>
       <c r="I79" s="26"/>
@@ -3095,11 +2950,21 @@
       <c r="B82" s="26">
         <v>4</v>
       </c>
-      <c r="C82" s="93"/>
-      <c r="D82" s="90"/>
-      <c r="E82" s="94"/>
-      <c r="F82" s="94"/>
-      <c r="G82" s="114"/>
+      <c r="C82" s="87">
+        <v>0</v>
+      </c>
+      <c r="D82" s="57">
+        <v>2</v>
+      </c>
+      <c r="E82" s="23">
+        <v>4</v>
+      </c>
+      <c r="F82" s="23">
+        <v>4</v>
+      </c>
+      <c r="G82" s="69">
+        <v>4</v>
+      </c>
       <c r="H82" s="25"/>
       <c r="I82" s="26"/>
     </row>
@@ -3110,19 +2975,19 @@
       <c r="B83" s="26">
         <v>4</v>
       </c>
-      <c r="C83" s="95">
-        <v>4</v>
-      </c>
-      <c r="D83" s="90">
-        <v>0</v>
-      </c>
-      <c r="E83" s="94">
-        <v>4</v>
-      </c>
-      <c r="F83" s="90">
-        <v>4</v>
-      </c>
-      <c r="G83" s="92">
+      <c r="C83" s="22">
+        <v>4</v>
+      </c>
+      <c r="D83" s="79">
+        <v>0</v>
+      </c>
+      <c r="E83" s="23">
+        <v>4</v>
+      </c>
+      <c r="F83" s="57">
+        <v>4</v>
+      </c>
+      <c r="G83" s="24">
         <v>4</v>
       </c>
       <c r="H83" s="25"/>
@@ -3135,11 +3000,21 @@
       <c r="B84" s="26">
         <v>2</v>
       </c>
-      <c r="C84" s="115"/>
-      <c r="D84" s="90"/>
-      <c r="E84" s="91"/>
-      <c r="F84" s="94"/>
-      <c r="G84" s="92"/>
+      <c r="C84" s="68">
+        <v>2</v>
+      </c>
+      <c r="D84" s="79">
+        <v>0</v>
+      </c>
+      <c r="E84" s="60">
+        <v>2</v>
+      </c>
+      <c r="F84" s="23">
+        <v>2</v>
+      </c>
+      <c r="G84" s="24">
+        <v>2</v>
+      </c>
       <c r="H84" s="25"/>
       <c r="I84" s="26"/>
     </row>
@@ -3169,7 +3044,7 @@
       <c r="D86" s="99"/>
       <c r="E86" s="98"/>
       <c r="F86" s="98"/>
-      <c r="G86" s="116"/>
+      <c r="G86" s="115"/>
       <c r="H86" s="43"/>
       <c r="I86" s="26"/>
     </row>
@@ -3183,23 +3058,23 @@
       </c>
       <c r="C87" s="46">
         <f t="shared" ref="C87:G87" si="9">SUM(C82:C86)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D87" s="47">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E87" s="47">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F87" s="47">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G87" s="48">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H87" s="49"/>
       <c r="I87" s="26"/>
@@ -3272,7 +3147,7 @@
       <c r="D93" s="94"/>
       <c r="E93" s="94"/>
       <c r="F93" s="90"/>
-      <c r="G93" s="117"/>
+      <c r="G93" s="116"/>
       <c r="H93" s="25"/>
       <c r="I93" s="26"/>
     </row>
@@ -3396,11 +3271,11 @@
         <v>5</v>
       </c>
       <c r="B102" s="63"/>
-      <c r="C102" s="118"/>
+      <c r="C102" s="117"/>
       <c r="D102" s="99"/>
       <c r="E102" s="98"/>
       <c r="F102" s="98"/>
-      <c r="G102" s="116"/>
+      <c r="G102" s="115"/>
       <c r="H102" s="43"/>
       <c r="I102" s="26"/>
     </row>
@@ -3445,7 +3320,7 @@
       <c r="A105" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="B105" s="119"/>
+      <c r="B105" s="118"/>
       <c r="C105" s="74"/>
       <c r="D105" s="73"/>
       <c r="E105" s="73"/>
@@ -3491,7 +3366,7 @@
         <v>46</v>
       </c>
       <c r="F108" s="55"/>
-      <c r="G108" s="120"/>
+      <c r="G108" s="119"/>
       <c r="H108" s="77"/>
       <c r="I108" s="26"/>
     </row>
@@ -3512,12 +3387,12 @@
       <c r="A110" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B110" s="121"/>
+      <c r="B110" s="120"/>
       <c r="C110" s="67"/>
-      <c r="D110" s="122"/>
+      <c r="D110" s="121"/>
       <c r="E110" s="64"/>
-      <c r="F110" s="122"/>
-      <c r="G110" s="123"/>
+      <c r="F110" s="121"/>
+      <c r="G110" s="122"/>
       <c r="H110" s="82"/>
       <c r="I110" s="26"/>
     </row>
@@ -3602,7 +3477,7 @@
       <c r="D117" s="99"/>
       <c r="E117" s="97"/>
       <c r="F117" s="99"/>
-      <c r="G117" s="116"/>
+      <c r="G117" s="115"/>
       <c r="H117" s="43"/>
       <c r="I117" s="26"/>
     </row>
@@ -3704,7 +3579,7 @@
       <c r="D124" s="94"/>
       <c r="E124" s="94"/>
       <c r="F124" s="94"/>
-      <c r="G124" s="117"/>
+      <c r="G124" s="116"/>
       <c r="H124" s="25"/>
       <c r="I124" s="26"/>
     </row>
@@ -3713,11 +3588,11 @@
         <v>5</v>
       </c>
       <c r="B125" s="63"/>
-      <c r="C125" s="118"/>
+      <c r="C125" s="117"/>
       <c r="D125" s="99"/>
       <c r="E125" s="98"/>
       <c r="F125" s="99"/>
-      <c r="G125" s="124"/>
+      <c r="G125" s="123"/>
       <c r="H125" s="43"/>
       <c r="I125" s="26"/>
     </row>
@@ -3832,7 +3707,7 @@
       <c r="D133" s="99"/>
       <c r="E133" s="97"/>
       <c r="F133" s="99"/>
-      <c r="G133" s="116"/>
+      <c r="G133" s="115"/>
       <c r="H133" s="43"/>
       <c r="I133" s="26"/>
     </row>
@@ -3978,7 +3853,7 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="H142" s="125"/>
+      <c r="H142" s="124"/>
       <c r="I142" s="26"/>
     </row>
     <row r="143" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3988,7 +3863,7 @@
       <c r="E143" s="45"/>
       <c r="F143" s="45"/>
       <c r="G143" s="45"/>
-      <c r="H143" s="126"/>
+      <c r="H143" s="125"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
@@ -4409,7 +4284,7 @@
       <c r="D173" s="99"/>
       <c r="E173" s="98"/>
       <c r="F173" s="99"/>
-      <c r="G173" s="116"/>
+      <c r="G173" s="115"/>
       <c r="H173" s="43"/>
       <c r="I173" s="26"/>
     </row>

</xml_diff>

<commit_message>
bug fix uren reg
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -1146,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J92" sqref="J92"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,7 +1208,7 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="J2" s="18">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="K2" s="19">
         <f>J2/I2</f>
-        <v>0.80829015544041449</v>
+        <v>0.77611940298507465</v>
       </c>
       <c r="L2" s="18" t="str">
         <f>C1</f>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="K3" s="28">
         <f>J3/I2</f>
-        <v>0.7098445595854922</v>
+        <v>0.68159203980099503</v>
       </c>
       <c r="L3" s="27" t="str">
         <f>D1</f>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="K4" s="30">
         <f>J4/I2</f>
-        <v>0.84974093264248707</v>
+        <v>0.8159203980099502</v>
       </c>
       <c r="L4" s="29" t="str">
         <f>E1</f>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="K5" s="32">
         <f>J5/I2</f>
-        <v>1.0155440414507773</v>
+        <v>0.97512437810945274</v>
       </c>
       <c r="L5" s="31" t="str">
         <f>F1</f>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="K6" s="35">
         <f>J6/I2</f>
-        <v>1.0259067357512954</v>
+        <v>0.9850746268656716</v>
       </c>
       <c r="L6" s="34" t="str">
         <f>G1</f>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="K8" s="50">
         <f>SUM(K2:K7)</f>
-        <v>4.409326424870466</v>
+        <v>4.233830845771144</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2833,7 +2833,7 @@
         <v>2</v>
       </c>
       <c r="B75" s="26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C75" s="54">
         <v>8</v>
@@ -2934,7 +2934,7 @@
       </c>
       <c r="B79" s="17">
         <f>B74+B75+B76+B77+B78</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C79" s="46">
         <f t="shared" ref="C79:G79" si="8">SUM(C74:C78)</f>
@@ -3036,7 +3036,7 @@
         <v>3</v>
       </c>
       <c r="B84" s="26">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C84" s="68">
         <v>6</v>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="B87" s="17">
         <f>B82+B83+B84+B85+B86</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C87" s="46">
         <f t="shared" ref="C87:G87" si="9">SUM(C82:C86)</f>

</xml_diff>

<commit_message>
Uren reg en lootpack
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -505,7 +505,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -858,6 +858,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1147,7 +1150,7 @@
   <dimension ref="A1:L175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,15 +1211,15 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="J2" s="18">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="K2" s="19">
         <f>J2/I2</f>
-        <v>0.77611940298507465</v>
+        <v>0.78260869565217395</v>
       </c>
       <c r="L2" s="18" t="str">
         <f>C1</f>
@@ -1249,11 +1252,11 @@
       <c r="I3" s="26"/>
       <c r="J3" s="27">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="K3" s="28">
         <f>J3/I2</f>
-        <v>0.68159203980099503</v>
+        <v>0.6908212560386473</v>
       </c>
       <c r="L3" s="27" t="str">
         <f>D1</f>
@@ -1286,11 +1289,11 @@
       <c r="I4" s="26"/>
       <c r="J4" s="29">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="K4" s="30">
         <f>J4/I2</f>
-        <v>0.8159203980099502</v>
+        <v>0.82125603864734298</v>
       </c>
       <c r="L4" s="29" t="str">
         <f>E1</f>
@@ -1323,11 +1326,11 @@
       <c r="I5" s="26"/>
       <c r="J5" s="31">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="K5" s="32">
         <f>J5/I2</f>
-        <v>0.97512437810945274</v>
+        <v>0.97584541062801933</v>
       </c>
       <c r="L5" s="31" t="str">
         <f>F1</f>
@@ -1360,11 +1363,11 @@
       <c r="I6" s="26"/>
       <c r="J6" s="34">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="K6" s="35">
         <f>J6/I2</f>
-        <v>0.9850746268656716</v>
+        <v>0.98550724637681164</v>
       </c>
       <c r="L6" s="34" t="str">
         <f>G1</f>
@@ -1432,7 +1435,7 @@
       </c>
       <c r="K8" s="50">
         <f>SUM(K2:K7)</f>
-        <v>4.233830845771144</v>
+        <v>4.2560386473429954</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3238,12 +3241,24 @@
       <c r="A93" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B93" s="26"/>
-      <c r="C93" s="95"/>
-      <c r="D93" s="94"/>
-      <c r="E93" s="94"/>
-      <c r="F93" s="90"/>
-      <c r="G93" s="115"/>
+      <c r="B93" s="26">
+        <v>2</v>
+      </c>
+      <c r="C93" s="22">
+        <v>2</v>
+      </c>
+      <c r="D93" s="23">
+        <v>2</v>
+      </c>
+      <c r="E93" s="23">
+        <v>2</v>
+      </c>
+      <c r="F93" s="57">
+        <v>2</v>
+      </c>
+      <c r="G93" s="132">
+        <v>2</v>
+      </c>
       <c r="H93" s="25"/>
       <c r="I93" s="26"/>
     </row>
@@ -3251,12 +3266,24 @@
       <c r="A94" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B94" s="63"/>
-      <c r="C94" s="96"/>
-      <c r="D94" s="99"/>
-      <c r="E94" s="97"/>
-      <c r="F94" s="98"/>
-      <c r="G94" s="100"/>
+      <c r="B94" s="63">
+        <v>4</v>
+      </c>
+      <c r="C94" s="38">
+        <v>4</v>
+      </c>
+      <c r="D94" s="41">
+        <v>4</v>
+      </c>
+      <c r="E94" s="65">
+        <v>4</v>
+      </c>
+      <c r="F94" s="39">
+        <v>4</v>
+      </c>
+      <c r="G94" s="71">
+        <v>4</v>
+      </c>
       <c r="H94" s="43"/>
       <c r="I94" s="26"/>
     </row>
@@ -3266,27 +3293,27 @@
       </c>
       <c r="B95" s="17">
         <f>B90+B91+B92+B93+B94</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C95" s="46">
         <f t="shared" ref="C95:G95" si="10">SUM(C90:C94)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D95" s="47">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E95" s="47">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F95" s="47">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G95" s="48">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H95" s="49"/>
       <c r="I95" s="26"/>

</xml_diff>

<commit_message>
kleine anapassingen bij presentatie en aanwezigheidscijfers
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2e Schooljaar\10. Game-Lab-2.1\Game-Lab-2.1\Algemeen\Uren Registratie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mack\Desktop\Game-Lab-2.1\Algemeen\Uren Registratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,15 +1211,15 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="J2" s="18">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="K2" s="19">
         <f>J2/I2</f>
-        <v>0.78260869565217395</v>
+        <v>0.79069767441860461</v>
       </c>
       <c r="L2" s="18" t="str">
         <f>C1</f>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="K3" s="28">
         <f>J3/I2</f>
-        <v>0.66183574879227058</v>
+        <v>0.63720930232558137</v>
       </c>
       <c r="L3" s="27" t="str">
         <f>D1</f>
@@ -1289,11 +1289,11 @@
       <c r="I4" s="26"/>
       <c r="J4" s="29">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="K4" s="30">
         <f>J4/I2</f>
-        <v>0.82125603864734298</v>
+        <v>0.82790697674418601</v>
       </c>
       <c r="L4" s="29" t="str">
         <f>E1</f>
@@ -1326,11 +1326,11 @@
       <c r="I5" s="26"/>
       <c r="J5" s="31">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="K5" s="32">
         <f>J5/I2</f>
-        <v>0.97584541062801933</v>
+        <v>0.97674418604651159</v>
       </c>
       <c r="L5" s="31" t="str">
         <f>F1</f>
@@ -1363,11 +1363,11 @@
       <c r="I6" s="26"/>
       <c r="J6" s="34">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="K6" s="35">
         <f>J6/I2</f>
-        <v>0.98550724637681164</v>
+        <v>0.98604651162790702</v>
       </c>
       <c r="L6" s="34" t="str">
         <f>G1</f>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="K8" s="50">
         <f>SUM(K2:K7)</f>
-        <v>4.2270531400966185</v>
+        <v>4.2186046511627904</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3344,12 +3344,24 @@
       <c r="A98" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B98" s="26"/>
-      <c r="C98" s="93"/>
-      <c r="D98" s="90"/>
-      <c r="E98" s="94"/>
-      <c r="F98" s="90"/>
-      <c r="G98" s="92"/>
+      <c r="B98" s="26">
+        <v>8</v>
+      </c>
+      <c r="C98" s="54">
+        <v>8</v>
+      </c>
+      <c r="D98" s="79">
+        <v>0</v>
+      </c>
+      <c r="E98" s="23">
+        <v>8</v>
+      </c>
+      <c r="F98" s="57">
+        <v>8</v>
+      </c>
+      <c r="G98" s="24">
+        <v>8</v>
+      </c>
       <c r="H98" s="25"/>
       <c r="I98" s="26"/>
     </row>
@@ -3370,12 +3382,24 @@
       <c r="A100" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B100" s="26"/>
-      <c r="C100" s="93"/>
-      <c r="D100" s="94"/>
-      <c r="E100" s="94"/>
-      <c r="F100" s="94"/>
-      <c r="G100" s="92"/>
+      <c r="B100" s="26">
+        <v>0</v>
+      </c>
+      <c r="C100" s="87">
+        <v>0</v>
+      </c>
+      <c r="D100" s="55">
+        <v>0</v>
+      </c>
+      <c r="E100" s="55">
+        <v>0</v>
+      </c>
+      <c r="F100" s="55">
+        <v>0</v>
+      </c>
+      <c r="G100" s="70">
+        <v>0</v>
+      </c>
       <c r="H100" s="25"/>
       <c r="I100" s="26"/>
     </row>
@@ -3410,11 +3434,12 @@
         <v>6</v>
       </c>
       <c r="B103" s="17">
-        <v>0</v>
+        <f>B98+B99+B100+B101+B102</f>
+        <v>8</v>
       </c>
       <c r="C103" s="46">
         <f t="shared" ref="C103:G103" si="11">SUM(C98:C102)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D103" s="47">
         <f t="shared" si="11"/>
@@ -3422,15 +3447,15 @@
       </c>
       <c r="E103" s="47">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F103" s="47">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G103" s="48">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H103" s="49"/>
       <c r="I103" s="26"/>

</xml_diff>

<commit_message>
Uren Registratie & Convo survivior
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I97" sqref="I97"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,15 +1211,15 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="J2" s="18">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="K2" s="19">
         <f>J2/I2</f>
-        <v>0.79452054794520544</v>
+        <v>0.80176211453744495</v>
       </c>
       <c r="L2" s="18" t="str">
         <f>C1</f>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="K3" s="28">
         <f>J3/I2</f>
-        <v>0.64383561643835618</v>
+        <v>0.62114537444933926</v>
       </c>
       <c r="L3" s="27" t="str">
         <f>D1</f>
@@ -1289,11 +1289,11 @@
       <c r="I4" s="26"/>
       <c r="J4" s="29">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="K4" s="30">
         <f>J4/I2</f>
-        <v>0.83105022831050224</v>
+        <v>0.83700440528634357</v>
       </c>
       <c r="L4" s="29" t="str">
         <f>E1</f>
@@ -1326,11 +1326,11 @@
       <c r="I5" s="26"/>
       <c r="J5" s="31">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="K5" s="32">
         <f>J5/I2</f>
-        <v>0.97716894977168944</v>
+        <v>0.97797356828193838</v>
       </c>
       <c r="L5" s="31" t="str">
         <f>F1</f>
@@ -1363,11 +1363,11 @@
       <c r="I6" s="26"/>
       <c r="J6" s="34">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="K6" s="35">
         <f>J6/I2</f>
-        <v>0.98630136986301364</v>
+        <v>0.986784140969163</v>
       </c>
       <c r="L6" s="34" t="str">
         <f>G1</f>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="K8" s="50">
         <f>SUM(K2:K7)</f>
-        <v>4.2328767123287676</v>
+        <v>4.2246696035242293</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3419,12 +3419,24 @@
       <c r="A101" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B101" s="26"/>
-      <c r="C101" s="93"/>
-      <c r="D101" s="90"/>
-      <c r="E101" s="94"/>
-      <c r="F101" s="94"/>
-      <c r="G101" s="92"/>
+      <c r="B101" s="26">
+        <v>4</v>
+      </c>
+      <c r="C101" s="54">
+        <v>4</v>
+      </c>
+      <c r="D101" s="79">
+        <v>0</v>
+      </c>
+      <c r="E101" s="23">
+        <v>4</v>
+      </c>
+      <c r="F101" s="23">
+        <v>4</v>
+      </c>
+      <c r="G101" s="24">
+        <v>4</v>
+      </c>
       <c r="H101" s="25"/>
       <c r="I101" s="26"/>
     </row>
@@ -3432,12 +3444,24 @@
       <c r="A102" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B102" s="63"/>
-      <c r="C102" s="116"/>
-      <c r="D102" s="99"/>
-      <c r="E102" s="98"/>
-      <c r="F102" s="98"/>
-      <c r="G102" s="114"/>
+      <c r="B102" s="63">
+        <v>4</v>
+      </c>
+      <c r="C102" s="89">
+        <v>4</v>
+      </c>
+      <c r="D102" s="120">
+        <v>0</v>
+      </c>
+      <c r="E102" s="39">
+        <v>4</v>
+      </c>
+      <c r="F102" s="39">
+        <v>4</v>
+      </c>
+      <c r="G102" s="42">
+        <v>4</v>
+      </c>
       <c r="H102" s="43"/>
       <c r="I102" s="26"/>
     </row>
@@ -3447,11 +3471,11 @@
       </c>
       <c r="B103" s="17">
         <f>B98+B99+B100+B101+B102</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C103" s="46">
         <f t="shared" ref="C103:G103" si="11">SUM(C98:C102)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D103" s="47">
         <f t="shared" si="11"/>
@@ -3459,15 +3483,15 @@
       </c>
       <c r="E103" s="47">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F103" s="47">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G103" s="48">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H103" s="49"/>
       <c r="I103" s="26"/>

</xml_diff>

<commit_message>
Uren Registratie & Small fixes met gun scripts
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -1150,7 +1150,7 @@
   <dimension ref="A1:L175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,15 +1211,15 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J2" s="18">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K2" s="19">
         <f>J2/I2</f>
-        <v>0.81927710843373491</v>
+        <v>0.81781376518218618</v>
       </c>
       <c r="L2" s="18" t="str">
         <f>C1</f>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="K3" s="28">
         <f>J3/I2</f>
-        <v>0.59036144578313254</v>
+        <v>0.59514170040485825</v>
       </c>
       <c r="L3" s="27" t="str">
         <f>D1</f>
@@ -1289,11 +1289,11 @@
       <c r="I4" s="26"/>
       <c r="J4" s="29">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K4" s="30">
         <f>J4/I2</f>
-        <v>0.85140562248995988</v>
+        <v>0.8502024291497976</v>
       </c>
       <c r="L4" s="29" t="str">
         <f>E1</f>
@@ -1326,11 +1326,11 @@
       <c r="I5" s="26"/>
       <c r="J5" s="31">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="K5" s="32">
         <f>J5/I2</f>
-        <v>0.97991967871485941</v>
+        <v>0.97975708502024295</v>
       </c>
       <c r="L5" s="31" t="str">
         <f>F1</f>
@@ -1363,11 +1363,11 @@
       <c r="I6" s="26"/>
       <c r="J6" s="34">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K6" s="35">
         <f>J6/I2</f>
-        <v>0.98795180722891562</v>
+        <v>0.98785425101214575</v>
       </c>
       <c r="L6" s="34" t="str">
         <f>G1</f>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="K8" s="50">
         <f>SUM(K2:K7)</f>
-        <v>4.2289156626506026</v>
+        <v>4.2307692307692308</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3612,22 +3612,22 @@
         <v>1</v>
       </c>
       <c r="B113" s="26">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C113" s="54">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D113" s="79">
         <v>0</v>
       </c>
       <c r="E113" s="23">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F113" s="57">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G113" s="24">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H113" s="25"/>
       <c r="I113" s="26"/>
@@ -3687,22 +3687,22 @@
         <v>4</v>
       </c>
       <c r="B116" s="26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C116" s="22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D116" s="79">
         <v>0</v>
       </c>
       <c r="E116" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F116" s="57">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G116" s="24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H116" s="25"/>
       <c r="I116" s="26"/>
@@ -3711,12 +3711,24 @@
       <c r="A117" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B117" s="63"/>
-      <c r="C117" s="96"/>
-      <c r="D117" s="99"/>
-      <c r="E117" s="97"/>
-      <c r="F117" s="99"/>
-      <c r="G117" s="114"/>
+      <c r="B117" s="63">
+        <v>4</v>
+      </c>
+      <c r="C117" s="38">
+        <v>4</v>
+      </c>
+      <c r="D117" s="120">
+        <v>0</v>
+      </c>
+      <c r="E117" s="65">
+        <v>4</v>
+      </c>
+      <c r="F117" s="41">
+        <v>4</v>
+      </c>
+      <c r="G117" s="42">
+        <v>4</v>
+      </c>
       <c r="H117" s="43"/>
       <c r="I117" s="26"/>
     </row>
@@ -3726,11 +3738,11 @@
       </c>
       <c r="B118" s="17">
         <f>B113+B114+B115+B116+B117</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C118" s="46">
         <f>SUM(C113:C117)</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D118" s="47">
         <f t="shared" ref="D118:G118" si="12">SUM(D113:D117)</f>
@@ -3738,15 +3750,15 @@
       </c>
       <c r="E118" s="47">
         <f t="shared" si="12"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F118" s="47">
         <f t="shared" si="12"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G118" s="48">
         <f t="shared" si="12"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H118" s="49"/>
       <c r="I118" s="26"/>

</xml_diff>

<commit_message>
Crossway en prefabs gemaakt
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -505,7 +505,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -767,9 +767,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -807,18 +804,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -832,9 +820,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -861,6 +846,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1149,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J122" sqref="J122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,15 +1199,15 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>247</v>
+        <v>307</v>
       </c>
       <c r="J2" s="18">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>202</v>
+        <v>262</v>
       </c>
       <c r="K2" s="19">
         <f>J2/I2</f>
-        <v>0.81781376518218618</v>
+        <v>0.85342019543973946</v>
       </c>
       <c r="L2" s="18" t="str">
         <f>C1</f>
@@ -1256,7 +1244,7 @@
       </c>
       <c r="K3" s="28">
         <f>J3/I2</f>
-        <v>0.59514170040485825</v>
+        <v>0.47882736156351791</v>
       </c>
       <c r="L3" s="27" t="str">
         <f>D1</f>
@@ -1289,11 +1277,11 @@
       <c r="I4" s="26"/>
       <c r="J4" s="29">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>210</v>
+        <v>270</v>
       </c>
       <c r="K4" s="30">
         <f>J4/I2</f>
-        <v>0.8502024291497976</v>
+        <v>0.87947882736156346</v>
       </c>
       <c r="L4" s="29" t="str">
         <f>E1</f>
@@ -1326,11 +1314,11 @@
       <c r="I5" s="26"/>
       <c r="J5" s="31">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>242</v>
+        <v>302</v>
       </c>
       <c r="K5" s="32">
         <f>J5/I2</f>
-        <v>0.97975708502024295</v>
+        <v>0.98371335504885993</v>
       </c>
       <c r="L5" s="31" t="str">
         <f>F1</f>
@@ -1363,11 +1351,11 @@
       <c r="I6" s="26"/>
       <c r="J6" s="34">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>244</v>
+        <v>304</v>
       </c>
       <c r="K6" s="35">
         <f>J6/I2</f>
-        <v>0.98785425101214575</v>
+        <v>0.99022801302931596</v>
       </c>
       <c r="L6" s="34" t="str">
         <f>G1</f>
@@ -1435,7 +1423,7 @@
       </c>
       <c r="K8" s="50">
         <f>SUM(K2:K7)</f>
-        <v>4.2307692307692308</v>
+        <v>4.1856677524429973</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2558,7 +2546,7 @@
       <c r="C62" s="67">
         <v>0</v>
       </c>
-      <c r="D62" s="120">
+      <c r="D62" s="116">
         <v>0</v>
       </c>
       <c r="E62" s="64">
@@ -2625,17 +2613,17 @@
       <c r="E65" s="52"/>
       <c r="F65" s="52"/>
       <c r="G65" s="66"/>
-      <c r="H65" s="101"/>
+      <c r="H65" s="100"/>
       <c r="I65" s="26"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="102">
-        <v>0</v>
-      </c>
-      <c r="C66" s="125">
+      <c r="B66" s="101">
+        <v>0</v>
+      </c>
+      <c r="C66" s="120">
         <v>0</v>
       </c>
       <c r="D66" s="78">
@@ -2647,20 +2635,20 @@
       <c r="F66" s="78">
         <v>0</v>
       </c>
-      <c r="G66" s="126">
-        <v>0</v>
-      </c>
-      <c r="H66" s="106"/>
+      <c r="G66" s="121">
+        <v>0</v>
+      </c>
+      <c r="H66" s="105"/>
       <c r="I66" s="26"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="102">
-        <v>0</v>
-      </c>
-      <c r="C67" s="125">
+      <c r="B67" s="101">
+        <v>0</v>
+      </c>
+      <c r="C67" s="120">
         <v>0</v>
       </c>
       <c r="D67" s="78">
@@ -2672,20 +2660,20 @@
       <c r="F67" s="78">
         <v>0</v>
       </c>
-      <c r="G67" s="126">
-        <v>0</v>
-      </c>
-      <c r="H67" s="106"/>
+      <c r="G67" s="121">
+        <v>0</v>
+      </c>
+      <c r="H67" s="105"/>
       <c r="I67" s="26"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="102">
-        <v>0</v>
-      </c>
-      <c r="C68" s="125">
+      <c r="B68" s="101">
+        <v>0</v>
+      </c>
+      <c r="C68" s="120">
         <v>0</v>
       </c>
       <c r="D68" s="78">
@@ -2697,64 +2685,64 @@
       <c r="F68" s="78">
         <v>0</v>
       </c>
-      <c r="G68" s="126">
-        <v>0</v>
-      </c>
-      <c r="H68" s="106"/>
+      <c r="G68" s="121">
+        <v>0</v>
+      </c>
+      <c r="H68" s="105"/>
       <c r="I68" s="26"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="102">
-        <v>2</v>
-      </c>
-      <c r="C69" s="125">
-        <v>0</v>
-      </c>
-      <c r="D69" s="127">
-        <v>2</v>
-      </c>
-      <c r="E69" s="127">
-        <v>2</v>
-      </c>
-      <c r="F69" s="127">
-        <v>2</v>
-      </c>
-      <c r="G69" s="128">
-        <v>2</v>
-      </c>
-      <c r="H69" s="106"/>
+      <c r="B69" s="101">
+        <v>2</v>
+      </c>
+      <c r="C69" s="120">
+        <v>0</v>
+      </c>
+      <c r="D69" s="122">
+        <v>2</v>
+      </c>
+      <c r="E69" s="122">
+        <v>2</v>
+      </c>
+      <c r="F69" s="122">
+        <v>2</v>
+      </c>
+      <c r="G69" s="123">
+        <v>2</v>
+      </c>
+      <c r="H69" s="105"/>
       <c r="I69" s="26"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B70" s="107">
-        <v>8</v>
-      </c>
-      <c r="C70" s="131">
-        <v>4</v>
-      </c>
-      <c r="D70" s="129">
-        <v>8</v>
-      </c>
-      <c r="E70" s="129">
-        <v>8</v>
-      </c>
-      <c r="F70" s="129">
-        <v>8</v>
-      </c>
-      <c r="G70" s="130">
-        <v>8</v>
-      </c>
-      <c r="H70" s="111"/>
+      <c r="B70" s="106">
+        <v>8</v>
+      </c>
+      <c r="C70" s="126">
+        <v>4</v>
+      </c>
+      <c r="D70" s="124">
+        <v>8</v>
+      </c>
+      <c r="E70" s="124">
+        <v>8</v>
+      </c>
+      <c r="F70" s="124">
+        <v>8</v>
+      </c>
+      <c r="G70" s="125">
+        <v>8</v>
+      </c>
+      <c r="H70" s="110"/>
       <c r="I70" s="26"/>
     </row>
     <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="112" t="s">
+      <c r="A71" s="111" t="s">
         <v>6</v>
       </c>
       <c r="B71" s="17">
@@ -3094,7 +3082,7 @@
       <c r="C86" s="38">
         <v>4</v>
       </c>
-      <c r="D86" s="120">
+      <c r="D86" s="116">
         <v>0</v>
       </c>
       <c r="E86" s="39">
@@ -3256,7 +3244,7 @@
       <c r="F93" s="57">
         <v>2</v>
       </c>
-      <c r="G93" s="132">
+      <c r="G93" s="127">
         <v>2</v>
       </c>
       <c r="H93" s="25"/>
@@ -3272,7 +3260,7 @@
       <c r="C94" s="38">
         <v>4</v>
       </c>
-      <c r="D94" s="120">
+      <c r="D94" s="116">
         <v>0</v>
       </c>
       <c r="E94" s="65">
@@ -3450,7 +3438,7 @@
       <c r="C102" s="89">
         <v>4</v>
       </c>
-      <c r="D102" s="120">
+      <c r="D102" s="116">
         <v>0</v>
       </c>
       <c r="E102" s="39">
@@ -3507,7 +3495,7 @@
       <c r="A105" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="B105" s="117" t="s">
+      <c r="B105" s="113" t="s">
         <v>51</v>
       </c>
       <c r="C105" s="74"/>
@@ -3555,7 +3543,7 @@
         <v>46</v>
       </c>
       <c r="F108" s="55"/>
-      <c r="G108" s="118"/>
+      <c r="G108" s="114"/>
       <c r="H108" s="77"/>
       <c r="I108" s="26"/>
     </row>
@@ -3576,12 +3564,12 @@
       <c r="A110" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B110" s="119"/>
+      <c r="B110" s="115"/>
       <c r="C110" s="67"/>
-      <c r="D110" s="120"/>
+      <c r="D110" s="116"/>
       <c r="E110" s="64"/>
-      <c r="F110" s="120"/>
-      <c r="G110" s="121"/>
+      <c r="F110" s="116"/>
+      <c r="G110" s="117"/>
       <c r="H110" s="82"/>
       <c r="I110" s="26"/>
     </row>
@@ -3717,7 +3705,7 @@
       <c r="C117" s="38">
         <v>4</v>
       </c>
-      <c r="D117" s="120">
+      <c r="D117" s="116">
         <v>0</v>
       </c>
       <c r="E117" s="65">
@@ -3789,12 +3777,24 @@
       <c r="A121" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B121" s="26"/>
-      <c r="C121" s="93"/>
-      <c r="D121" s="90"/>
-      <c r="E121" s="94"/>
-      <c r="F121" s="94"/>
-      <c r="G121" s="92"/>
+      <c r="B121" s="26">
+        <v>4</v>
+      </c>
+      <c r="C121" s="54">
+        <v>4</v>
+      </c>
+      <c r="D121" s="79">
+        <v>0</v>
+      </c>
+      <c r="E121" s="23">
+        <v>4</v>
+      </c>
+      <c r="F121" s="23">
+        <v>4</v>
+      </c>
+      <c r="G121" s="24">
+        <v>4</v>
+      </c>
       <c r="H121" s="25"/>
       <c r="I121" s="26"/>
     </row>
@@ -3802,12 +3802,24 @@
       <c r="A122" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B122" s="26"/>
-      <c r="C122" s="93"/>
-      <c r="D122" s="90"/>
-      <c r="E122" s="94"/>
-      <c r="F122" s="91"/>
-      <c r="G122" s="92"/>
+      <c r="B122" s="26">
+        <v>4</v>
+      </c>
+      <c r="C122" s="54">
+        <v>4</v>
+      </c>
+      <c r="D122" s="79">
+        <v>0</v>
+      </c>
+      <c r="E122" s="23">
+        <v>4</v>
+      </c>
+      <c r="F122" s="60">
+        <v>4</v>
+      </c>
+      <c r="G122" s="24">
+        <v>4</v>
+      </c>
       <c r="H122" s="25"/>
       <c r="I122" s="26"/>
     </row>
@@ -3815,12 +3827,24 @@
       <c r="A123" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B123" s="26"/>
-      <c r="C123" s="93"/>
-      <c r="D123" s="90"/>
-      <c r="E123" s="94"/>
-      <c r="F123" s="94"/>
-      <c r="G123" s="92"/>
+      <c r="B123" s="26">
+        <v>6</v>
+      </c>
+      <c r="C123" s="54">
+        <v>6</v>
+      </c>
+      <c r="D123" s="79">
+        <v>0</v>
+      </c>
+      <c r="E123" s="23">
+        <v>6</v>
+      </c>
+      <c r="F123" s="23">
+        <v>6</v>
+      </c>
+      <c r="G123" s="24">
+        <v>6</v>
+      </c>
       <c r="H123" s="25"/>
       <c r="I123" s="26"/>
     </row>
@@ -3828,12 +3852,24 @@
       <c r="A124" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B124" s="26"/>
-      <c r="C124" s="93"/>
-      <c r="D124" s="94"/>
-      <c r="E124" s="94"/>
-      <c r="F124" s="94"/>
-      <c r="G124" s="115"/>
+      <c r="B124" s="26">
+        <v>2</v>
+      </c>
+      <c r="C124" s="54">
+        <v>2</v>
+      </c>
+      <c r="D124" s="55">
+        <v>0</v>
+      </c>
+      <c r="E124" s="23">
+        <v>2</v>
+      </c>
+      <c r="F124" s="23">
+        <v>2</v>
+      </c>
+      <c r="G124" s="127">
+        <v>2</v>
+      </c>
       <c r="H124" s="25"/>
       <c r="I124" s="26"/>
     </row>
@@ -3841,12 +3877,24 @@
       <c r="A125" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B125" s="63"/>
-      <c r="C125" s="116"/>
-      <c r="D125" s="99"/>
-      <c r="E125" s="98"/>
-      <c r="F125" s="99"/>
-      <c r="G125" s="122"/>
+      <c r="B125" s="63">
+        <v>4</v>
+      </c>
+      <c r="C125" s="89">
+        <v>4</v>
+      </c>
+      <c r="D125" s="116">
+        <v>0</v>
+      </c>
+      <c r="E125" s="39">
+        <v>4</v>
+      </c>
+      <c r="F125" s="41">
+        <v>4</v>
+      </c>
+      <c r="G125" s="128">
+        <v>4</v>
+      </c>
       <c r="H125" s="43"/>
       <c r="I125" s="26"/>
     </row>
@@ -3855,11 +3903,12 @@
         <v>6</v>
       </c>
       <c r="B126" s="17">
-        <v>0</v>
+        <f>B121+B122+B123+B124+B125</f>
+        <v>20</v>
       </c>
       <c r="C126" s="46">
         <f t="shared" ref="C126:G126" si="13">SUM(C121:C125)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D126" s="47">
         <f t="shared" si="13"/>
@@ -3867,15 +3916,15 @@
       </c>
       <c r="E126" s="47">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F126" s="47">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G126" s="48">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H126" s="49"/>
       <c r="I126" s="26"/>
@@ -3906,12 +3955,24 @@
       <c r="A129" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B129" s="26"/>
-      <c r="C129" s="95"/>
-      <c r="D129" s="90"/>
-      <c r="E129" s="91"/>
-      <c r="F129" s="94"/>
-      <c r="G129" s="113"/>
+      <c r="B129" s="26">
+        <v>4</v>
+      </c>
+      <c r="C129" s="54">
+        <v>4</v>
+      </c>
+      <c r="D129" s="79">
+        <v>0</v>
+      </c>
+      <c r="E129" s="23">
+        <v>4</v>
+      </c>
+      <c r="F129" s="23">
+        <v>4</v>
+      </c>
+      <c r="G129" s="24">
+        <v>4</v>
+      </c>
       <c r="H129" s="25"/>
       <c r="I129" s="26"/>
     </row>
@@ -3919,12 +3980,24 @@
       <c r="A130" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B130" s="26"/>
-      <c r="C130" s="93"/>
-      <c r="D130" s="91"/>
-      <c r="E130" s="94"/>
-      <c r="F130" s="94"/>
-      <c r="G130" s="113"/>
+      <c r="B130" s="26">
+        <v>4</v>
+      </c>
+      <c r="C130" s="54">
+        <v>4</v>
+      </c>
+      <c r="D130" s="79">
+        <v>0</v>
+      </c>
+      <c r="E130" s="23">
+        <v>4</v>
+      </c>
+      <c r="F130" s="60">
+        <v>4</v>
+      </c>
+      <c r="G130" s="24">
+        <v>4</v>
+      </c>
       <c r="H130" s="25"/>
       <c r="I130" s="26"/>
     </row>
@@ -3932,12 +4005,24 @@
       <c r="A131" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B131" s="26"/>
-      <c r="C131" s="93"/>
-      <c r="D131" s="90"/>
-      <c r="E131" s="94"/>
-      <c r="F131" s="94"/>
-      <c r="G131" s="92"/>
+      <c r="B131" s="26">
+        <v>6</v>
+      </c>
+      <c r="C131" s="54">
+        <v>6</v>
+      </c>
+      <c r="D131" s="79">
+        <v>0</v>
+      </c>
+      <c r="E131" s="23">
+        <v>6</v>
+      </c>
+      <c r="F131" s="23">
+        <v>6</v>
+      </c>
+      <c r="G131" s="24">
+        <v>6</v>
+      </c>
       <c r="H131" s="25"/>
       <c r="I131" s="26"/>
     </row>
@@ -3945,12 +4030,24 @@
       <c r="A132" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B132" s="26"/>
-      <c r="C132" s="93"/>
-      <c r="D132" s="94"/>
-      <c r="E132" s="94"/>
-      <c r="F132" s="94"/>
-      <c r="G132" s="92"/>
+      <c r="B132" s="26">
+        <v>2</v>
+      </c>
+      <c r="C132" s="54">
+        <v>2</v>
+      </c>
+      <c r="D132" s="55">
+        <v>0</v>
+      </c>
+      <c r="E132" s="23">
+        <v>2</v>
+      </c>
+      <c r="F132" s="23">
+        <v>2</v>
+      </c>
+      <c r="G132" s="127">
+        <v>2</v>
+      </c>
       <c r="H132" s="25"/>
       <c r="I132" s="26"/>
     </row>
@@ -3958,12 +4055,24 @@
       <c r="A133" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B133" s="63"/>
-      <c r="C133" s="96"/>
-      <c r="D133" s="99"/>
-      <c r="E133" s="97"/>
-      <c r="F133" s="99"/>
-      <c r="G133" s="114"/>
+      <c r="B133" s="63">
+        <v>4</v>
+      </c>
+      <c r="C133" s="89">
+        <v>4</v>
+      </c>
+      <c r="D133" s="116">
+        <v>0</v>
+      </c>
+      <c r="E133" s="39">
+        <v>4</v>
+      </c>
+      <c r="F133" s="41">
+        <v>4</v>
+      </c>
+      <c r="G133" s="128">
+        <v>4</v>
+      </c>
       <c r="H133" s="43"/>
       <c r="I133" s="26"/>
     </row>
@@ -3972,11 +4081,12 @@
         <v>6</v>
       </c>
       <c r="B134" s="17">
-        <v>0</v>
+        <f>B129+B130+B131+B132+B133</f>
+        <v>20</v>
       </c>
       <c r="C134" s="46">
         <f t="shared" ref="C134:G134" si="14">SUM(C129:C133)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D134" s="47">
         <f t="shared" si="14"/>
@@ -3984,15 +4094,15 @@
       </c>
       <c r="E134" s="47">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F134" s="47">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G134" s="48">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H134" s="49"/>
       <c r="I134" s="26"/>
@@ -4016,72 +4126,132 @@
       <c r="E136" s="52"/>
       <c r="F136" s="52"/>
       <c r="G136" s="66"/>
-      <c r="H136" s="101"/>
+      <c r="H136" s="100"/>
       <c r="I136" s="26"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B137" s="103"/>
-      <c r="C137" s="103"/>
-      <c r="D137" s="104"/>
-      <c r="E137" s="104"/>
-      <c r="F137" s="104"/>
-      <c r="G137" s="105"/>
-      <c r="H137" s="106"/>
+      <c r="B137" s="26">
+        <v>4</v>
+      </c>
+      <c r="C137" s="54">
+        <v>4</v>
+      </c>
+      <c r="D137" s="79">
+        <v>0</v>
+      </c>
+      <c r="E137" s="23">
+        <v>4</v>
+      </c>
+      <c r="F137" s="23">
+        <v>4</v>
+      </c>
+      <c r="G137" s="24">
+        <v>4</v>
+      </c>
+      <c r="H137" s="105"/>
       <c r="I137" s="26"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B138" s="103"/>
-      <c r="C138" s="103"/>
-      <c r="D138" s="104"/>
-      <c r="E138" s="104"/>
-      <c r="F138" s="104"/>
-      <c r="G138" s="105"/>
-      <c r="H138" s="106"/>
+      <c r="B138" s="26">
+        <v>4</v>
+      </c>
+      <c r="C138" s="54">
+        <v>4</v>
+      </c>
+      <c r="D138" s="79">
+        <v>0</v>
+      </c>
+      <c r="E138" s="23">
+        <v>4</v>
+      </c>
+      <c r="F138" s="60">
+        <v>4</v>
+      </c>
+      <c r="G138" s="24">
+        <v>4</v>
+      </c>
+      <c r="H138" s="105"/>
       <c r="I138" s="26"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B139" s="103"/>
-      <c r="C139" s="103"/>
-      <c r="D139" s="104"/>
-      <c r="E139" s="104"/>
-      <c r="F139" s="104"/>
-      <c r="G139" s="105"/>
-      <c r="H139" s="106"/>
+      <c r="B139" s="26">
+        <v>6</v>
+      </c>
+      <c r="C139" s="54">
+        <v>6</v>
+      </c>
+      <c r="D139" s="79">
+        <v>0</v>
+      </c>
+      <c r="E139" s="23">
+        <v>6</v>
+      </c>
+      <c r="F139" s="23">
+        <v>6</v>
+      </c>
+      <c r="G139" s="24">
+        <v>6</v>
+      </c>
+      <c r="H139" s="105"/>
       <c r="I139" s="26"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B140" s="103"/>
-      <c r="C140" s="103"/>
-      <c r="D140" s="104"/>
-      <c r="E140" s="104"/>
-      <c r="F140" s="104"/>
-      <c r="G140" s="105"/>
-      <c r="H140" s="106"/>
+      <c r="B140" s="26">
+        <v>2</v>
+      </c>
+      <c r="C140" s="54">
+        <v>2</v>
+      </c>
+      <c r="D140" s="55">
+        <v>0</v>
+      </c>
+      <c r="E140" s="23">
+        <v>2</v>
+      </c>
+      <c r="F140" s="23">
+        <v>2</v>
+      </c>
+      <c r="G140" s="127">
+        <v>2</v>
+      </c>
+      <c r="H140" s="105"/>
       <c r="I140" s="26"/>
     </row>
     <row r="141" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B141" s="108"/>
-      <c r="C141" s="108"/>
-      <c r="D141" s="109"/>
-      <c r="E141" s="109"/>
-      <c r="F141" s="109"/>
-      <c r="G141" s="110"/>
-      <c r="H141" s="111"/>
+      <c r="B141" s="63">
+        <v>4</v>
+      </c>
+      <c r="C141" s="89">
+        <v>4</v>
+      </c>
+      <c r="D141" s="116">
+        <v>0</v>
+      </c>
+      <c r="E141" s="39">
+        <v>4</v>
+      </c>
+      <c r="F141" s="41">
+        <v>4</v>
+      </c>
+      <c r="G141" s="128">
+        <v>4</v>
+      </c>
+      <c r="H141" s="110"/>
       <c r="I141" s="26"/>
     </row>
     <row r="142" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4089,11 +4259,12 @@
         <v>6</v>
       </c>
       <c r="B142" s="17">
-        <v>0</v>
+        <f>B137+B138+B139+B140+B141</f>
+        <v>20</v>
       </c>
       <c r="C142" s="46">
         <f t="shared" ref="C142:G142" si="15">SUM(C137:C141)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D142" s="47">
         <f t="shared" si="15"/>
@@ -4101,17 +4272,17 @@
       </c>
       <c r="E142" s="47">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F142" s="47">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G142" s="48">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="H142" s="123"/>
+        <v>20</v>
+      </c>
+      <c r="H142" s="118"/>
       <c r="I142" s="26"/>
     </row>
     <row r="143" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4121,7 +4292,7 @@
       <c r="E143" s="45"/>
       <c r="F143" s="45"/>
       <c r="G143" s="45"/>
-      <c r="H143" s="124"/>
+      <c r="H143" s="119"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
@@ -4135,72 +4306,72 @@
       <c r="E144" s="52"/>
       <c r="F144" s="52"/>
       <c r="G144" s="66"/>
-      <c r="H144" s="101"/>
+      <c r="H144" s="100"/>
       <c r="I144" s="26"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B145" s="103"/>
-      <c r="C145" s="103"/>
-      <c r="D145" s="104"/>
-      <c r="E145" s="104"/>
-      <c r="F145" s="104"/>
-      <c r="G145" s="105"/>
-      <c r="H145" s="106"/>
+      <c r="B145" s="102"/>
+      <c r="C145" s="102"/>
+      <c r="D145" s="103"/>
+      <c r="E145" s="103"/>
+      <c r="F145" s="103"/>
+      <c r="G145" s="104"/>
+      <c r="H145" s="105"/>
       <c r="I145" s="26"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B146" s="103"/>
-      <c r="C146" s="103"/>
-      <c r="D146" s="104"/>
-      <c r="E146" s="104"/>
-      <c r="F146" s="104"/>
-      <c r="G146" s="105"/>
-      <c r="H146" s="106"/>
+      <c r="B146" s="102"/>
+      <c r="C146" s="102"/>
+      <c r="D146" s="103"/>
+      <c r="E146" s="103"/>
+      <c r="F146" s="103"/>
+      <c r="G146" s="104"/>
+      <c r="H146" s="105"/>
       <c r="I146" s="26"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B147" s="103"/>
-      <c r="C147" s="103"/>
-      <c r="D147" s="104"/>
-      <c r="E147" s="104"/>
-      <c r="F147" s="104"/>
-      <c r="G147" s="105"/>
-      <c r="H147" s="106"/>
+      <c r="B147" s="102"/>
+      <c r="C147" s="102"/>
+      <c r="D147" s="103"/>
+      <c r="E147" s="103"/>
+      <c r="F147" s="103"/>
+      <c r="G147" s="104"/>
+      <c r="H147" s="105"/>
       <c r="I147" s="26"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B148" s="103"/>
-      <c r="C148" s="103"/>
-      <c r="D148" s="104"/>
-      <c r="E148" s="104"/>
-      <c r="F148" s="104"/>
-      <c r="G148" s="105"/>
-      <c r="H148" s="106"/>
+      <c r="B148" s="102"/>
+      <c r="C148" s="102"/>
+      <c r="D148" s="103"/>
+      <c r="E148" s="103"/>
+      <c r="F148" s="103"/>
+      <c r="G148" s="104"/>
+      <c r="H148" s="105"/>
       <c r="I148" s="26"/>
     </row>
     <row r="149" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B149" s="108"/>
-      <c r="C149" s="108"/>
-      <c r="D149" s="109"/>
-      <c r="E149" s="109"/>
-      <c r="F149" s="109"/>
-      <c r="G149" s="110"/>
-      <c r="H149" s="111"/>
+      <c r="B149" s="107"/>
+      <c r="C149" s="107"/>
+      <c r="D149" s="108"/>
+      <c r="E149" s="108"/>
+      <c r="F149" s="108"/>
+      <c r="G149" s="109"/>
+      <c r="H149" s="110"/>
       <c r="I149" s="26"/>
     </row>
     <row r="150" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4313,10 +4484,10 @@
       </c>
       <c r="B157" s="63"/>
       <c r="C157" s="96"/>
-      <c r="D157" s="99"/>
-      <c r="E157" s="98"/>
-      <c r="F157" s="98"/>
-      <c r="G157" s="100"/>
+      <c r="D157" s="98"/>
+      <c r="E157" s="97"/>
+      <c r="F157" s="97"/>
+      <c r="G157" s="99"/>
       <c r="H157" s="43"/>
       <c r="I157" s="26"/>
     </row>
@@ -4430,10 +4601,10 @@
       </c>
       <c r="B165" s="63"/>
       <c r="C165" s="96"/>
-      <c r="D165" s="98"/>
-      <c r="E165" s="98"/>
-      <c r="F165" s="98"/>
-      <c r="G165" s="100"/>
+      <c r="D165" s="97"/>
+      <c r="E165" s="97"/>
+      <c r="F165" s="97"/>
+      <c r="G165" s="99"/>
       <c r="H165" s="43"/>
       <c r="I165" s="26"/>
     </row>
@@ -4547,10 +4718,10 @@
       </c>
       <c r="B173" s="63"/>
       <c r="C173" s="96"/>
-      <c r="D173" s="99"/>
-      <c r="E173" s="98"/>
-      <c r="F173" s="99"/>
-      <c r="G173" s="114"/>
+      <c r="D173" s="98"/>
+      <c r="E173" s="97"/>
+      <c r="F173" s="98"/>
+      <c r="G173" s="112"/>
       <c r="H173" s="43"/>
       <c r="I173" s="26"/>
     </row>

</xml_diff>

<commit_message>
Presentatie & uren reg
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie/Uren Registratie Game-Lab-2.1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -505,7 +505,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -746,67 +746,16 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -948,6 +897,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -983,6 +949,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -1137,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J122" sqref="J122"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,15 +1182,15 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>307</v>
+        <v>387</v>
       </c>
       <c r="J2" s="18">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>262</v>
+        <v>350</v>
       </c>
       <c r="K2" s="19">
         <f>J2/I2</f>
-        <v>0.85342019543973946</v>
+        <v>0.90439276485788112</v>
       </c>
       <c r="L2" s="18" t="str">
         <f>C1</f>
@@ -1240,11 +1223,11 @@
       <c r="I3" s="26"/>
       <c r="J3" s="27">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="K3" s="28">
         <f>J3/I2</f>
-        <v>0.47882736156351791</v>
+        <v>0.4005167958656331</v>
       </c>
       <c r="L3" s="27" t="str">
         <f>D1</f>
@@ -1277,11 +1260,11 @@
       <c r="I4" s="26"/>
       <c r="J4" s="29">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>270</v>
+        <v>350</v>
       </c>
       <c r="K4" s="30">
         <f>J4/I2</f>
-        <v>0.87947882736156346</v>
+        <v>0.90439276485788112</v>
       </c>
       <c r="L4" s="29" t="str">
         <f>E1</f>
@@ -1314,11 +1297,11 @@
       <c r="I5" s="26"/>
       <c r="J5" s="31">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>302</v>
+        <v>382</v>
       </c>
       <c r="K5" s="32">
         <f>J5/I2</f>
-        <v>0.98371335504885993</v>
+        <v>0.98708010335917318</v>
       </c>
       <c r="L5" s="31" t="str">
         <f>F1</f>
@@ -1351,11 +1334,11 @@
       <c r="I6" s="26"/>
       <c r="J6" s="34">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>304</v>
+        <v>384</v>
       </c>
       <c r="K6" s="35">
         <f>J6/I2</f>
-        <v>0.99022801302931596</v>
+        <v>0.99224806201550386</v>
       </c>
       <c r="L6" s="34" t="str">
         <f>G1</f>
@@ -1423,7 +1406,7 @@
       </c>
       <c r="K8" s="50">
         <f>SUM(K2:K7)</f>
-        <v>4.1856677524429973</v>
+        <v>4.1886304909560721</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2546,7 +2529,7 @@
       <c r="C62" s="67">
         <v>0</v>
       </c>
-      <c r="D62" s="116">
+      <c r="D62" s="99">
         <v>0</v>
       </c>
       <c r="E62" s="64">
@@ -2613,17 +2596,17 @@
       <c r="E65" s="52"/>
       <c r="F65" s="52"/>
       <c r="G65" s="66"/>
-      <c r="H65" s="100"/>
+      <c r="H65" s="90"/>
       <c r="I65" s="26"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="101">
-        <v>0</v>
-      </c>
-      <c r="C66" s="120">
+      <c r="B66" s="91">
+        <v>0</v>
+      </c>
+      <c r="C66" s="103">
         <v>0</v>
       </c>
       <c r="D66" s="78">
@@ -2635,20 +2618,20 @@
       <c r="F66" s="78">
         <v>0</v>
       </c>
-      <c r="G66" s="121">
-        <v>0</v>
-      </c>
-      <c r="H66" s="105"/>
+      <c r="G66" s="104">
+        <v>0</v>
+      </c>
+      <c r="H66" s="92"/>
       <c r="I66" s="26"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="101">
-        <v>0</v>
-      </c>
-      <c r="C67" s="120">
+      <c r="B67" s="91">
+        <v>0</v>
+      </c>
+      <c r="C67" s="103">
         <v>0</v>
       </c>
       <c r="D67" s="78">
@@ -2660,20 +2643,20 @@
       <c r="F67" s="78">
         <v>0</v>
       </c>
-      <c r="G67" s="121">
-        <v>0</v>
-      </c>
-      <c r="H67" s="105"/>
+      <c r="G67" s="104">
+        <v>0</v>
+      </c>
+      <c r="H67" s="92"/>
       <c r="I67" s="26"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="101">
-        <v>0</v>
-      </c>
-      <c r="C68" s="120">
+      <c r="B68" s="91">
+        <v>0</v>
+      </c>
+      <c r="C68" s="103">
         <v>0</v>
       </c>
       <c r="D68" s="78">
@@ -2685,64 +2668,64 @@
       <c r="F68" s="78">
         <v>0</v>
       </c>
-      <c r="G68" s="121">
-        <v>0</v>
-      </c>
-      <c r="H68" s="105"/>
+      <c r="G68" s="104">
+        <v>0</v>
+      </c>
+      <c r="H68" s="92"/>
       <c r="I68" s="26"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="101">
-        <v>2</v>
-      </c>
-      <c r="C69" s="120">
-        <v>0</v>
-      </c>
-      <c r="D69" s="122">
-        <v>2</v>
-      </c>
-      <c r="E69" s="122">
-        <v>2</v>
-      </c>
-      <c r="F69" s="122">
-        <v>2</v>
-      </c>
-      <c r="G69" s="123">
-        <v>2</v>
-      </c>
-      <c r="H69" s="105"/>
+      <c r="B69" s="91">
+        <v>2</v>
+      </c>
+      <c r="C69" s="103">
+        <v>0</v>
+      </c>
+      <c r="D69" s="105">
+        <v>2</v>
+      </c>
+      <c r="E69" s="105">
+        <v>2</v>
+      </c>
+      <c r="F69" s="105">
+        <v>2</v>
+      </c>
+      <c r="G69" s="106">
+        <v>2</v>
+      </c>
+      <c r="H69" s="92"/>
       <c r="I69" s="26"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B70" s="106">
+      <c r="B70" s="93">
         <v>8</v>
       </c>
-      <c r="C70" s="126">
-        <v>4</v>
-      </c>
-      <c r="D70" s="124">
+      <c r="C70" s="109">
+        <v>4</v>
+      </c>
+      <c r="D70" s="107">
         <v>8</v>
       </c>
-      <c r="E70" s="124">
+      <c r="E70" s="107">
         <v>8</v>
       </c>
-      <c r="F70" s="124">
+      <c r="F70" s="107">
         <v>8</v>
       </c>
-      <c r="G70" s="125">
+      <c r="G70" s="108">
         <v>8</v>
       </c>
-      <c r="H70" s="110"/>
+      <c r="H70" s="94"/>
       <c r="I70" s="26"/>
     </row>
     <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="111" t="s">
+      <c r="A71" s="95" t="s">
         <v>6</v>
       </c>
       <c r="B71" s="17">
@@ -2979,8 +2962,8 @@
       <c r="B82" s="26">
         <v>4</v>
       </c>
-      <c r="C82" s="87">
-        <v>0</v>
+      <c r="C82" s="54">
+        <v>4</v>
       </c>
       <c r="D82" s="57">
         <v>2</v>
@@ -3082,7 +3065,7 @@
       <c r="C86" s="38">
         <v>4</v>
       </c>
-      <c r="D86" s="116">
+      <c r="D86" s="99">
         <v>0</v>
       </c>
       <c r="E86" s="39">
@@ -3107,7 +3090,7 @@
       </c>
       <c r="C87" s="46">
         <f t="shared" ref="C87:G87" si="9">SUM(C82:C86)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D87" s="47">
         <f t="shared" si="9"/>
@@ -3157,8 +3140,8 @@
       <c r="B90" s="26">
         <v>4</v>
       </c>
-      <c r="C90" s="87">
-        <v>0</v>
+      <c r="C90" s="54">
+        <v>4</v>
       </c>
       <c r="D90" s="79">
         <v>0</v>
@@ -3244,7 +3227,7 @@
       <c r="F93" s="57">
         <v>2</v>
       </c>
-      <c r="G93" s="127">
+      <c r="G93" s="110">
         <v>2</v>
       </c>
       <c r="H93" s="25"/>
@@ -3260,7 +3243,7 @@
       <c r="C94" s="38">
         <v>4</v>
       </c>
-      <c r="D94" s="116">
+      <c r="D94" s="99">
         <v>0</v>
       </c>
       <c r="E94" s="65">
@@ -3285,7 +3268,7 @@
       </c>
       <c r="C95" s="46">
         <f t="shared" ref="C95:G95" si="10">SUM(C90:C94)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D95" s="47">
         <f t="shared" si="10"/>
@@ -3438,7 +3421,7 @@
       <c r="C102" s="89">
         <v>4</v>
       </c>
-      <c r="D102" s="116">
+      <c r="D102" s="99">
         <v>0</v>
       </c>
       <c r="E102" s="39">
@@ -3495,7 +3478,7 @@
       <c r="A105" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="B105" s="113" t="s">
+      <c r="B105" s="96" t="s">
         <v>51</v>
       </c>
       <c r="C105" s="74"/>
@@ -3543,7 +3526,7 @@
         <v>46</v>
       </c>
       <c r="F108" s="55"/>
-      <c r="G108" s="114"/>
+      <c r="G108" s="97"/>
       <c r="H108" s="77"/>
       <c r="I108" s="26"/>
     </row>
@@ -3564,12 +3547,12 @@
       <c r="A110" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B110" s="115"/>
+      <c r="B110" s="98"/>
       <c r="C110" s="67"/>
-      <c r="D110" s="116"/>
+      <c r="D110" s="99"/>
       <c r="E110" s="64"/>
-      <c r="F110" s="116"/>
-      <c r="G110" s="117"/>
+      <c r="F110" s="99"/>
+      <c r="G110" s="100"/>
       <c r="H110" s="82"/>
       <c r="I110" s="26"/>
     </row>
@@ -3705,7 +3688,7 @@
       <c r="C117" s="38">
         <v>4</v>
       </c>
-      <c r="D117" s="116">
+      <c r="D117" s="99">
         <v>0</v>
       </c>
       <c r="E117" s="65">
@@ -3867,7 +3850,7 @@
       <c r="F124" s="23">
         <v>2</v>
       </c>
-      <c r="G124" s="127">
+      <c r="G124" s="110">
         <v>2</v>
       </c>
       <c r="H124" s="25"/>
@@ -3883,7 +3866,7 @@
       <c r="C125" s="89">
         <v>4</v>
       </c>
-      <c r="D125" s="116">
+      <c r="D125" s="99">
         <v>0</v>
       </c>
       <c r="E125" s="39">
@@ -3892,7 +3875,7 @@
       <c r="F125" s="41">
         <v>4</v>
       </c>
-      <c r="G125" s="128">
+      <c r="G125" s="111">
         <v>4</v>
       </c>
       <c r="H125" s="43"/>
@@ -4045,7 +4028,7 @@
       <c r="F132" s="23">
         <v>2</v>
       </c>
-      <c r="G132" s="127">
+      <c r="G132" s="110">
         <v>2</v>
       </c>
       <c r="H132" s="25"/>
@@ -4061,7 +4044,7 @@
       <c r="C133" s="89">
         <v>4</v>
       </c>
-      <c r="D133" s="116">
+      <c r="D133" s="99">
         <v>0</v>
       </c>
       <c r="E133" s="39">
@@ -4070,7 +4053,7 @@
       <c r="F133" s="41">
         <v>4</v>
       </c>
-      <c r="G133" s="128">
+      <c r="G133" s="111">
         <v>4</v>
       </c>
       <c r="H133" s="43"/>
@@ -4126,7 +4109,7 @@
       <c r="E136" s="52"/>
       <c r="F136" s="52"/>
       <c r="G136" s="66"/>
-      <c r="H136" s="100"/>
+      <c r="H136" s="90"/>
       <c r="I136" s="26"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -4151,7 +4134,7 @@
       <c r="G137" s="24">
         <v>4</v>
       </c>
-      <c r="H137" s="105"/>
+      <c r="H137" s="92"/>
       <c r="I137" s="26"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -4176,7 +4159,7 @@
       <c r="G138" s="24">
         <v>4</v>
       </c>
-      <c r="H138" s="105"/>
+      <c r="H138" s="92"/>
       <c r="I138" s="26"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -4201,7 +4184,7 @@
       <c r="G139" s="24">
         <v>6</v>
       </c>
-      <c r="H139" s="105"/>
+      <c r="H139" s="92"/>
       <c r="I139" s="26"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -4223,10 +4206,10 @@
       <c r="F140" s="23">
         <v>2</v>
       </c>
-      <c r="G140" s="127">
-        <v>2</v>
-      </c>
-      <c r="H140" s="105"/>
+      <c r="G140" s="110">
+        <v>2</v>
+      </c>
+      <c r="H140" s="92"/>
       <c r="I140" s="26"/>
     </row>
     <row r="141" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4239,7 +4222,7 @@
       <c r="C141" s="89">
         <v>4</v>
       </c>
-      <c r="D141" s="116">
+      <c r="D141" s="99">
         <v>0</v>
       </c>
       <c r="E141" s="39">
@@ -4248,10 +4231,10 @@
       <c r="F141" s="41">
         <v>4</v>
       </c>
-      <c r="G141" s="128">
-        <v>4</v>
-      </c>
-      <c r="H141" s="110"/>
+      <c r="G141" s="111">
+        <v>4</v>
+      </c>
+      <c r="H141" s="94"/>
       <c r="I141" s="26"/>
     </row>
     <row r="142" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4282,7 +4265,7 @@
         <f t="shared" si="15"/>
         <v>20</v>
       </c>
-      <c r="H142" s="118"/>
+      <c r="H142" s="101"/>
       <c r="I142" s="26"/>
     </row>
     <row r="143" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4292,7 +4275,7 @@
       <c r="E143" s="45"/>
       <c r="F143" s="45"/>
       <c r="G143" s="45"/>
-      <c r="H143" s="119"/>
+      <c r="H143" s="102"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
@@ -4306,72 +4289,132 @@
       <c r="E144" s="52"/>
       <c r="F144" s="52"/>
       <c r="G144" s="66"/>
-      <c r="H144" s="100"/>
+      <c r="H144" s="90"/>
       <c r="I144" s="26"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B145" s="102"/>
-      <c r="C145" s="102"/>
-      <c r="D145" s="103"/>
-      <c r="E145" s="103"/>
-      <c r="F145" s="103"/>
-      <c r="G145" s="104"/>
-      <c r="H145" s="105"/>
+      <c r="B145" s="26">
+        <v>4</v>
+      </c>
+      <c r="C145" s="54">
+        <v>4</v>
+      </c>
+      <c r="D145" s="79">
+        <v>0</v>
+      </c>
+      <c r="E145" s="23">
+        <v>4</v>
+      </c>
+      <c r="F145" s="23">
+        <v>4</v>
+      </c>
+      <c r="G145" s="24">
+        <v>4</v>
+      </c>
+      <c r="H145" s="92"/>
       <c r="I145" s="26"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B146" s="102"/>
-      <c r="C146" s="102"/>
-      <c r="D146" s="103"/>
-      <c r="E146" s="103"/>
-      <c r="F146" s="103"/>
-      <c r="G146" s="104"/>
-      <c r="H146" s="105"/>
+      <c r="B146" s="26">
+        <v>4</v>
+      </c>
+      <c r="C146" s="54">
+        <v>4</v>
+      </c>
+      <c r="D146" s="79">
+        <v>0</v>
+      </c>
+      <c r="E146" s="23">
+        <v>4</v>
+      </c>
+      <c r="F146" s="60">
+        <v>4</v>
+      </c>
+      <c r="G146" s="24">
+        <v>4</v>
+      </c>
+      <c r="H146" s="92"/>
       <c r="I146" s="26"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B147" s="102"/>
-      <c r="C147" s="102"/>
-      <c r="D147" s="103"/>
-      <c r="E147" s="103"/>
-      <c r="F147" s="103"/>
-      <c r="G147" s="104"/>
-      <c r="H147" s="105"/>
+      <c r="B147" s="26">
+        <v>6</v>
+      </c>
+      <c r="C147" s="54">
+        <v>6</v>
+      </c>
+      <c r="D147" s="79">
+        <v>0</v>
+      </c>
+      <c r="E147" s="23">
+        <v>6</v>
+      </c>
+      <c r="F147" s="23">
+        <v>6</v>
+      </c>
+      <c r="G147" s="24">
+        <v>6</v>
+      </c>
+      <c r="H147" s="92"/>
       <c r="I147" s="26"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B148" s="102"/>
-      <c r="C148" s="102"/>
-      <c r="D148" s="103"/>
-      <c r="E148" s="103"/>
-      <c r="F148" s="103"/>
-      <c r="G148" s="104"/>
-      <c r="H148" s="105"/>
+      <c r="B148" s="26">
+        <v>2</v>
+      </c>
+      <c r="C148" s="54">
+        <v>2</v>
+      </c>
+      <c r="D148" s="55">
+        <v>0</v>
+      </c>
+      <c r="E148" s="23">
+        <v>2</v>
+      </c>
+      <c r="F148" s="23">
+        <v>2</v>
+      </c>
+      <c r="G148" s="110">
+        <v>2</v>
+      </c>
+      <c r="H148" s="92"/>
       <c r="I148" s="26"/>
     </row>
     <row r="149" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B149" s="107"/>
-      <c r="C149" s="107"/>
-      <c r="D149" s="108"/>
-      <c r="E149" s="108"/>
-      <c r="F149" s="108"/>
-      <c r="G149" s="109"/>
-      <c r="H149" s="110"/>
+      <c r="B149" s="63">
+        <v>4</v>
+      </c>
+      <c r="C149" s="89">
+        <v>4</v>
+      </c>
+      <c r="D149" s="99">
+        <v>0</v>
+      </c>
+      <c r="E149" s="39">
+        <v>4</v>
+      </c>
+      <c r="F149" s="41">
+        <v>4</v>
+      </c>
+      <c r="G149" s="111">
+        <v>4</v>
+      </c>
+      <c r="H149" s="94"/>
       <c r="I149" s="26"/>
     </row>
     <row r="150" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4379,11 +4422,12 @@
         <v>6</v>
       </c>
       <c r="B150" s="17">
-        <v>0</v>
+        <f>B145+B146+B147+B148+B149</f>
+        <v>20</v>
       </c>
       <c r="C150" s="46">
         <f t="shared" ref="C150:G150" si="16">SUM(C145:C149)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D150" s="47">
         <f t="shared" si="16"/>
@@ -4391,15 +4435,15 @@
       </c>
       <c r="E150" s="47">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F150" s="47">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G150" s="48">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H150" s="49"/>
       <c r="I150" s="26"/>
@@ -4430,12 +4474,24 @@
       <c r="A153" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B153" s="26"/>
-      <c r="C153" s="93"/>
-      <c r="D153" s="90"/>
-      <c r="E153" s="94"/>
-      <c r="F153" s="94"/>
-      <c r="G153" s="92"/>
+      <c r="B153" s="26">
+        <v>4</v>
+      </c>
+      <c r="C153" s="54">
+        <v>4</v>
+      </c>
+      <c r="D153" s="79">
+        <v>0</v>
+      </c>
+      <c r="E153" s="23">
+        <v>4</v>
+      </c>
+      <c r="F153" s="23">
+        <v>4</v>
+      </c>
+      <c r="G153" s="24">
+        <v>4</v>
+      </c>
       <c r="H153" s="25"/>
       <c r="I153" s="26"/>
     </row>
@@ -4443,12 +4499,24 @@
       <c r="A154" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B154" s="26"/>
-      <c r="C154" s="95"/>
-      <c r="D154" s="90"/>
-      <c r="E154" s="94"/>
-      <c r="F154" s="90"/>
-      <c r="G154" s="92"/>
+      <c r="B154" s="26">
+        <v>4</v>
+      </c>
+      <c r="C154" s="54">
+        <v>4</v>
+      </c>
+      <c r="D154" s="79">
+        <v>0</v>
+      </c>
+      <c r="E154" s="23">
+        <v>4</v>
+      </c>
+      <c r="F154" s="60">
+        <v>4</v>
+      </c>
+      <c r="G154" s="24">
+        <v>4</v>
+      </c>
       <c r="H154" s="25"/>
       <c r="I154" s="26"/>
     </row>
@@ -4456,12 +4524,24 @@
       <c r="A155" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B155" s="26"/>
-      <c r="C155" s="95"/>
-      <c r="D155" s="91"/>
-      <c r="E155" s="94"/>
-      <c r="F155" s="94"/>
-      <c r="G155" s="92"/>
+      <c r="B155" s="26">
+        <v>6</v>
+      </c>
+      <c r="C155" s="54">
+        <v>6</v>
+      </c>
+      <c r="D155" s="79">
+        <v>0</v>
+      </c>
+      <c r="E155" s="23">
+        <v>6</v>
+      </c>
+      <c r="F155" s="23">
+        <v>6</v>
+      </c>
+      <c r="G155" s="24">
+        <v>6</v>
+      </c>
       <c r="H155" s="25"/>
       <c r="I155" s="26"/>
     </row>
@@ -4469,12 +4549,24 @@
       <c r="A156" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B156" s="26"/>
-      <c r="C156" s="95"/>
-      <c r="D156" s="90"/>
-      <c r="E156" s="94"/>
-      <c r="F156" s="94"/>
-      <c r="G156" s="92"/>
+      <c r="B156" s="26">
+        <v>2</v>
+      </c>
+      <c r="C156" s="54">
+        <v>2</v>
+      </c>
+      <c r="D156" s="55">
+        <v>0</v>
+      </c>
+      <c r="E156" s="23">
+        <v>2</v>
+      </c>
+      <c r="F156" s="23">
+        <v>2</v>
+      </c>
+      <c r="G156" s="110">
+        <v>2</v>
+      </c>
       <c r="H156" s="25"/>
       <c r="I156" s="26"/>
     </row>
@@ -4482,12 +4574,24 @@
       <c r="A157" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B157" s="63"/>
-      <c r="C157" s="96"/>
-      <c r="D157" s="98"/>
-      <c r="E157" s="97"/>
-      <c r="F157" s="97"/>
-      <c r="G157" s="99"/>
+      <c r="B157" s="63">
+        <v>4</v>
+      </c>
+      <c r="C157" s="89">
+        <v>4</v>
+      </c>
+      <c r="D157" s="99">
+        <v>0</v>
+      </c>
+      <c r="E157" s="39">
+        <v>4</v>
+      </c>
+      <c r="F157" s="41">
+        <v>4</v>
+      </c>
+      <c r="G157" s="111">
+        <v>4</v>
+      </c>
       <c r="H157" s="43"/>
       <c r="I157" s="26"/>
     </row>
@@ -4496,11 +4600,12 @@
         <v>6</v>
       </c>
       <c r="B158" s="17">
-        <v>0</v>
+        <f>B153+B154+B155+B156+B157</f>
+        <v>20</v>
       </c>
       <c r="C158" s="46">
         <f t="shared" ref="C158:G158" si="17">SUM(C153:C157)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D158" s="47">
         <f t="shared" si="17"/>
@@ -4508,15 +4613,15 @@
       </c>
       <c r="E158" s="47">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F158" s="47">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G158" s="48">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H158" s="49"/>
       <c r="I158" s="26"/>
@@ -4547,12 +4652,24 @@
       <c r="A161" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B161" s="26"/>
-      <c r="C161" s="95"/>
-      <c r="D161" s="90"/>
-      <c r="E161" s="91"/>
-      <c r="F161" s="90"/>
-      <c r="G161" s="92"/>
+      <c r="B161" s="26">
+        <v>4</v>
+      </c>
+      <c r="C161" s="54">
+        <v>4</v>
+      </c>
+      <c r="D161" s="79">
+        <v>0</v>
+      </c>
+      <c r="E161" s="23">
+        <v>4</v>
+      </c>
+      <c r="F161" s="23">
+        <v>4</v>
+      </c>
+      <c r="G161" s="24">
+        <v>4</v>
+      </c>
       <c r="H161" s="25"/>
       <c r="I161" s="26"/>
     </row>
@@ -4560,12 +4677,24 @@
       <c r="A162" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B162" s="26"/>
-      <c r="C162" s="95"/>
-      <c r="D162" s="91"/>
-      <c r="E162" s="94"/>
-      <c r="F162" s="90"/>
-      <c r="G162" s="92"/>
+      <c r="B162" s="26">
+        <v>4</v>
+      </c>
+      <c r="C162" s="54">
+        <v>4</v>
+      </c>
+      <c r="D162" s="79">
+        <v>0</v>
+      </c>
+      <c r="E162" s="23">
+        <v>4</v>
+      </c>
+      <c r="F162" s="60">
+        <v>4</v>
+      </c>
+      <c r="G162" s="24">
+        <v>4</v>
+      </c>
       <c r="H162" s="25"/>
       <c r="I162" s="26"/>
     </row>
@@ -4573,12 +4702,24 @@
       <c r="A163" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B163" s="26"/>
-      <c r="C163" s="95"/>
-      <c r="D163" s="91"/>
-      <c r="E163" s="91"/>
-      <c r="F163" s="94"/>
-      <c r="G163" s="92"/>
+      <c r="B163" s="26">
+        <v>6</v>
+      </c>
+      <c r="C163" s="54">
+        <v>6</v>
+      </c>
+      <c r="D163" s="79">
+        <v>0</v>
+      </c>
+      <c r="E163" s="23">
+        <v>6</v>
+      </c>
+      <c r="F163" s="23">
+        <v>6</v>
+      </c>
+      <c r="G163" s="24">
+        <v>6</v>
+      </c>
       <c r="H163" s="25"/>
       <c r="I163" s="26"/>
     </row>
@@ -4586,12 +4727,24 @@
       <c r="A164" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B164" s="26"/>
-      <c r="C164" s="95"/>
-      <c r="D164" s="91"/>
-      <c r="E164" s="94"/>
-      <c r="F164" s="94"/>
-      <c r="G164" s="92"/>
+      <c r="B164" s="26">
+        <v>2</v>
+      </c>
+      <c r="C164" s="54">
+        <v>2</v>
+      </c>
+      <c r="D164" s="55">
+        <v>0</v>
+      </c>
+      <c r="E164" s="23">
+        <v>2</v>
+      </c>
+      <c r="F164" s="23">
+        <v>2</v>
+      </c>
+      <c r="G164" s="110">
+        <v>2</v>
+      </c>
       <c r="H164" s="25"/>
       <c r="I164" s="26"/>
     </row>
@@ -4599,12 +4752,24 @@
       <c r="A165" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B165" s="63"/>
-      <c r="C165" s="96"/>
-      <c r="D165" s="97"/>
-      <c r="E165" s="97"/>
-      <c r="F165" s="97"/>
-      <c r="G165" s="99"/>
+      <c r="B165" s="63">
+        <v>4</v>
+      </c>
+      <c r="C165" s="89">
+        <v>4</v>
+      </c>
+      <c r="D165" s="99">
+        <v>0</v>
+      </c>
+      <c r="E165" s="39">
+        <v>4</v>
+      </c>
+      <c r="F165" s="41">
+        <v>4</v>
+      </c>
+      <c r="G165" s="111">
+        <v>4</v>
+      </c>
       <c r="H165" s="43"/>
       <c r="I165" s="26"/>
     </row>
@@ -4613,11 +4778,12 @@
         <v>6</v>
       </c>
       <c r="B166" s="17">
-        <v>0</v>
+        <f>B161+B162+B163+B164+B165</f>
+        <v>20</v>
       </c>
       <c r="C166" s="46">
         <f t="shared" ref="C166:G166" si="18">SUM(C161:C165)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D166" s="47">
         <f t="shared" si="18"/>
@@ -4625,15 +4791,15 @@
       </c>
       <c r="E166" s="47">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F166" s="47">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G166" s="48">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H166" s="49"/>
       <c r="I166" s="26"/>
@@ -4664,12 +4830,24 @@
       <c r="A169" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B169" s="26"/>
-      <c r="C169" s="95"/>
-      <c r="D169" s="90"/>
-      <c r="E169" s="91"/>
-      <c r="F169" s="94"/>
-      <c r="G169" s="92"/>
+      <c r="B169" s="26">
+        <v>4</v>
+      </c>
+      <c r="C169" s="54">
+        <v>4</v>
+      </c>
+      <c r="D169" s="79">
+        <v>0</v>
+      </c>
+      <c r="E169" s="23">
+        <v>4</v>
+      </c>
+      <c r="F169" s="23">
+        <v>4</v>
+      </c>
+      <c r="G169" s="24">
+        <v>4</v>
+      </c>
       <c r="H169" s="25"/>
       <c r="I169" s="26"/>
     </row>
@@ -4677,12 +4855,24 @@
       <c r="A170" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B170" s="26"/>
-      <c r="C170" s="95"/>
-      <c r="D170" s="91"/>
-      <c r="E170" s="94"/>
-      <c r="F170" s="90"/>
-      <c r="G170" s="92"/>
+      <c r="B170" s="26">
+        <v>4</v>
+      </c>
+      <c r="C170" s="54">
+        <v>4</v>
+      </c>
+      <c r="D170" s="57">
+        <v>4</v>
+      </c>
+      <c r="E170" s="23">
+        <v>4</v>
+      </c>
+      <c r="F170" s="60">
+        <v>4</v>
+      </c>
+      <c r="G170" s="24">
+        <v>4</v>
+      </c>
       <c r="H170" s="25"/>
       <c r="I170" s="26"/>
     </row>
@@ -4690,12 +4880,24 @@
       <c r="A171" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B171" s="26"/>
-      <c r="C171" s="95"/>
-      <c r="D171" s="90"/>
-      <c r="E171" s="94"/>
-      <c r="F171" s="94"/>
-      <c r="G171" s="92"/>
+      <c r="B171" s="26">
+        <v>6</v>
+      </c>
+      <c r="C171" s="54">
+        <v>6</v>
+      </c>
+      <c r="D171" s="79">
+        <v>0</v>
+      </c>
+      <c r="E171" s="23">
+        <v>6</v>
+      </c>
+      <c r="F171" s="23">
+        <v>6</v>
+      </c>
+      <c r="G171" s="24">
+        <v>6</v>
+      </c>
       <c r="H171" s="25"/>
       <c r="I171" s="26"/>
     </row>
@@ -4703,12 +4905,24 @@
       <c r="A172" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B172" s="26"/>
-      <c r="C172" s="95"/>
-      <c r="D172" s="94"/>
-      <c r="E172" s="94"/>
-      <c r="F172" s="94"/>
-      <c r="G172" s="92"/>
+      <c r="B172" s="26">
+        <v>2</v>
+      </c>
+      <c r="C172" s="54">
+        <v>2</v>
+      </c>
+      <c r="D172" s="55">
+        <v>0</v>
+      </c>
+      <c r="E172" s="23">
+        <v>2</v>
+      </c>
+      <c r="F172" s="23">
+        <v>2</v>
+      </c>
+      <c r="G172" s="110">
+        <v>2</v>
+      </c>
       <c r="H172" s="25"/>
       <c r="I172" s="26"/>
     </row>
@@ -4716,12 +4930,24 @@
       <c r="A173" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B173" s="63"/>
-      <c r="C173" s="96"/>
-      <c r="D173" s="98"/>
-      <c r="E173" s="97"/>
-      <c r="F173" s="98"/>
-      <c r="G173" s="112"/>
+      <c r="B173" s="63">
+        <v>4</v>
+      </c>
+      <c r="C173" s="89">
+        <v>4</v>
+      </c>
+      <c r="D173" s="41">
+        <v>4</v>
+      </c>
+      <c r="E173" s="39">
+        <v>4</v>
+      </c>
+      <c r="F173" s="41">
+        <v>4</v>
+      </c>
+      <c r="G173" s="111">
+        <v>4</v>
+      </c>
       <c r="H173" s="43"/>
       <c r="I173" s="26"/>
     </row>
@@ -4730,27 +4956,28 @@
         <v>6</v>
       </c>
       <c r="B174" s="17">
-        <v>0</v>
+        <f>B169+B170+B171+B172+B173</f>
+        <v>20</v>
       </c>
       <c r="C174" s="46">
         <f t="shared" ref="C174:G174" si="19">SUM(C169:C173)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D174" s="47">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E174" s="47">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F174" s="47">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G174" s="48">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H174" s="49"/>
       <c r="I174" s="26"/>

</xml_diff>